<commit_message>
Issue #4: Change the Upper limits of the non-detects (#8)
* Change the Upper limits of the non-detects

* Update the processed data

* Update figures

* Update the results

* Add an explaining comment
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-12.9327702514742</v>
+        <v>-2.39909375345095</v>
       </c>
       <c r="C2" t="n">
-        <v>1.01693037356109</v>
+        <v>62420.4525398934</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000000000000000000000000000000472992995655613</v>
+        <v>0.999969333771425</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.266518690518715</v>
+        <v>-0.621726438125615</v>
       </c>
       <c r="C3" t="n">
-        <v>0.264647878857453</v>
+        <v>0.446563396294826</v>
       </c>
       <c r="D3" t="n">
-        <v>0.313901588422124</v>
+        <v>0.163847689793895</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0957802438048524</v>
+        <v>-0.346837641952026</v>
       </c>
       <c r="C4" t="n">
-        <v>0.249579255983658</v>
+        <v>0.358494562257901</v>
       </c>
       <c r="D4" t="n">
-        <v>0.701151263274278</v>
+        <v>0.333302290818082</v>
       </c>
     </row>
     <row r="5">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.834873267937437</v>
+        <v>3.83220696378058</v>
       </c>
       <c r="C5" t="n">
-        <v>0.479735822939903</v>
+        <v>62420.4525255146</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0818103726556742</v>
+        <v>0.999951015113724</v>
       </c>
     </row>
     <row r="6">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0282811131126521</v>
+        <v>-0.415959452875481</v>
       </c>
       <c r="C6" t="n">
-        <v>0.498435787468425</v>
+        <v>83119.3212186157</v>
       </c>
       <c r="D6" t="n">
-        <v>0.954752523241398</v>
+        <v>0.999996007094133</v>
       </c>
     </row>
     <row r="7">
@@ -520,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0432002480523183</v>
+        <v>-0.0571973230482257</v>
       </c>
       <c r="C7" t="n">
-        <v>0.447160082190111</v>
+        <v>80488.0075943448</v>
       </c>
       <c r="D7" t="n">
-        <v>0.923035914970508</v>
+        <v>0.999999432998004</v>
       </c>
     </row>
     <row r="8">
@@ -534,13 +534,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.134241204130493</v>
+        <v>0.775637968087059</v>
       </c>
       <c r="C8" t="n">
-        <v>0.483370414929918</v>
+        <v>92489.6876247333</v>
       </c>
       <c r="D8" t="n">
-        <v>0.781227985514082</v>
+        <v>0.999993308772303</v>
       </c>
     </row>
     <row r="9">
@@ -548,13 +548,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.422256623442575</v>
+        <v>3.81123870903567</v>
       </c>
       <c r="C9" t="n">
-        <v>0.589424329577645</v>
+        <v>62420.4525255564</v>
       </c>
       <c r="D9" t="n">
-        <v>0.473751690654345</v>
+        <v>0.999951283138802</v>
       </c>
     </row>
     <row r="10">
@@ -562,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>1.00568388655994</v>
+        <v>3.74202116607166</v>
       </c>
       <c r="C10" t="n">
-        <v>0.467214515493615</v>
+        <v>62420.4525252916</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0313572136153694</v>
+        <v>0.999952167906639</v>
       </c>
     </row>
     <row r="11">
@@ -576,13 +576,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0193647411776502</v>
+        <v>-0.317939108720248</v>
       </c>
       <c r="C11" t="n">
-        <v>0.492530433383032</v>
+        <v>83906.3177659629</v>
       </c>
       <c r="D11" t="n">
-        <v>0.968637779107759</v>
+        <v>0.999996976643561</v>
       </c>
     </row>
     <row r="12">
@@ -590,13 +590,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.506462859924022</v>
+        <v>-0.973735851366318</v>
       </c>
       <c r="C12" t="n">
-        <v>0.693737567675257</v>
+        <v>1.14334031208868</v>
       </c>
       <c r="D12" t="n">
-        <v>0.46535984388239</v>
+        <v>0.394403487475458</v>
       </c>
     </row>
     <row r="13">
@@ -604,13 +604,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.948142270367192</v>
+        <v>-1.69128793957788</v>
       </c>
       <c r="C13" t="n">
-        <v>0.99421272005645</v>
+        <v>1.56989329119463</v>
       </c>
       <c r="D13" t="n">
-        <v>0.340255077233942</v>
+        <v>0.281334343559962</v>
       </c>
     </row>
     <row r="14">
@@ -618,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.04412527568886</v>
+        <v>-1.58435939633627</v>
       </c>
       <c r="C14" t="n">
-        <v>1.05573781121467</v>
+        <v>1.55224082586339</v>
       </c>
       <c r="D14" t="n">
-        <v>0.322662872692488</v>
+        <v>0.307400507066783</v>
       </c>
     </row>
     <row r="15">
@@ -632,13 +632,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.871217680413162</v>
+        <v>-1.03566860498879</v>
       </c>
       <c r="C15" t="n">
-        <v>1.04244347790254</v>
+        <v>1.38946683614383</v>
       </c>
       <c r="D15" t="n">
-        <v>0.403297965688405</v>
+        <v>0.456047331093435</v>
       </c>
     </row>
     <row r="16">
@@ -646,13 +646,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.811001991690047</v>
+        <v>-0.552095268289528</v>
       </c>
       <c r="C16" t="n">
-        <v>1.00224158740966</v>
+        <v>1.32275580150065</v>
       </c>
       <c r="D16" t="n">
-        <v>0.41840694395365</v>
+        <v>0.676398572897828</v>
       </c>
     </row>
     <row r="17">
@@ -660,13 +660,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.785521105580506</v>
+        <v>-0.178518779772545</v>
       </c>
       <c r="C17" t="n">
-        <v>0.970870280782964</v>
+        <v>1.26830203636834</v>
       </c>
       <c r="D17" t="n">
-        <v>0.418463575304483</v>
+        <v>0.888064162430655</v>
       </c>
     </row>
     <row r="18">
@@ -674,13 +674,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.741301286323711</v>
+        <v>-0.108125524782969</v>
       </c>
       <c r="C18" t="n">
-        <v>0.953942469415266</v>
+        <v>1.23430033652575</v>
       </c>
       <c r="D18" t="n">
-        <v>0.437104354452557</v>
+        <v>0.930194077165221</v>
       </c>
     </row>
     <row r="19">
@@ -688,13 +688,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.854659383233111</v>
+        <v>-0.478542851681695</v>
       </c>
       <c r="C19" t="n">
-        <v>0.953596724124445</v>
+        <v>1.23744721552008</v>
       </c>
       <c r="D19" t="n">
-        <v>0.370120197954985</v>
+        <v>0.698965144865284</v>
       </c>
     </row>
     <row r="20">
@@ -702,13 +702,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.80123458591608</v>
+        <v>-0.707018679798631</v>
       </c>
       <c r="C20" t="n">
-        <v>0.981728812636145</v>
+        <v>1.33615055931206</v>
       </c>
       <c r="D20" t="n">
-        <v>0.414416321338111</v>
+        <v>0.596704196078925</v>
       </c>
     </row>
     <row r="21">
@@ -716,13 +716,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.624531295523265</v>
+        <v>-0.787972102479502</v>
       </c>
       <c r="C21" t="n">
-        <v>0.995852589838104</v>
+        <v>1.39564683618295</v>
       </c>
       <c r="D21" t="n">
-        <v>0.530572535491734</v>
+        <v>0.572350789285024</v>
       </c>
     </row>
     <row r="22">
@@ -730,13 +730,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.571643467733107</v>
+        <v>-0.837547376183614</v>
       </c>
       <c r="C22" t="n">
-        <v>1.01546057730031</v>
+        <v>1.76436770351332</v>
       </c>
       <c r="D22" t="n">
-        <v>0.573475680657119</v>
+        <v>0.634999998830929</v>
       </c>
     </row>
     <row r="23">
@@ -744,13 +744,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.556170290608392</v>
+        <v>-0.887078765314423</v>
       </c>
       <c r="C23" t="n">
-        <v>1.27430581328131</v>
+        <v>2.72866102915728</v>
       </c>
       <c r="D23" t="n">
-        <v>0.662510542848946</v>
+        <v>0.745107867222508</v>
       </c>
     </row>
     <row r="24">
@@ -758,13 +758,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.744427144499975</v>
+        <v>-0.644780512481345</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0345116311592407</v>
+        <v>0.208200131659363</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000341278591947983</v>
+        <v>0.00195538326513929</v>
       </c>
     </row>
   </sheetData>
@@ -800,13 +800,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.4263709804496</v>
+        <v>1.87344337189236</v>
       </c>
       <c r="C2" t="n">
-        <v>1.61430468730633</v>
+        <v>0.700792680433909</v>
       </c>
       <c r="D2" t="n">
-        <v>0.376921760085615</v>
+        <v>0.00751044791351729</v>
       </c>
     </row>
     <row r="3">
@@ -814,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.284967157280777</v>
+        <v>0.183062160944288</v>
       </c>
       <c r="C3" t="n">
-        <v>0.433278476014575</v>
+        <v>0.183410500628311</v>
       </c>
       <c r="D3" t="n">
-        <v>0.510731065353607</v>
+        <v>0.31823049932207</v>
       </c>
     </row>
     <row r="4">
@@ -828,13 +828,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.140726130798729</v>
+        <v>0.0930228721293085</v>
       </c>
       <c r="C4" t="n">
-        <v>0.401042238378188</v>
+        <v>0.170832307431283</v>
       </c>
       <c r="D4" t="n">
-        <v>0.725662605696018</v>
+        <v>0.586078598863253</v>
       </c>
     </row>
     <row r="5">
@@ -842,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>2.62122006411562</v>
+        <v>-0.1321907583995</v>
       </c>
       <c r="C5" t="n">
-        <v>0.76068445637432</v>
+        <v>0.323816503312254</v>
       </c>
       <c r="D5" t="n">
-        <v>0.000569223246541038</v>
+        <v>0.683106758379441</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.24156697093558</v>
+        <v>-1.12105693994151</v>
       </c>
       <c r="C6" t="n">
-        <v>0.827082239224352</v>
+        <v>0.356033394513466</v>
       </c>
       <c r="D6" t="n">
-        <v>0.133319123972765</v>
+        <v>0.00163975464278277</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +870,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>4.30885899459859</v>
+        <v>0.377639777202835</v>
       </c>
       <c r="C7" t="n">
-        <v>0.689221349866713</v>
+        <v>0.304016139312999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000000000405805501753515</v>
+        <v>0.214173785886877</v>
       </c>
     </row>
     <row r="8">
@@ -884,13 +884,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>4.3587006847049</v>
+        <v>0.821756402549003</v>
       </c>
       <c r="C8" t="n">
-        <v>0.737393372372035</v>
+        <v>0.319701329503895</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00000000340125349688817</v>
+        <v>0.010158472210531</v>
       </c>
     </row>
     <row r="9">
@@ -898,13 +898,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.705678851778342</v>
+        <v>-1.35849522573185</v>
       </c>
       <c r="C9" t="n">
-        <v>0.987862427825322</v>
+        <v>0.420233788296791</v>
       </c>
       <c r="D9" t="n">
-        <v>0.475011203055809</v>
+        <v>0.00122620690118946</v>
       </c>
     </row>
     <row r="10">
@@ -912,13 +912,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>1.23769466115759</v>
+        <v>-0.861099148009334</v>
       </c>
       <c r="C10" t="n">
-        <v>0.761429663117052</v>
+        <v>0.324529533720654</v>
       </c>
       <c r="D10" t="n">
-        <v>0.104058652000108</v>
+        <v>0.00796908469785711</v>
       </c>
     </row>
     <row r="11">
@@ -926,13 +926,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>3.24292779797949</v>
+        <v>-0.0387198775245461</v>
       </c>
       <c r="C11" t="n">
-        <v>0.757789028452108</v>
+        <v>0.325526911155548</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0000187347344738273</v>
+        <v>0.905318737498331</v>
       </c>
     </row>
     <row r="12">
@@ -940,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.829245461415649</v>
+        <v>-0.564998778904266</v>
       </c>
       <c r="C12" t="n">
-        <v>1.10913259690617</v>
+        <v>0.485716135157964</v>
       </c>
       <c r="D12" t="n">
-        <v>0.454669950876483</v>
+        <v>0.244736866701062</v>
       </c>
     </row>
     <row r="13">
@@ -954,13 +954,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.55695206839847</v>
+        <v>-1.05729719321019</v>
       </c>
       <c r="C13" t="n">
-        <v>1.60442090569531</v>
+        <v>0.697494778217006</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3318403098272</v>
+        <v>0.129557382297949</v>
       </c>
     </row>
     <row r="14">
@@ -968,13 +968,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.82360427772803</v>
+        <v>-1.28542080199948</v>
       </c>
       <c r="C14" t="n">
-        <v>1.71197944424297</v>
+        <v>0.740278039169894</v>
       </c>
       <c r="D14" t="n">
-        <v>0.286784436333874</v>
+        <v>0.0824926513703027</v>
       </c>
     </row>
     <row r="15">
@@ -982,13 +982,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.81907837469931</v>
+        <v>-1.41578815361765</v>
       </c>
       <c r="C15" t="n">
-        <v>1.68677310255858</v>
+        <v>0.728684508681899</v>
       </c>
       <c r="D15" t="n">
-        <v>0.280838822100672</v>
+        <v>0.0520237607165542</v>
       </c>
     </row>
     <row r="16">
@@ -996,13 +996,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.46927855996044</v>
+        <v>-1.30314677801982</v>
       </c>
       <c r="C16" t="n">
-        <v>1.61506139108791</v>
+        <v>0.698657237185131</v>
       </c>
       <c r="D16" t="n">
-        <v>0.362962057454579</v>
+        <v>0.0621511095168702</v>
       </c>
     </row>
     <row r="17">
@@ -1010,13 +1010,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.17579606535521</v>
+        <v>-1.09277975165252</v>
       </c>
       <c r="C17" t="n">
-        <v>1.55148260614557</v>
+        <v>0.672031993071463</v>
       </c>
       <c r="D17" t="n">
-        <v>0.44853886695377</v>
+        <v>0.103932015032744</v>
       </c>
     </row>
     <row r="18">
@@ -1024,13 +1024,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.26527714456529</v>
+        <v>-1.03818696892916</v>
       </c>
       <c r="C18" t="n">
-        <v>1.51771583238927</v>
+        <v>0.657653502071145</v>
       </c>
       <c r="D18" t="n">
-        <v>0.404465858707069</v>
+        <v>0.114422547327424</v>
       </c>
     </row>
     <row r="19">
@@ -1038,13 +1038,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.54203069029381</v>
+        <v>-1.13035524651131</v>
       </c>
       <c r="C19" t="n">
-        <v>1.51747153254613</v>
+        <v>0.657506776848006</v>
       </c>
       <c r="D19" t="n">
-        <v>0.309541649096078</v>
+        <v>0.0855863782746068</v>
       </c>
     </row>
     <row r="20">
@@ -1052,13 +1052,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.56774602433861</v>
+        <v>-1.05174806831519</v>
       </c>
       <c r="C20" t="n">
-        <v>1.55964932764874</v>
+        <v>0.675630795008506</v>
       </c>
       <c r="D20" t="n">
-        <v>0.314804716088383</v>
+        <v>0.119543975327657</v>
       </c>
     </row>
     <row r="21">
@@ -1066,13 +1066,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-2.02263367336433</v>
+        <v>-0.93456171186514</v>
       </c>
       <c r="C21" t="n">
-        <v>1.5773323771143</v>
+        <v>0.683281959505787</v>
       </c>
       <c r="D21" t="n">
-        <v>0.199732900358586</v>
+        <v>0.171389054787642</v>
       </c>
     </row>
     <row r="22">
@@ -1080,13 +1080,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-3.58565924103971</v>
+        <v>-1.13360040303422</v>
       </c>
       <c r="C22" t="n">
-        <v>1.60267000194338</v>
+        <v>0.695163678473655</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0252665091460345</v>
+        <v>0.102954549911525</v>
       </c>
     </row>
     <row r="23">
@@ -1094,13 +1094,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-5.3449817529099</v>
+        <v>-1.4025892235245</v>
       </c>
       <c r="C23" t="n">
-        <v>2.00341041608238</v>
+        <v>0.87400605496044</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00763175493740844</v>
+        <v>0.108541778870265</v>
       </c>
     </row>
     <row r="24">
@@ -1108,13 +1108,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>1.07208353602469</v>
+        <v>0.232917522181786</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0502468667359195</v>
+        <v>0.0549784234871216</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000522419514479313</v>
+        <v>0.000022700461552089</v>
       </c>
     </row>
   </sheetData>
@@ -1150,13 +1150,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.88943024620484</v>
+        <v>-1.63985760396549</v>
       </c>
       <c r="C2" t="n">
-        <v>2.95601489647507</v>
+        <v>1.7119847068233</v>
       </c>
       <c r="D2" t="n">
-        <v>0.522704819297734</v>
+        <v>0.338128665494533</v>
       </c>
     </row>
     <row r="3">
@@ -1164,13 +1164,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.261458858653706</v>
+        <v>-0.119268163369971</v>
       </c>
       <c r="C3" t="n">
-        <v>0.728271673603757</v>
+        <v>0.336747928873695</v>
       </c>
       <c r="D3" t="n">
-        <v>0.719585507628283</v>
+        <v>0.723206701711976</v>
       </c>
     </row>
     <row r="4">
@@ -1178,13 +1178,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.03206796101374</v>
+        <v>-0.178101232029074</v>
       </c>
       <c r="C4" t="n">
-        <v>0.772451420388194</v>
+        <v>0.364103154406656</v>
       </c>
       <c r="D4" t="n">
-        <v>0.181518443869726</v>
+        <v>0.624735166663663</v>
       </c>
     </row>
     <row r="5">
@@ -1192,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.5181707099916</v>
+        <v>-1.22544325378988</v>
       </c>
       <c r="C5" t="n">
-        <v>2.07147011225296</v>
+        <v>0.69844192290108</v>
       </c>
       <c r="D5" t="n">
-        <v>0.029172906372962</v>
+        <v>0.0793382764903816</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1206,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.17289582146218</v>
+        <v>-0.102629469930867</v>
       </c>
       <c r="C6" t="n">
-        <v>1.53249701029379</v>
+        <v>1.10090224972129</v>
       </c>
       <c r="D6" t="n">
-        <v>0.444063455253783</v>
+        <v>0.925726359654848</v>
       </c>
     </row>
     <row r="7">
@@ -1220,55 +1220,47 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.781247588708464</v>
+        <v>0.42266763175141</v>
       </c>
       <c r="C7" t="n">
-        <v>1.07873044435819</v>
+        <v>0.713752428241443</v>
       </c>
       <c r="D7" t="n">
-        <v>0.468925318082714</v>
+        <v>0.553732200594692</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>-3.63394014115844</v>
-      </c>
+      <c r="B8"/>
       <c r="C8" t="n">
-        <v>2.58775042328804</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.160233879765827</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="n">
-        <v>-3.11737844645137</v>
-      </c>
+      <c r="B9"/>
       <c r="C9" t="n">
-        <v>3.69493301289952</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.398842594564099</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0154181303946</v>
+        <v>0.556340293043207</v>
       </c>
       <c r="C10" t="n">
-        <v>1.13235123188979</v>
+        <v>0.736415560952545</v>
       </c>
       <c r="D10" t="n">
-        <v>0.36986074103033</v>
+        <v>0.449966676533983</v>
       </c>
     </row>
     <row r="11">
@@ -1276,13 +1268,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.936778625864349</v>
+        <v>-0.247554106150954</v>
       </c>
       <c r="C11" t="n">
-        <v>1.56982205614473</v>
+        <v>1.04768200033696</v>
       </c>
       <c r="D11" t="n">
-        <v>0.55067970103085</v>
+        <v>0.813209626275475</v>
       </c>
     </row>
     <row r="12">
@@ -1290,13 +1282,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.238840783933809</v>
+        <v>0.0679442525922799</v>
       </c>
       <c r="C12" t="n">
-        <v>2.01987218402012</v>
+        <v>1.05191018149522</v>
       </c>
       <c r="D12" t="n">
-        <v>0.905873143892926</v>
+        <v>0.948499406930426</v>
       </c>
     </row>
     <row r="13">
@@ -1304,13 +1296,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.417792811946882</v>
+        <v>0.143798307076691</v>
       </c>
       <c r="C13" t="n">
-        <v>2.95353907672677</v>
+        <v>1.59378385483527</v>
       </c>
       <c r="D13" t="n">
-        <v>0.887510522859754</v>
+        <v>0.928108837643466</v>
       </c>
     </row>
     <row r="14">
@@ -1318,13 +1310,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.353961217075726</v>
+        <v>0.249830958106449</v>
       </c>
       <c r="C14" t="n">
-        <v>3.16087526455475</v>
+        <v>1.7451710978706</v>
       </c>
       <c r="D14" t="n">
-        <v>0.910837657841271</v>
+        <v>0.88616732066207</v>
       </c>
     </row>
     <row r="15">
@@ -1332,13 +1324,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0571808970014877</v>
+        <v>0.369631336503031</v>
       </c>
       <c r="C15" t="n">
-        <v>3.0942903984245</v>
+        <v>1.72149704582523</v>
       </c>
       <c r="D15" t="n">
-        <v>0.985256342339484</v>
+        <v>0.829989482493843</v>
       </c>
     </row>
     <row r="16">
@@ -1346,13 +1338,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.767396458378999</v>
+        <v>0.468118911313132</v>
       </c>
       <c r="C16" t="n">
-        <v>2.92079170597324</v>
+        <v>1.66711784833335</v>
       </c>
       <c r="D16" t="n">
-        <v>0.792754244457577</v>
+        <v>0.778867383431452</v>
       </c>
     </row>
     <row r="17">
@@ -1360,13 +1352,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>1.39625557337217</v>
+        <v>0.507487011531612</v>
       </c>
       <c r="C17" t="n">
-        <v>2.80149672133235</v>
+        <v>1.61437219466819</v>
       </c>
       <c r="D17" t="n">
-        <v>0.618204750940148</v>
+        <v>0.753250940428615</v>
       </c>
     </row>
     <row r="18">
@@ -1374,13 +1366,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>1.39468778492588</v>
+        <v>0.484083843909326</v>
       </c>
       <c r="C18" t="n">
-        <v>2.76835926830002</v>
+        <v>1.59680811921259</v>
       </c>
       <c r="D18" t="n">
-        <v>0.614404876203097</v>
+        <v>0.761770080970127</v>
       </c>
     </row>
     <row r="19">
@@ -1388,13 +1380,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.130008610327689</v>
+        <v>0.377353312920755</v>
       </c>
       <c r="C19" t="n">
-        <v>2.77673226061517</v>
+        <v>1.59908776690256</v>
       </c>
       <c r="D19" t="n">
-        <v>0.962656113064298</v>
+        <v>0.813447907373067</v>
       </c>
     </row>
     <row r="20">
@@ -1402,13 +1394,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.41366900109614</v>
+        <v>0.221082067033935</v>
       </c>
       <c r="C20" t="n">
-        <v>2.87529139232716</v>
+        <v>1.631638168552</v>
       </c>
       <c r="D20" t="n">
-        <v>0.622958924369526</v>
+        <v>0.892218940830233</v>
       </c>
     </row>
     <row r="21">
@@ -1416,13 +1408,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-2.15297350868795</v>
+        <v>0.0864441601164589</v>
       </c>
       <c r="C21" t="n">
-        <v>2.91459449190639</v>
+        <v>1.63848131917373</v>
       </c>
       <c r="D21" t="n">
-        <v>0.460096988329264</v>
+        <v>0.957924160613751</v>
       </c>
     </row>
     <row r="22">
@@ -1430,13 +1422,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.01450429681209</v>
+        <v>0.00510728173720448</v>
       </c>
       <c r="C22" t="n">
-        <v>2.86388033971916</v>
+        <v>1.64115674043549</v>
       </c>
       <c r="D22" t="n">
-        <v>0.723158158847498</v>
+        <v>0.997516986301226</v>
       </c>
     </row>
     <row r="23">
@@ -1444,13 +1436,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.601410382238928</v>
+        <v>-0.0627879417631931</v>
       </c>
       <c r="C23" t="n">
-        <v>3.4892827697095</v>
+        <v>1.94811596841063</v>
       </c>
       <c r="D23" t="n">
-        <v>0.863155056682611</v>
+        <v>0.974288564885443</v>
       </c>
     </row>
     <row r="24">
@@ -1458,13 +1450,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.883246561420671</v>
+        <v>0.54117999425717</v>
       </c>
       <c r="C24" t="n">
-        <v>0.107805268244883</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00000000000000025483349211657</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2550,13 +2542,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-6.31804266577476</v>
+        <v>3.25402503775698</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7473537424344</v>
+        <v>2.13881401084254</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000299447288703455</v>
+        <v>0.128155572292059</v>
       </c>
     </row>
     <row r="3">
@@ -2564,13 +2556,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.58747966977656</v>
+        <v>1.53907634076338</v>
       </c>
       <c r="C3" t="n">
-        <v>0.447208854284711</v>
+        <v>0.574731256408406</v>
       </c>
       <c r="D3" t="n">
-        <v>0.000385597017243224</v>
+        <v>0.00740839828488199</v>
       </c>
     </row>
     <row r="4">
@@ -2578,13 +2570,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.717547679854374</v>
+        <v>0.710125630822808</v>
       </c>
       <c r="C4" t="n">
-        <v>0.42771926504593</v>
+        <v>0.547540426182637</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0934225452037561</v>
+        <v>0.194652743043003</v>
       </c>
     </row>
     <row r="5">
@@ -2592,13 +2584,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.28145631062883</v>
+        <v>0.923979976331419</v>
       </c>
       <c r="C5" t="n">
-        <v>0.868794026797192</v>
+        <v>0.703277924798839</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00863938836123437</v>
+        <v>0.188907085510505</v>
       </c>
     </row>
     <row r="6">
@@ -2606,13 +2598,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-3.30458119250338</v>
+        <v>-1.01127397393401</v>
       </c>
       <c r="C6" t="n">
-        <v>0.91026131550173</v>
+        <v>0.932337078422503</v>
       </c>
       <c r="D6" t="n">
-        <v>0.000283020257736503</v>
+        <v>0.27806978074295</v>
       </c>
     </row>
     <row r="7">
@@ -2620,13 +2612,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-4.77237182726425</v>
+        <v>-5.23716093251764</v>
       </c>
       <c r="C7" t="n">
-        <v>0.807288187320429</v>
+        <v>12.4554408663258</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00000000338782691914456</v>
+        <v>0.674140867534233</v>
       </c>
     </row>
     <row r="8">
@@ -2634,13 +2626,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.55547215715677</v>
+        <v>1.45725880003159</v>
       </c>
       <c r="C8" t="n">
-        <v>0.875042089032136</v>
+        <v>0.63528096155391</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0754700734796012</v>
+        <v>0.0217973465847249</v>
       </c>
     </row>
     <row r="9">
@@ -2648,13 +2640,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.16396861112612</v>
+        <v>-1.72274911916047</v>
       </c>
       <c r="C9" t="n">
-        <v>1.04705893426996</v>
+        <v>1.33523999513731</v>
       </c>
       <c r="D9" t="n">
-        <v>0.000000814421077420427</v>
+        <v>0.19697538288805</v>
       </c>
     </row>
     <row r="10">
@@ -2662,13 +2654,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.97661347537519</v>
+        <v>-0.384527599158822</v>
       </c>
       <c r="C10" t="n">
-        <v>0.851225862576662</v>
+        <v>1.02540886924046</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000470777517397139</v>
+        <v>0.707660993793897</v>
       </c>
     </row>
     <row r="11">
@@ -2676,13 +2668,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-4.03090137628473</v>
+        <v>-5.20407102590059</v>
       </c>
       <c r="C11" t="n">
-        <v>0.876334520170271</v>
+        <v>40.5621218446947</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00000423040754834032</v>
+        <v>0.897912525103192</v>
       </c>
     </row>
     <row r="12">
@@ -2690,13 +2682,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.13200099776414</v>
+        <v>-3.18362628089906</v>
       </c>
       <c r="C12" t="n">
-        <v>1.16154346666499</v>
+        <v>1.54801078167911</v>
       </c>
       <c r="D12" t="n">
-        <v>0.329775488510455</v>
+        <v>0.0397255076041237</v>
       </c>
     </row>
     <row r="13">
@@ -2704,13 +2696,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.04046185351128</v>
+        <v>-5.93043878459935</v>
       </c>
       <c r="C13" t="n">
-        <v>1.68310723331235</v>
+        <v>2.24558990895221</v>
       </c>
       <c r="D13" t="n">
-        <v>0.225390526478034</v>
+        <v>0.00826795577584686</v>
       </c>
     </row>
     <row r="14">
@@ -2718,13 +2710,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.56782997670186</v>
+        <v>-7.09382529525264</v>
       </c>
       <c r="C14" t="n">
-        <v>1.80440496911179</v>
+        <v>2.49752648275794</v>
       </c>
       <c r="D14" t="n">
-        <v>0.154710177841274</v>
+        <v>0.00450654211861647</v>
       </c>
     </row>
     <row r="15">
@@ -2732,13 +2724,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-3.24133757766255</v>
+        <v>-6.9859325494539</v>
       </c>
       <c r="C15" t="n">
-        <v>1.77687223944553</v>
+        <v>2.50476169523193</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0681246280731995</v>
+        <v>0.00528611472540033</v>
       </c>
     </row>
     <row r="16">
@@ -2746,13 +2738,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-3.6857480249778</v>
+        <v>-6.32193424020449</v>
       </c>
       <c r="C16" t="n">
-        <v>1.70048730205045</v>
+        <v>2.3375280494704</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0301993567609542</v>
+        <v>0.00683993750772423</v>
       </c>
     </row>
     <row r="17">
@@ -2760,13 +2752,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-3.89783749088239</v>
+        <v>-5.88091794014399</v>
       </c>
       <c r="C17" t="n">
-        <v>1.64374296556388</v>
+        <v>2.15031821097157</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0177247676127386</v>
+        <v>0.00623981130848142</v>
       </c>
     </row>
     <row r="18">
@@ -2774,13 +2766,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-3.99418146633018</v>
+        <v>-5.7223695222892</v>
       </c>
       <c r="C18" t="n">
-        <v>1.61565907956938</v>
+        <v>2.04890879544729</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0134296204819783</v>
+        <v>0.00522400332781252</v>
       </c>
     </row>
     <row r="19">
@@ -2788,13 +2780,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-3.84248728327681</v>
+        <v>-5.3076533241389</v>
       </c>
       <c r="C19" t="n">
-        <v>1.61520892913251</v>
+        <v>2.04641909185465</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0173624390076182</v>
+        <v>0.00949687127309367</v>
       </c>
     </row>
     <row r="20">
@@ -2802,13 +2794,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-3.71733309417328</v>
+        <v>-5.04379259407137</v>
       </c>
       <c r="C20" t="n">
-        <v>1.66081755430062</v>
+        <v>2.11539561305439</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0252044347936263</v>
+        <v>0.0171104410393367</v>
       </c>
     </row>
     <row r="21">
@@ -2816,13 +2808,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.3212102587093</v>
+        <v>-4.80431512712981</v>
       </c>
       <c r="C21" t="n">
-        <v>1.6814262369765</v>
+        <v>2.16726859787823</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0482416000469013</v>
+        <v>0.0266394713259504</v>
       </c>
     </row>
     <row r="22">
@@ -2830,13 +2822,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-2.61329996161115</v>
+        <v>-4.4976754222135</v>
       </c>
       <c r="C22" t="n">
-        <v>1.71348572390215</v>
+        <v>2.19374627134785</v>
       </c>
       <c r="D22" t="n">
-        <v>0.12722500516967</v>
+        <v>0.0403423917403379</v>
       </c>
     </row>
     <row r="23">
@@ -2844,13 +2836,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.86421239245288</v>
+        <v>-4.22020817142323</v>
       </c>
       <c r="C23" t="n">
-        <v>2.13988260184279</v>
+        <v>2.66924305710593</v>
       </c>
       <c r="D23" t="n">
-        <v>0.383658565484165</v>
+        <v>0.113866482793387</v>
       </c>
     </row>
     <row r="24">
@@ -2858,13 +2850,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>1.18763568404331</v>
+        <v>0.300710509927211</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0390058758623999</v>
+        <v>0.16640196290246</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000128843872650272</v>
+        <v>0.0707415148980519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #15: Export the results to a .csv (#27)
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.39909375345095</v>
+        <v>-2.3991</v>
       </c>
       <c r="C2" t="n">
-        <v>62420.4525398934</v>
+        <v>62420.4525</v>
       </c>
       <c r="D2" t="n">
-        <v>0.999969333771425</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.621726438125615</v>
+        <v>-0.6217</v>
       </c>
       <c r="C3" t="n">
-        <v>0.446563396294826</v>
+        <v>0.4466</v>
       </c>
       <c r="D3" t="n">
-        <v>0.163847689793895</v>
+        <v>0.1638</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.346837641952026</v>
+        <v>-0.3468</v>
       </c>
       <c r="C4" t="n">
-        <v>0.358494562257901</v>
+        <v>0.3585</v>
       </c>
       <c r="D4" t="n">
-        <v>0.333302290818082</v>
+        <v>0.3333</v>
       </c>
     </row>
     <row r="5">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>3.83220696378058</v>
+        <v>3.8322</v>
       </c>
       <c r="C5" t="n">
-        <v>62420.4525255146</v>
+        <v>62420.4525</v>
       </c>
       <c r="D5" t="n">
-        <v>0.999951015113724</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.415959452875481</v>
+        <v>-0.416</v>
       </c>
       <c r="C6" t="n">
-        <v>83119.3212186157</v>
+        <v>83119.3212</v>
       </c>
       <c r="D6" t="n">
-        <v>0.999996007094133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -520,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.0571973230482257</v>
+        <v>-0.0572</v>
       </c>
       <c r="C7" t="n">
-        <v>80488.0075943448</v>
+        <v>80488.0076</v>
       </c>
       <c r="D7" t="n">
-        <v>0.999999432998004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -534,13 +534,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.775637968087059</v>
+        <v>0.7756</v>
       </c>
       <c r="C8" t="n">
-        <v>92489.6876247333</v>
+        <v>92489.6876</v>
       </c>
       <c r="D8" t="n">
-        <v>0.999993308772303</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -548,13 +548,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>3.81123870903567</v>
+        <v>3.8112</v>
       </c>
       <c r="C9" t="n">
-        <v>62420.4525255564</v>
+        <v>62420.4525</v>
       </c>
       <c r="D9" t="n">
-        <v>0.999951283138802</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -562,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>3.74202116607166</v>
+        <v>3.742</v>
       </c>
       <c r="C10" t="n">
-        <v>62420.4525252916</v>
+        <v>62420.4525</v>
       </c>
       <c r="D10" t="n">
-        <v>0.999952167906639</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -576,13 +576,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.317939108720248</v>
+        <v>-0.3179</v>
       </c>
       <c r="C11" t="n">
-        <v>83906.3177659629</v>
+        <v>83906.3178</v>
       </c>
       <c r="D11" t="n">
-        <v>0.999996976643561</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -590,13 +590,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.973735851366318</v>
+        <v>-0.9737</v>
       </c>
       <c r="C12" t="n">
-        <v>1.14334031208868</v>
+        <v>1.1433</v>
       </c>
       <c r="D12" t="n">
-        <v>0.394403487475458</v>
+        <v>0.3944</v>
       </c>
     </row>
     <row r="13">
@@ -604,13 +604,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.69128793957788</v>
+        <v>-1.6913</v>
       </c>
       <c r="C13" t="n">
-        <v>1.56989329119463</v>
+        <v>1.5699</v>
       </c>
       <c r="D13" t="n">
-        <v>0.281334343559962</v>
+        <v>0.2813</v>
       </c>
     </row>
     <row r="14">
@@ -618,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.58435939633627</v>
+        <v>-1.5844</v>
       </c>
       <c r="C14" t="n">
-        <v>1.55224082586339</v>
+        <v>1.5522</v>
       </c>
       <c r="D14" t="n">
-        <v>0.307400507066783</v>
+        <v>0.3074</v>
       </c>
     </row>
     <row r="15">
@@ -632,13 +632,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.03566860498879</v>
+        <v>-1.0357</v>
       </c>
       <c r="C15" t="n">
-        <v>1.38946683614383</v>
+        <v>1.3895</v>
       </c>
       <c r="D15" t="n">
-        <v>0.456047331093435</v>
+        <v>0.456</v>
       </c>
     </row>
     <row r="16">
@@ -646,13 +646,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.552095268289528</v>
+        <v>-0.5521</v>
       </c>
       <c r="C16" t="n">
-        <v>1.32275580150065</v>
+        <v>1.3228</v>
       </c>
       <c r="D16" t="n">
-        <v>0.676398572897828</v>
+        <v>0.6764</v>
       </c>
     </row>
     <row r="17">
@@ -660,13 +660,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.178518779772545</v>
+        <v>-0.1785</v>
       </c>
       <c r="C17" t="n">
-        <v>1.26830203636834</v>
+        <v>1.2683</v>
       </c>
       <c r="D17" t="n">
-        <v>0.888064162430655</v>
+        <v>0.8881</v>
       </c>
     </row>
     <row r="18">
@@ -674,13 +674,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.108125524782969</v>
+        <v>-0.1081</v>
       </c>
       <c r="C18" t="n">
-        <v>1.23430033652575</v>
+        <v>1.2343</v>
       </c>
       <c r="D18" t="n">
-        <v>0.930194077165221</v>
+        <v>0.9302</v>
       </c>
     </row>
     <row r="19">
@@ -688,13 +688,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.478542851681695</v>
+        <v>-0.4785</v>
       </c>
       <c r="C19" t="n">
-        <v>1.23744721552008</v>
+        <v>1.2374</v>
       </c>
       <c r="D19" t="n">
-        <v>0.698965144865284</v>
+        <v>0.699</v>
       </c>
     </row>
     <row r="20">
@@ -702,13 +702,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.707018679798631</v>
+        <v>-0.707</v>
       </c>
       <c r="C20" t="n">
-        <v>1.33615055931206</v>
+        <v>1.3362</v>
       </c>
       <c r="D20" t="n">
-        <v>0.596704196078925</v>
+        <v>0.5967</v>
       </c>
     </row>
     <row r="21">
@@ -716,13 +716,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.787972102479502</v>
+        <v>-0.788</v>
       </c>
       <c r="C21" t="n">
-        <v>1.39564683618295</v>
+        <v>1.3956</v>
       </c>
       <c r="D21" t="n">
-        <v>0.572350789285024</v>
+        <v>0.5724</v>
       </c>
     </row>
     <row r="22">
@@ -730,13 +730,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.837547376183614</v>
+        <v>-0.8375</v>
       </c>
       <c r="C22" t="n">
-        <v>1.76436770351332</v>
+        <v>1.7644</v>
       </c>
       <c r="D22" t="n">
-        <v>0.634999998830929</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="23">
@@ -744,13 +744,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.887078765314423</v>
+        <v>-0.8871</v>
       </c>
       <c r="C23" t="n">
-        <v>2.72866102915728</v>
+        <v>2.7287</v>
       </c>
       <c r="D23" t="n">
-        <v>0.745107867222508</v>
+        <v>0.7451</v>
       </c>
     </row>
     <row r="24">
@@ -758,13 +758,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.644780512481345</v>
+        <v>-0.6448</v>
       </c>
       <c r="C24" t="n">
-        <v>0.208200131659363</v>
+        <v>0.2082</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00195538326513929</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>
@@ -800,13 +800,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.87344337189236</v>
+        <v>1.8734</v>
       </c>
       <c r="C2" t="n">
-        <v>0.700792680433909</v>
+        <v>0.7008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00751044791351729</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="3">
@@ -814,13 +814,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.183062160944288</v>
+        <v>0.1831</v>
       </c>
       <c r="C3" t="n">
-        <v>0.183410500628311</v>
+        <v>0.1834</v>
       </c>
       <c r="D3" t="n">
-        <v>0.31823049932207</v>
+        <v>0.3182</v>
       </c>
     </row>
     <row r="4">
@@ -828,13 +828,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0930228721293085</v>
+        <v>0.093</v>
       </c>
       <c r="C4" t="n">
-        <v>0.170832307431283</v>
+        <v>0.1708</v>
       </c>
       <c r="D4" t="n">
-        <v>0.586078598863253</v>
+        <v>0.5861</v>
       </c>
     </row>
     <row r="5">
@@ -842,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1321907583995</v>
+        <v>-0.1322</v>
       </c>
       <c r="C5" t="n">
-        <v>0.323816503312254</v>
+        <v>0.3238</v>
       </c>
       <c r="D5" t="n">
-        <v>0.683106758379441</v>
+        <v>0.6831</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.12105693994151</v>
+        <v>-1.1211</v>
       </c>
       <c r="C6" t="n">
-        <v>0.356033394513466</v>
+        <v>0.356</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00163975464278277</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +870,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.377639777202835</v>
+        <v>0.3776</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304016139312999</v>
+        <v>0.304</v>
       </c>
       <c r="D7" t="n">
-        <v>0.214173785886877</v>
+        <v>0.2142</v>
       </c>
     </row>
     <row r="8">
@@ -884,13 +884,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.821756402549003</v>
+        <v>0.8218</v>
       </c>
       <c r="C8" t="n">
-        <v>0.319701329503895</v>
+        <v>0.3197</v>
       </c>
       <c r="D8" t="n">
-        <v>0.010158472210531</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="9">
@@ -898,13 +898,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.35849522573185</v>
+        <v>-1.3585</v>
       </c>
       <c r="C9" t="n">
-        <v>0.420233788296791</v>
+        <v>0.4202</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00122620690118946</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="10">
@@ -912,13 +912,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.861099148009334</v>
+        <v>-0.8611</v>
       </c>
       <c r="C10" t="n">
-        <v>0.324529533720654</v>
+        <v>0.3245</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00796908469785711</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="11">
@@ -926,13 +926,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0387198775245461</v>
+        <v>-0.0387</v>
       </c>
       <c r="C11" t="n">
-        <v>0.325526911155548</v>
+        <v>0.3255</v>
       </c>
       <c r="D11" t="n">
-        <v>0.905318737498331</v>
+        <v>0.9053</v>
       </c>
     </row>
     <row r="12">
@@ -940,13 +940,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.564998778904266</v>
+        <v>-0.565</v>
       </c>
       <c r="C12" t="n">
-        <v>0.485716135157964</v>
+        <v>0.4857</v>
       </c>
       <c r="D12" t="n">
-        <v>0.244736866701062</v>
+        <v>0.2447</v>
       </c>
     </row>
     <row r="13">
@@ -954,13 +954,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.05729719321019</v>
+        <v>-1.0573</v>
       </c>
       <c r="C13" t="n">
-        <v>0.697494778217006</v>
+        <v>0.6975</v>
       </c>
       <c r="D13" t="n">
-        <v>0.129557382297949</v>
+        <v>0.1296</v>
       </c>
     </row>
     <row r="14">
@@ -968,13 +968,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.28542080199948</v>
+        <v>-1.2854</v>
       </c>
       <c r="C14" t="n">
-        <v>0.740278039169894</v>
+        <v>0.7403</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0824926513703027</v>
+        <v>0.0825</v>
       </c>
     </row>
     <row r="15">
@@ -982,13 +982,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.41578815361765</v>
+        <v>-1.4158</v>
       </c>
       <c r="C15" t="n">
-        <v>0.728684508681899</v>
+        <v>0.7287</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0520237607165542</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="16">
@@ -996,13 +996,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.30314677801982</v>
+        <v>-1.3031</v>
       </c>
       <c r="C16" t="n">
-        <v>0.698657237185131</v>
+        <v>0.6987</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0621511095168702</v>
+        <v>0.0622</v>
       </c>
     </row>
     <row r="17">
@@ -1010,13 +1010,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.09277975165252</v>
+        <v>-1.0928</v>
       </c>
       <c r="C17" t="n">
-        <v>0.672031993071463</v>
+        <v>0.672</v>
       </c>
       <c r="D17" t="n">
-        <v>0.103932015032744</v>
+        <v>0.1039</v>
       </c>
     </row>
     <row r="18">
@@ -1024,13 +1024,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.03818696892916</v>
+        <v>-1.0382</v>
       </c>
       <c r="C18" t="n">
-        <v>0.657653502071145</v>
+        <v>0.6577</v>
       </c>
       <c r="D18" t="n">
-        <v>0.114422547327424</v>
+        <v>0.1144</v>
       </c>
     </row>
     <row r="19">
@@ -1038,13 +1038,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.13035524651131</v>
+        <v>-1.1304</v>
       </c>
       <c r="C19" t="n">
-        <v>0.657506776848006</v>
+        <v>0.6575</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0855863782746068</v>
+        <v>0.0856</v>
       </c>
     </row>
     <row r="20">
@@ -1052,13 +1052,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.05174806831519</v>
+        <v>-1.0517</v>
       </c>
       <c r="C20" t="n">
-        <v>0.675630795008506</v>
+        <v>0.6756</v>
       </c>
       <c r="D20" t="n">
-        <v>0.119543975327657</v>
+        <v>0.1195</v>
       </c>
     </row>
     <row r="21">
@@ -1066,13 +1066,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.93456171186514</v>
+        <v>-0.9346</v>
       </c>
       <c r="C21" t="n">
-        <v>0.683281959505787</v>
+        <v>0.6833</v>
       </c>
       <c r="D21" t="n">
-        <v>0.171389054787642</v>
+        <v>0.1714</v>
       </c>
     </row>
     <row r="22">
@@ -1080,13 +1080,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.13360040303422</v>
+        <v>-1.1336</v>
       </c>
       <c r="C22" t="n">
-        <v>0.695163678473655</v>
+        <v>0.6952</v>
       </c>
       <c r="D22" t="n">
-        <v>0.102954549911525</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="23">
@@ -1094,13 +1094,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.4025892235245</v>
+        <v>-1.4026</v>
       </c>
       <c r="C23" t="n">
-        <v>0.87400605496044</v>
+        <v>0.874</v>
       </c>
       <c r="D23" t="n">
-        <v>0.108541778870265</v>
+        <v>0.1085</v>
       </c>
     </row>
     <row r="24">
@@ -1108,13 +1108,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.232917522181786</v>
+        <v>0.2329</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0549784234871216</v>
+        <v>0.055</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000022700461552089</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1150,13 +1150,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.63985760396549</v>
+        <v>-1.6399</v>
       </c>
       <c r="C2" t="n">
-        <v>1.7119847068233</v>
+        <v>1.712</v>
       </c>
       <c r="D2" t="n">
-        <v>0.338128665494533</v>
+        <v>0.3381</v>
       </c>
     </row>
     <row r="3">
@@ -1164,13 +1164,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.119268163369971</v>
+        <v>-0.1193</v>
       </c>
       <c r="C3" t="n">
-        <v>0.336747928873695</v>
+        <v>0.3367</v>
       </c>
       <c r="D3" t="n">
-        <v>0.723206701711976</v>
+        <v>0.7232</v>
       </c>
     </row>
     <row r="4">
@@ -1178,13 +1178,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.178101232029074</v>
+        <v>-0.1781</v>
       </c>
       <c r="C4" t="n">
-        <v>0.364103154406656</v>
+        <v>0.3641</v>
       </c>
       <c r="D4" t="n">
-        <v>0.624735166663663</v>
+        <v>0.6247</v>
       </c>
     </row>
     <row r="5">
@@ -1192,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.22544325378988</v>
+        <v>-1.2254</v>
       </c>
       <c r="C5" t="n">
-        <v>0.69844192290108</v>
+        <v>0.6984</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0793382764903816</v>
+        <v>0.0793</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1206,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.102629469930867</v>
+        <v>-0.1026</v>
       </c>
       <c r="C6" t="n">
-        <v>1.10090224972129</v>
+        <v>1.1009</v>
       </c>
       <c r="D6" t="n">
-        <v>0.925726359654848</v>
+        <v>0.9257</v>
       </c>
     </row>
     <row r="7">
@@ -1220,13 +1220,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.42266763175141</v>
+        <v>0.4227</v>
       </c>
       <c r="C7" t="n">
-        <v>0.713752428241443</v>
+        <v>0.7138</v>
       </c>
       <c r="D7" t="n">
-        <v>0.553732200594692</v>
+        <v>0.5537</v>
       </c>
     </row>
     <row r="8">
@@ -1254,13 +1254,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.556340293043207</v>
+        <v>0.5563</v>
       </c>
       <c r="C10" t="n">
-        <v>0.736415560952545</v>
+        <v>0.7364</v>
       </c>
       <c r="D10" t="n">
-        <v>0.449966676533983</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="11">
@@ -1268,13 +1268,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.247554106150954</v>
+        <v>-0.2476</v>
       </c>
       <c r="C11" t="n">
-        <v>1.04768200033696</v>
+        <v>1.0477</v>
       </c>
       <c r="D11" t="n">
-        <v>0.813209626275475</v>
+        <v>0.8132</v>
       </c>
     </row>
     <row r="12">
@@ -1282,13 +1282,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0679442525922799</v>
+        <v>0.0679</v>
       </c>
       <c r="C12" t="n">
-        <v>1.05191018149522</v>
+        <v>1.0519</v>
       </c>
       <c r="D12" t="n">
-        <v>0.948499406930426</v>
+        <v>0.9485</v>
       </c>
     </row>
     <row r="13">
@@ -1296,13 +1296,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.143798307076691</v>
+        <v>0.1438</v>
       </c>
       <c r="C13" t="n">
-        <v>1.59378385483527</v>
+        <v>1.5938</v>
       </c>
       <c r="D13" t="n">
-        <v>0.928108837643466</v>
+        <v>0.9281</v>
       </c>
     </row>
     <row r="14">
@@ -1310,13 +1310,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.249830958106449</v>
+        <v>0.2498</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7451710978706</v>
+        <v>1.7452</v>
       </c>
       <c r="D14" t="n">
-        <v>0.88616732066207</v>
+        <v>0.8862</v>
       </c>
     </row>
     <row r="15">
@@ -1324,13 +1324,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.369631336503031</v>
+        <v>0.3696</v>
       </c>
       <c r="C15" t="n">
-        <v>1.72149704582523</v>
+        <v>1.7215</v>
       </c>
       <c r="D15" t="n">
-        <v>0.829989482493843</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="16">
@@ -1338,13 +1338,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.468118911313132</v>
+        <v>0.4681</v>
       </c>
       <c r="C16" t="n">
-        <v>1.66711784833335</v>
+        <v>1.6671</v>
       </c>
       <c r="D16" t="n">
-        <v>0.778867383431452</v>
+        <v>0.7789</v>
       </c>
     </row>
     <row r="17">
@@ -1352,13 +1352,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.507487011531612</v>
+        <v>0.5075</v>
       </c>
       <c r="C17" t="n">
-        <v>1.61437219466819</v>
+        <v>1.6144</v>
       </c>
       <c r="D17" t="n">
-        <v>0.753250940428615</v>
+        <v>0.7533</v>
       </c>
     </row>
     <row r="18">
@@ -1366,13 +1366,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.484083843909326</v>
+        <v>0.4841</v>
       </c>
       <c r="C18" t="n">
-        <v>1.59680811921259</v>
+        <v>1.5968</v>
       </c>
       <c r="D18" t="n">
-        <v>0.761770080970127</v>
+        <v>0.7618</v>
       </c>
     </row>
     <row r="19">
@@ -1380,13 +1380,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.377353312920755</v>
+        <v>0.3774</v>
       </c>
       <c r="C19" t="n">
-        <v>1.59908776690256</v>
+        <v>1.5991</v>
       </c>
       <c r="D19" t="n">
-        <v>0.813447907373067</v>
+        <v>0.8134</v>
       </c>
     </row>
     <row r="20">
@@ -1394,13 +1394,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.221082067033935</v>
+        <v>0.2211</v>
       </c>
       <c r="C20" t="n">
-        <v>1.631638168552</v>
+        <v>1.6316</v>
       </c>
       <c r="D20" t="n">
-        <v>0.892218940830233</v>
+        <v>0.8922</v>
       </c>
     </row>
     <row r="21">
@@ -1408,13 +1408,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0864441601164589</v>
+        <v>0.0864</v>
       </c>
       <c r="C21" t="n">
-        <v>1.63848131917373</v>
+        <v>1.6385</v>
       </c>
       <c r="D21" t="n">
-        <v>0.957924160613751</v>
+        <v>0.9579</v>
       </c>
     </row>
     <row r="22">
@@ -1422,13 +1422,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.00510728173720448</v>
+        <v>0.0051</v>
       </c>
       <c r="C22" t="n">
-        <v>1.64115674043549</v>
+        <v>1.6412</v>
       </c>
       <c r="D22" t="n">
-        <v>0.997516986301226</v>
+        <v>0.9975</v>
       </c>
     </row>
     <row r="23">
@@ -1436,13 +1436,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0627879417631931</v>
+        <v>-0.0628</v>
       </c>
       <c r="C23" t="n">
-        <v>1.94811596841063</v>
+        <v>1.9481</v>
       </c>
       <c r="D23" t="n">
-        <v>0.974288564885443</v>
+        <v>0.9743</v>
       </c>
     </row>
     <row r="24">
@@ -1450,7 +1450,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.54117999425717</v>
+        <v>0.5412</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -1492,13 +1492,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.80921671535414</v>
+        <v>2.8092</v>
       </c>
       <c r="C2" t="n">
-        <v>0.17971370267126</v>
+        <v>0.1797</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000000000000000000000000000000000000000000000000443369840522243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1506,13 +1506,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0311812545682837</v>
+        <v>0.0312</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0490708280547933</v>
+        <v>0.0491</v>
       </c>
       <c r="D3" t="n">
-        <v>0.525145638145358</v>
+        <v>0.5251</v>
       </c>
     </row>
     <row r="4">
@@ -1520,13 +1520,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0392402105844459</v>
+        <v>0.0392</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0460097081402118</v>
+        <v>0.046</v>
       </c>
       <c r="D4" t="n">
-        <v>0.393732475083097</v>
+        <v>0.3937</v>
       </c>
     </row>
     <row r="5">
@@ -1534,13 +1534,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0530443618803046</v>
+        <v>-0.053</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0902600601625659</v>
+        <v>0.0903</v>
       </c>
       <c r="D5" t="n">
-        <v>0.556744649907599</v>
+        <v>0.5567</v>
       </c>
     </row>
     <row r="6">
@@ -1548,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0402986182974082</v>
+        <v>0.0403</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0823863715467429</v>
+        <v>0.0824</v>
       </c>
       <c r="D6" t="n">
-        <v>0.624741308096634</v>
+        <v>0.6247</v>
       </c>
     </row>
     <row r="7">
@@ -1562,13 +1562,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.137599147008558</v>
+        <v>-0.1376</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0857643887189523</v>
+        <v>0.0858</v>
       </c>
       <c r="D7" t="n">
-        <v>0.108629091472212</v>
+        <v>0.1086</v>
       </c>
     </row>
     <row r="8">
@@ -1576,13 +1576,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0719631758589172</v>
+        <v>-0.072</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0931481340208779</v>
+        <v>0.0931</v>
       </c>
       <c r="D8" t="n">
-        <v>0.439778671870282</v>
+        <v>0.4398</v>
       </c>
     </row>
     <row r="9">
@@ -1590,13 +1590,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.178165127817341</v>
+        <v>-0.1782</v>
       </c>
       <c r="C9" t="n">
-        <v>0.104990486716803</v>
+        <v>0.105</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0897033740931516</v>
+        <v>0.0897</v>
       </c>
     </row>
     <row r="10">
@@ -1604,13 +1604,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.00382618498303945</v>
+        <v>0.0038</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0809810829033103</v>
+        <v>0.081</v>
       </c>
       <c r="D10" t="n">
-        <v>0.962315662505998</v>
+        <v>0.9623</v>
       </c>
     </row>
     <row r="11">
@@ -1618,13 +1618,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.116371816022432</v>
+        <v>-0.1164</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0933863872994384</v>
+        <v>0.0934</v>
       </c>
       <c r="D11" t="n">
-        <v>0.212715740220356</v>
+        <v>0.2127</v>
       </c>
     </row>
     <row r="12">
@@ -1632,13 +1632,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0717851526046283</v>
+        <v>-0.0718</v>
       </c>
       <c r="C12" t="n">
-        <v>0.128340297560921</v>
+        <v>0.1283</v>
       </c>
       <c r="D12" t="n">
-        <v>0.575933473140579</v>
+        <v>0.5759</v>
       </c>
     </row>
     <row r="13">
@@ -1646,13 +1646,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.133660251290937</v>
+        <v>-0.1337</v>
       </c>
       <c r="C13" t="n">
-        <v>0.179610977150743</v>
+        <v>0.1796</v>
       </c>
       <c r="D13" t="n">
-        <v>0.45677649620694</v>
+        <v>0.4568</v>
       </c>
     </row>
     <row r="14">
@@ -1660,13 +1660,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.15030957941767</v>
+        <v>-0.1503</v>
       </c>
       <c r="C14" t="n">
-        <v>0.187033705783792</v>
+        <v>0.187</v>
       </c>
       <c r="D14" t="n">
-        <v>0.421599317918137</v>
+        <v>0.4216</v>
       </c>
     </row>
     <row r="15">
@@ -1674,13 +1674,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.17458224909525</v>
+        <v>-0.1746</v>
       </c>
       <c r="C15" t="n">
-        <v>0.183424234839812</v>
+        <v>0.1834</v>
       </c>
       <c r="D15" t="n">
-        <v>0.341201015010159</v>
+        <v>0.3412</v>
       </c>
     </row>
     <row r="16">
@@ -1688,13 +1688,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.220741946719498</v>
+        <v>-0.2207</v>
       </c>
       <c r="C16" t="n">
-        <v>0.175879982929213</v>
+        <v>0.1759</v>
       </c>
       <c r="D16" t="n">
-        <v>0.209452820384383</v>
+        <v>0.2095</v>
       </c>
     </row>
     <row r="17">
@@ -1702,13 +1702,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.247196309050597</v>
+        <v>-0.2472</v>
       </c>
       <c r="C17" t="n">
-        <v>0.170779236598456</v>
+        <v>0.1708</v>
       </c>
       <c r="D17" t="n">
-        <v>0.147767811700006</v>
+        <v>0.1478</v>
       </c>
     </row>
     <row r="18">
@@ -1716,13 +1716,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.233535084545207</v>
+        <v>-0.2335</v>
       </c>
       <c r="C18" t="n">
-        <v>0.167087630976878</v>
+        <v>0.1671</v>
       </c>
       <c r="D18" t="n">
-        <v>0.162209102777322</v>
+        <v>0.1622</v>
       </c>
     </row>
     <row r="19">
@@ -1730,13 +1730,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.199407339193454</v>
+        <v>-0.1994</v>
       </c>
       <c r="C19" t="n">
-        <v>0.166605134964734</v>
+        <v>0.1666</v>
       </c>
       <c r="D19" t="n">
-        <v>0.231351025308984</v>
+        <v>0.2314</v>
       </c>
     </row>
     <row r="20">
@@ -1744,13 +1744,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.195575636546001</v>
+        <v>-0.1956</v>
       </c>
       <c r="C20" t="n">
-        <v>0.17327044805438</v>
+        <v>0.1733</v>
       </c>
       <c r="D20" t="n">
-        <v>0.259011545939185</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="21">
@@ -1758,13 +1758,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.205999822162982</v>
+        <v>-0.206</v>
       </c>
       <c r="C21" t="n">
-        <v>0.177325960331365</v>
+        <v>0.1773</v>
       </c>
       <c r="D21" t="n">
-        <v>0.245356763577084</v>
+        <v>0.2454</v>
       </c>
     </row>
     <row r="22">
@@ -1772,13 +1772,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.174246659552308</v>
+        <v>-0.1742</v>
       </c>
       <c r="C22" t="n">
-        <v>0.181883022830822</v>
+        <v>0.1819</v>
       </c>
       <c r="D22" t="n">
-        <v>0.33805520744544</v>
+        <v>0.3381</v>
       </c>
     </row>
     <row r="23">
@@ -1786,13 +1786,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.130172041649697</v>
+        <v>-0.1302</v>
       </c>
       <c r="C23" t="n">
-        <v>0.234320638206979</v>
+        <v>0.2343</v>
       </c>
       <c r="D23" t="n">
-        <v>0.578532495223294</v>
+        <v>0.5785</v>
       </c>
     </row>
     <row r="24">
@@ -1800,13 +1800,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.50924124144369</v>
+        <v>-1.5092</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0795660774058807</v>
+        <v>0.0796</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000311231882259371</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1842,13 +1842,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0942210348075</v>
+        <v>3.0942</v>
       </c>
       <c r="C2" t="n">
-        <v>0.374278601057852</v>
+        <v>0.3743</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000000000137187930526539</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1856,13 +1856,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0018233624772592</v>
+        <v>-0.0018</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0958362360129506</v>
+        <v>0.0958</v>
       </c>
       <c r="D3" t="n">
-        <v>0.984820511904647</v>
+        <v>0.9848</v>
       </c>
     </row>
     <row r="4">
@@ -1870,13 +1870,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.000884055833716306</v>
+        <v>-0.0009</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0900396542386214</v>
+        <v>0.09</v>
       </c>
       <c r="D4" t="n">
-        <v>0.992166083118184</v>
+        <v>0.9922</v>
       </c>
     </row>
     <row r="5">
@@ -1884,13 +1884,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00168418118929125</v>
+        <v>0.0017</v>
       </c>
       <c r="C5" t="n">
-        <v>0.18722871366248</v>
+        <v>0.1872</v>
       </c>
       <c r="D5" t="n">
-        <v>0.992822874118568</v>
+        <v>0.9928</v>
       </c>
     </row>
     <row r="6">
@@ -1898,13 +1898,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.179948245896301</v>
+        <v>0.1799</v>
       </c>
       <c r="C6" t="n">
-        <v>0.186679542470245</v>
+        <v>0.1867</v>
       </c>
       <c r="D6" t="n">
-        <v>0.335075020443712</v>
+        <v>0.3351</v>
       </c>
     </row>
     <row r="7">
@@ -1912,13 +1912,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.313591601023681</v>
+        <v>-0.3136</v>
       </c>
       <c r="C7" t="n">
-        <v>0.18349091225726</v>
+        <v>0.1835</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874452641308215</v>
+        <v>0.0874</v>
       </c>
     </row>
     <row r="8">
@@ -1926,13 +1926,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.171476049410045</v>
+        <v>-0.1715</v>
       </c>
       <c r="C8" t="n">
-        <v>0.204153038738045</v>
+        <v>0.2042</v>
       </c>
       <c r="D8" t="n">
-        <v>0.40094272610526</v>
+        <v>0.4009</v>
       </c>
     </row>
     <row r="9">
@@ -1940,13 +1940,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0584331618589349</v>
+        <v>0.0584</v>
       </c>
       <c r="C9" t="n">
-        <v>0.218043606032045</v>
+        <v>0.218</v>
       </c>
       <c r="D9" t="n">
-        <v>0.78870823096141</v>
+        <v>0.7887</v>
       </c>
     </row>
     <row r="10">
@@ -1954,13 +1954,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.395004633748591</v>
+        <v>0.395</v>
       </c>
       <c r="C10" t="n">
-        <v>0.17039983116384</v>
+        <v>0.1704</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0204436365692366</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="11">
@@ -1968,13 +1968,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0789423134082052</v>
+        <v>-0.0789</v>
       </c>
       <c r="C11" t="n">
-        <v>0.195759283366634</v>
+        <v>0.1958</v>
       </c>
       <c r="D11" t="n">
-        <v>0.686755368363364</v>
+        <v>0.6868</v>
       </c>
     </row>
     <row r="12">
@@ -1982,13 +1982,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.323188701534309</v>
+        <v>-0.3232</v>
       </c>
       <c r="C12" t="n">
-        <v>0.266760143374256</v>
+        <v>0.2668</v>
       </c>
       <c r="D12" t="n">
-        <v>0.225691217014766</v>
+        <v>0.2257</v>
       </c>
     </row>
     <row r="13">
@@ -1996,13 +1996,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.613236545029909</v>
+        <v>-0.6132</v>
       </c>
       <c r="C13" t="n">
-        <v>0.374045116129475</v>
+        <v>0.374</v>
       </c>
       <c r="D13" t="n">
-        <v>0.101114969365379</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="14">
@@ -2010,13 +2010,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.688493638434468</v>
+        <v>-0.6885</v>
       </c>
       <c r="C14" t="n">
-        <v>0.392585109734575</v>
+        <v>0.3926</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0794744446092783</v>
+        <v>0.0795</v>
       </c>
     </row>
     <row r="15">
@@ -2024,13 +2024,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.584239368799399</v>
+        <v>-0.5842</v>
       </c>
       <c r="C15" t="n">
-        <v>0.383659419522862</v>
+        <v>0.3837</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1278069204593</v>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="16">
@@ -2038,13 +2038,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.472078083046865</v>
+        <v>-0.4721</v>
       </c>
       <c r="C16" t="n">
-        <v>0.362257271919948</v>
+        <v>0.3623</v>
       </c>
       <c r="D16" t="n">
-        <v>0.192521182694599</v>
+        <v>0.1925</v>
       </c>
     </row>
     <row r="17">
@@ -2052,13 +2052,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.377150049585725</v>
+        <v>-0.3772</v>
       </c>
       <c r="C17" t="n">
-        <v>0.34857958331942</v>
+        <v>0.3486</v>
       </c>
       <c r="D17" t="n">
-        <v>0.279269175720271</v>
+        <v>0.2793</v>
       </c>
     </row>
     <row r="18">
@@ -2066,13 +2066,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.341141072721015</v>
+        <v>-0.3411</v>
       </c>
       <c r="C18" t="n">
-        <v>0.342756922556087</v>
+        <v>0.3428</v>
       </c>
       <c r="D18" t="n">
-        <v>0.319597317780357</v>
+        <v>0.3196</v>
       </c>
     </row>
     <row r="19">
@@ -2080,13 +2080,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.371409432904821</v>
+        <v>-0.3714</v>
       </c>
       <c r="C19" t="n">
-        <v>0.342501725314751</v>
+        <v>0.3425</v>
       </c>
       <c r="D19" t="n">
-        <v>0.278186756556359</v>
+        <v>0.2782</v>
       </c>
     </row>
     <row r="20">
@@ -2094,13 +2094,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.423721884485117</v>
+        <v>-0.4237</v>
       </c>
       <c r="C20" t="n">
-        <v>0.358940738430898</v>
+        <v>0.3589</v>
       </c>
       <c r="D20" t="n">
-        <v>0.237809890191846</v>
+        <v>0.2378</v>
       </c>
     </row>
     <row r="21">
@@ -2108,13 +2108,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.465170008006705</v>
+        <v>-0.4652</v>
       </c>
       <c r="C21" t="n">
-        <v>0.371703588638339</v>
+        <v>0.3717</v>
       </c>
       <c r="D21" t="n">
-        <v>0.210768822413617</v>
+        <v>0.2108</v>
       </c>
     </row>
     <row r="22">
@@ -2122,13 +2122,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.51025058521999</v>
+        <v>-0.5103</v>
       </c>
       <c r="C22" t="n">
-        <v>0.388498067555917</v>
+        <v>0.3885</v>
       </c>
       <c r="D22" t="n">
-        <v>0.189050604650804</v>
+        <v>0.1891</v>
       </c>
     </row>
     <row r="23">
@@ -2136,13 +2136,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.564670607661701</v>
+        <v>-0.5647</v>
       </c>
       <c r="C23" t="n">
-        <v>0.506301873102446</v>
+        <v>0.5063</v>
       </c>
       <c r="D23" t="n">
-        <v>0.264728545492681</v>
+        <v>0.2647</v>
       </c>
     </row>
     <row r="24">
@@ -2150,13 +2150,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.845226728084796</v>
+        <v>-0.8452</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0784253825954999</v>
+        <v>0.0784</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00000000000000000000000000439845636742376</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2192,13 +2192,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.2969057781922</v>
+        <v>1.2969</v>
       </c>
       <c r="C2" t="n">
-        <v>0.301976620366303</v>
+        <v>0.302</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000017491200275895</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2206,13 +2206,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.358299583071426</v>
+        <v>-0.3583</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0817359408466906</v>
+        <v>0.0817</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0000116721481454232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2220,13 +2220,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.446931567738043</v>
+        <v>-0.4469</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0836292150471837</v>
+        <v>0.0836</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000000908153523362293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2234,13 +2234,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.280407229496759</v>
+        <v>-0.2804</v>
       </c>
       <c r="C5" t="n">
-        <v>0.180269665044719</v>
+        <v>0.1803</v>
       </c>
       <c r="D5" t="n">
-        <v>0.119829984378295</v>
+        <v>0.1198</v>
       </c>
     </row>
     <row r="6">
@@ -2248,13 +2248,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.83268591652951</v>
+        <v>0.8327</v>
       </c>
       <c r="C6" t="n">
-        <v>0.158404954630576</v>
+        <v>0.1584</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00000014667035339377</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2262,13 +2262,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.255770064964641</v>
+        <v>0.2558</v>
       </c>
       <c r="C7" t="n">
-        <v>0.149635907652562</v>
+        <v>0.1496</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0873986003550043</v>
+        <v>0.0874</v>
       </c>
     </row>
     <row r="8">
@@ -2276,13 +2276,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.03090488684111</v>
+        <v>-1.0309</v>
       </c>
       <c r="C8" t="n">
-        <v>0.201040535432247</v>
+        <v>0.201</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000000293076163738361</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2290,13 +2290,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.704448297634375</v>
+        <v>0.7044</v>
       </c>
       <c r="C9" t="n">
-        <v>0.179504804511613</v>
+        <v>0.1795</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0000869468847603924</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="10">
@@ -2304,13 +2304,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.602560533319542</v>
+        <v>0.6026</v>
       </c>
       <c r="C10" t="n">
-        <v>0.155945647351354</v>
+        <v>0.1559</v>
       </c>
       <c r="D10" t="n">
-        <v>0.000111584628811875</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="11">
@@ -2318,13 +2318,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0585492487112331</v>
+        <v>-0.0585</v>
       </c>
       <c r="C11" t="n">
-        <v>0.20959025422241</v>
+        <v>0.2096</v>
       </c>
       <c r="D11" t="n">
-        <v>0.779975465192125</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="12">
@@ -2332,13 +2332,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0269242355406962</v>
+        <v>0.0269</v>
       </c>
       <c r="C12" t="n">
-        <v>0.207330862653963</v>
+        <v>0.2073</v>
       </c>
       <c r="D12" t="n">
-        <v>0.896676238685559</v>
+        <v>0.8967</v>
       </c>
     </row>
     <row r="13">
@@ -2346,13 +2346,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.052308310572871</v>
+        <v>0.0523</v>
       </c>
       <c r="C13" t="n">
-        <v>0.289020898077135</v>
+        <v>0.289</v>
       </c>
       <c r="D13" t="n">
-        <v>0.85637972100604</v>
+        <v>0.8564</v>
       </c>
     </row>
     <row r="14">
@@ -2360,13 +2360,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0778760728399267</v>
+        <v>0.0779</v>
       </c>
       <c r="C14" t="n">
-        <v>0.30112299363397</v>
+        <v>0.3011</v>
       </c>
       <c r="D14" t="n">
-        <v>0.795929362037257</v>
+        <v>0.7959</v>
       </c>
     </row>
     <row r="15">
@@ -2374,13 +2374,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0991995481238758</v>
+        <v>0.0992</v>
       </c>
       <c r="C15" t="n">
-        <v>0.295164560658492</v>
+        <v>0.2952</v>
       </c>
       <c r="D15" t="n">
-        <v>0.736808898202418</v>
+        <v>0.7368</v>
       </c>
     </row>
     <row r="16">
@@ -2388,13 +2388,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0602266881069433</v>
+        <v>0.0602</v>
       </c>
       <c r="C16" t="n">
-        <v>0.282782391858891</v>
+        <v>0.2828</v>
       </c>
       <c r="D16" t="n">
-        <v>0.831343405725632</v>
+        <v>0.8313</v>
       </c>
     </row>
     <row r="17">
@@ -2402,13 +2402,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0191399367893719</v>
+        <v>0.0191</v>
       </c>
       <c r="C17" t="n">
-        <v>0.27656870770341</v>
+        <v>0.2766</v>
       </c>
       <c r="D17" t="n">
-        <v>0.944826445032952</v>
+        <v>0.9448</v>
       </c>
     </row>
     <row r="18">
@@ -2416,13 +2416,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0500879153338468</v>
+        <v>-0.0501</v>
       </c>
       <c r="C18" t="n">
-        <v>0.273721297366712</v>
+        <v>0.2737</v>
       </c>
       <c r="D18" t="n">
-        <v>0.854806853573217</v>
+        <v>0.8548</v>
       </c>
     </row>
     <row r="19">
@@ -2430,13 +2430,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.11586269795559</v>
+        <v>-0.1159</v>
       </c>
       <c r="C19" t="n">
-        <v>0.272998437927959</v>
+        <v>0.273</v>
       </c>
       <c r="D19" t="n">
-        <v>0.67126834905191</v>
+        <v>0.6713</v>
       </c>
     </row>
     <row r="20">
@@ -2444,13 +2444,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.0912120596425448</v>
+        <v>-0.0912</v>
       </c>
       <c r="C20" t="n">
-        <v>0.284289075261788</v>
+        <v>0.2843</v>
       </c>
       <c r="D20" t="n">
-        <v>0.748329638279143</v>
+        <v>0.7483</v>
       </c>
     </row>
     <row r="21">
@@ -2458,13 +2458,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0396405836665468</v>
+        <v>0.0396</v>
       </c>
       <c r="C21" t="n">
-        <v>0.289731962166835</v>
+        <v>0.2897</v>
       </c>
       <c r="D21" t="n">
-        <v>0.891174557100648</v>
+        <v>0.8912</v>
       </c>
     </row>
     <row r="22">
@@ -2472,13 +2472,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.186404419725476</v>
+        <v>0.1864</v>
       </c>
       <c r="C22" t="n">
-        <v>0.29404053812076</v>
+        <v>0.294</v>
       </c>
       <c r="D22" t="n">
-        <v>0.526119178466631</v>
+        <v>0.5261</v>
       </c>
     </row>
     <row r="23">
@@ -2486,13 +2486,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.335308635618812</v>
+        <v>0.3353</v>
       </c>
       <c r="C23" t="n">
-        <v>0.378533932614072</v>
+        <v>0.3785</v>
       </c>
       <c r="D23" t="n">
-        <v>0.37572064245356</v>
+        <v>0.3757</v>
       </c>
     </row>
     <row r="24">
@@ -2500,13 +2500,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.738426191743074</v>
+        <v>-0.7384</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0537767234145931</v>
+        <v>0.0538</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000000000000000000000000000000000000000000659080114814377</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2542,13 +2542,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.25402503775698</v>
+        <v>3.254</v>
       </c>
       <c r="C2" t="n">
-        <v>2.13881401084254</v>
+        <v>2.1388</v>
       </c>
       <c r="D2" t="n">
-        <v>0.128155572292059</v>
+        <v>0.1282</v>
       </c>
     </row>
     <row r="3">
@@ -2556,13 +2556,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.53907634076338</v>
+        <v>1.5391</v>
       </c>
       <c r="C3" t="n">
-        <v>0.574731256408406</v>
+        <v>0.5747</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00740839828488199</v>
+        <v>0.0074</v>
       </c>
     </row>
     <row r="4">
@@ -2570,13 +2570,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.710125630822808</v>
+        <v>0.7101</v>
       </c>
       <c r="C4" t="n">
-        <v>0.547540426182637</v>
+        <v>0.5475</v>
       </c>
       <c r="D4" t="n">
-        <v>0.194652743043003</v>
+        <v>0.1947</v>
       </c>
     </row>
     <row r="5">
@@ -2584,13 +2584,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.923979976331419</v>
+        <v>0.924</v>
       </c>
       <c r="C5" t="n">
-        <v>0.703277924798839</v>
+        <v>0.7033</v>
       </c>
       <c r="D5" t="n">
-        <v>0.188907085510505</v>
+        <v>0.1889</v>
       </c>
     </row>
     <row r="6">
@@ -2598,13 +2598,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.01127397393401</v>
+        <v>-1.0113</v>
       </c>
       <c r="C6" t="n">
-        <v>0.932337078422503</v>
+        <v>0.9323</v>
       </c>
       <c r="D6" t="n">
-        <v>0.27806978074295</v>
+        <v>0.2781</v>
       </c>
     </row>
     <row r="7">
@@ -2612,13 +2612,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-5.23716093251764</v>
+        <v>-5.2372</v>
       </c>
       <c r="C7" t="n">
-        <v>12.4554408663258</v>
+        <v>12.4554</v>
       </c>
       <c r="D7" t="n">
-        <v>0.674140867534233</v>
+        <v>0.6741</v>
       </c>
     </row>
     <row r="8">
@@ -2626,13 +2626,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.45725880003159</v>
+        <v>1.4573</v>
       </c>
       <c r="C8" t="n">
-        <v>0.63528096155391</v>
+        <v>0.6353</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0217973465847249</v>
+        <v>0.0218</v>
       </c>
     </row>
     <row r="9">
@@ -2640,13 +2640,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.72274911916047</v>
+        <v>-1.7227</v>
       </c>
       <c r="C9" t="n">
-        <v>1.33523999513731</v>
+        <v>1.3352</v>
       </c>
       <c r="D9" t="n">
-        <v>0.19697538288805</v>
+        <v>0.197</v>
       </c>
     </row>
     <row r="10">
@@ -2654,13 +2654,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.384527599158822</v>
+        <v>-0.3845</v>
       </c>
       <c r="C10" t="n">
-        <v>1.02540886924046</v>
+        <v>1.0254</v>
       </c>
       <c r="D10" t="n">
-        <v>0.707660993793897</v>
+        <v>0.7077</v>
       </c>
     </row>
     <row r="11">
@@ -2668,13 +2668,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.20407102590059</v>
+        <v>-5.2041</v>
       </c>
       <c r="C11" t="n">
-        <v>40.5621218446947</v>
+        <v>40.5621</v>
       </c>
       <c r="D11" t="n">
-        <v>0.897912525103192</v>
+        <v>0.8979</v>
       </c>
     </row>
     <row r="12">
@@ -2682,13 +2682,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-3.18362628089906</v>
+        <v>-3.1836</v>
       </c>
       <c r="C12" t="n">
-        <v>1.54801078167911</v>
+        <v>1.548</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0397255076041237</v>
+        <v>0.0397</v>
       </c>
     </row>
     <row r="13">
@@ -2696,13 +2696,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-5.93043878459935</v>
+        <v>-5.9304</v>
       </c>
       <c r="C13" t="n">
-        <v>2.24558990895221</v>
+        <v>2.2456</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00826795577584686</v>
+        <v>0.0083</v>
       </c>
     </row>
     <row r="14">
@@ -2710,13 +2710,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.09382529525264</v>
+        <v>-7.0938</v>
       </c>
       <c r="C14" t="n">
-        <v>2.49752648275794</v>
+        <v>2.4975</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00450654211861647</v>
+        <v>0.0045</v>
       </c>
     </row>
     <row r="15">
@@ -2724,13 +2724,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-6.9859325494539</v>
+        <v>-6.9859</v>
       </c>
       <c r="C15" t="n">
-        <v>2.50476169523193</v>
+        <v>2.5048</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00528611472540033</v>
+        <v>0.0053</v>
       </c>
     </row>
     <row r="16">
@@ -2738,13 +2738,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.32193424020449</v>
+        <v>-6.3219</v>
       </c>
       <c r="C16" t="n">
-        <v>2.3375280494704</v>
+        <v>2.3375</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00683993750772423</v>
+        <v>0.0068</v>
       </c>
     </row>
     <row r="17">
@@ -2752,13 +2752,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-5.88091794014399</v>
+        <v>-5.8809</v>
       </c>
       <c r="C17" t="n">
-        <v>2.15031821097157</v>
+        <v>2.1503</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00623981130848142</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="18">
@@ -2766,13 +2766,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.7223695222892</v>
+        <v>-5.7224</v>
       </c>
       <c r="C18" t="n">
-        <v>2.04890879544729</v>
+        <v>2.0489</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00522400332781252</v>
+        <v>0.0052</v>
       </c>
     </row>
     <row r="19">
@@ -2780,13 +2780,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-5.3076533241389</v>
+        <v>-5.3077</v>
       </c>
       <c r="C19" t="n">
-        <v>2.04641909185465</v>
+        <v>2.0464</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00949687127309367</v>
+        <v>0.0095</v>
       </c>
     </row>
     <row r="20">
@@ -2794,13 +2794,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.04379259407137</v>
+        <v>-5.0438</v>
       </c>
       <c r="C20" t="n">
-        <v>2.11539561305439</v>
+        <v>2.1154</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0171104410393367</v>
+        <v>0.0171</v>
       </c>
     </row>
     <row r="21">
@@ -2808,13 +2808,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.80431512712981</v>
+        <v>-4.8043</v>
       </c>
       <c r="C21" t="n">
-        <v>2.16726859787823</v>
+        <v>2.1673</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0266394713259504</v>
+        <v>0.0266</v>
       </c>
     </row>
     <row r="22">
@@ -2822,13 +2822,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.4976754222135</v>
+        <v>-4.4977</v>
       </c>
       <c r="C22" t="n">
-        <v>2.19374627134785</v>
+        <v>2.1937</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0403423917403379</v>
+        <v>0.0403</v>
       </c>
     </row>
     <row r="23">
@@ -2836,13 +2836,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.22020817142323</v>
+        <v>-4.2202</v>
       </c>
       <c r="C23" t="n">
-        <v>2.66924305710593</v>
+        <v>2.6692</v>
       </c>
       <c r="D23" t="n">
-        <v>0.113866482793387</v>
+        <v>0.1139</v>
       </c>
     </row>
     <row r="24">
@@ -2850,13 +2850,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.300710509927211</v>
+        <v>0.3007</v>
       </c>
       <c r="C24" t="n">
-        <v>0.16640196290246</v>
+        <v>0.1664</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0707415148980519</v>
+        <v>0.0707</v>
       </c>
     </row>
   </sheetData>
@@ -2892,13 +2892,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.22939812473685</v>
+        <v>3.2294</v>
       </c>
       <c r="C2" t="n">
-        <v>0.523033890351718</v>
+        <v>0.523</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000000000664331471450255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2906,13 +2906,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0638985704384752</v>
+        <v>-0.0639</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1525947434978</v>
+        <v>0.1526</v>
       </c>
       <c r="D3" t="n">
-        <v>0.67540114136511</v>
+        <v>0.6754</v>
       </c>
     </row>
     <row r="4">
@@ -2920,13 +2920,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.221256414812613</v>
+        <v>0.2213</v>
       </c>
       <c r="C4" t="n">
-        <v>0.132666309798706</v>
+        <v>0.1327</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0953621069566502</v>
+        <v>0.0954</v>
       </c>
     </row>
     <row r="5">
@@ -2934,13 +2934,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.137340352397815</v>
+        <v>-0.1373</v>
       </c>
       <c r="C5" t="n">
-        <v>0.244044088156356</v>
+        <v>0.244</v>
       </c>
       <c r="D5" t="n">
-        <v>0.573592457377822</v>
+        <v>0.5736</v>
       </c>
     </row>
     <row r="6">
@@ -2948,13 +2948,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0174368985549959</v>
+        <v>0.0174</v>
       </c>
       <c r="C6" t="n">
-        <v>0.247853395914897</v>
+        <v>0.2479</v>
       </c>
       <c r="D6" t="n">
-        <v>0.943913763296226</v>
+        <v>0.9439</v>
       </c>
     </row>
     <row r="7">
@@ -2962,13 +2962,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.858778922268932</v>
+        <v>-0.8588</v>
       </c>
       <c r="C7" t="n">
-        <v>0.269043644917213</v>
+        <v>0.269</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00141306592054011</v>
+        <v>0.0014</v>
       </c>
     </row>
     <row r="8">
@@ -2976,13 +2976,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.257408277671643</v>
+        <v>-0.2574</v>
       </c>
       <c r="C8" t="n">
-        <v>0.260883956197871</v>
+        <v>0.2609</v>
       </c>
       <c r="D8" t="n">
-        <v>0.323800861469911</v>
+        <v>0.3238</v>
       </c>
     </row>
     <row r="9">
@@ -2990,13 +2990,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.371325972008166</v>
+        <v>-0.3713</v>
       </c>
       <c r="C9" t="n">
-        <v>0.304837669082233</v>
+        <v>0.3048</v>
       </c>
       <c r="D9" t="n">
-        <v>0.223181976176494</v>
+        <v>0.2232</v>
       </c>
     </row>
     <row r="10">
@@ -3004,13 +3004,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0462645658198621</v>
+        <v>-0.0463</v>
       </c>
       <c r="C10" t="n">
-        <v>0.243426232462401</v>
+        <v>0.2434</v>
       </c>
       <c r="D10" t="n">
-        <v>0.849265410146681</v>
+        <v>0.8493</v>
       </c>
     </row>
     <row r="11">
@@ -3018,13 +3018,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.171009871089868</v>
+        <v>0.171</v>
       </c>
       <c r="C11" t="n">
-        <v>0.245563184507662</v>
+        <v>0.2456</v>
       </c>
       <c r="D11" t="n">
-        <v>0.486179205939902</v>
+        <v>0.4862</v>
       </c>
     </row>
     <row r="12">
@@ -3032,13 +3032,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.198676997716067</v>
+        <v>-0.1987</v>
       </c>
       <c r="C12" t="n">
-        <v>0.368507173783138</v>
+        <v>0.3685</v>
       </c>
       <c r="D12" t="n">
-        <v>0.589790182085035</v>
+        <v>0.5898</v>
       </c>
     </row>
     <row r="13">
@@ -3046,13 +3046,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.350918870736727</v>
+        <v>-0.3509</v>
       </c>
       <c r="C13" t="n">
-        <v>0.521377959944596</v>
+        <v>0.5214</v>
       </c>
       <c r="D13" t="n">
-        <v>0.500908850534131</v>
+        <v>0.5009</v>
       </c>
     </row>
     <row r="14">
@@ -3060,13 +3060,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.304066838978776</v>
+        <v>-0.3041</v>
       </c>
       <c r="C14" t="n">
-        <v>0.546306609784913</v>
+        <v>0.5463</v>
       </c>
       <c r="D14" t="n">
-        <v>0.577810035701122</v>
+        <v>0.5778</v>
       </c>
     </row>
     <row r="15">
@@ -3074,13 +3074,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.272922754796057</v>
+        <v>-0.2729</v>
       </c>
       <c r="C15" t="n">
-        <v>0.536366643946169</v>
+        <v>0.5364</v>
       </c>
       <c r="D15" t="n">
-        <v>0.610867056224194</v>
+        <v>0.6109</v>
       </c>
     </row>
     <row r="16">
@@ -3088,13 +3088,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.375491921131798</v>
+        <v>-0.3755</v>
       </c>
       <c r="C16" t="n">
-        <v>0.515627434549903</v>
+        <v>0.5156</v>
       </c>
       <c r="D16" t="n">
-        <v>0.466476894161327</v>
+        <v>0.4665</v>
       </c>
     </row>
     <row r="17">
@@ -3102,13 +3102,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.495709830448953</v>
+        <v>-0.4957</v>
       </c>
       <c r="C17" t="n">
-        <v>0.50128125221702</v>
+        <v>0.5013</v>
       </c>
       <c r="D17" t="n">
-        <v>0.322719098565502</v>
+        <v>0.3227</v>
       </c>
     </row>
     <row r="18">
@@ -3116,13 +3116,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.565269396398953</v>
+        <v>-0.5653</v>
       </c>
       <c r="C18" t="n">
-        <v>0.493227601880066</v>
+        <v>0.4932</v>
       </c>
       <c r="D18" t="n">
-        <v>0.251769512316663</v>
+        <v>0.2518</v>
       </c>
     </row>
     <row r="19">
@@ -3130,13 +3130,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.577648809669089</v>
+        <v>-0.5776</v>
       </c>
       <c r="C19" t="n">
-        <v>0.494047436676341</v>
+        <v>0.494</v>
       </c>
       <c r="D19" t="n">
-        <v>0.242316093012056</v>
+        <v>0.2423</v>
       </c>
     </row>
     <row r="20">
@@ -3144,13 +3144,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.602742422552697</v>
+        <v>-0.6027</v>
       </c>
       <c r="C20" t="n">
-        <v>0.512761223830128</v>
+        <v>0.5128</v>
       </c>
       <c r="D20" t="n">
-        <v>0.239801284299003</v>
+        <v>0.2398</v>
       </c>
     </row>
     <row r="21">
@@ -3158,13 +3158,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.479381137064827</v>
+        <v>-0.4794</v>
       </c>
       <c r="C21" t="n">
-        <v>0.523945871270541</v>
+        <v>0.5239</v>
       </c>
       <c r="D21" t="n">
-        <v>0.360221023670381</v>
+        <v>0.3602</v>
       </c>
     </row>
     <row r="22">
@@ -3172,13 +3172,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.247493274973949</v>
+        <v>-0.2475</v>
       </c>
       <c r="C22" t="n">
-        <v>0.543108616563125</v>
+        <v>0.5431</v>
       </c>
       <c r="D22" t="n">
-        <v>0.648607472078708</v>
+        <v>0.6486</v>
       </c>
     </row>
     <row r="23">
@@ -3186,13 +3186,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0137880033876967</v>
+        <v>-0.0138</v>
       </c>
       <c r="C23" t="n">
-        <v>0.695838130213171</v>
+        <v>0.6958</v>
       </c>
       <c r="D23" t="n">
-        <v>0.984190985396012</v>
+        <v>0.9842</v>
       </c>
     </row>
     <row r="24">
@@ -3200,13 +3200,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.235736282944101</v>
+        <v>-0.2357</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0734220473422019</v>
+        <v>0.0734</v>
       </c>
       <c r="D24" t="n">
-        <v>0.00132411365598545</v>
+        <v>0.0013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #34: Add the non-detects to the quantified values too (#38)
* Account for the uncertainty about non-detects everywhere
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.3991</v>
+        <v>2.0747</v>
       </c>
       <c r="C2" t="n">
-        <v>62420.4525</v>
+        <v>1.5514</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.1811</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.6217</v>
+        <v>-0.406</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4466</v>
+        <v>1.5495</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1638</v>
+        <v>0.7933</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3468</v>
+        <v>-0.3068</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3585</v>
+        <v>0.5054</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3333</v>
+        <v>0.5438</v>
       </c>
     </row>
     <row r="5">
@@ -492,111 +492,91 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>3.8322</v>
+        <v>0.9294</v>
       </c>
       <c r="C5" t="n">
-        <v>62420.4525</v>
+        <v>0.2186</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="n">
-        <v>-0.416</v>
-      </c>
+      <c r="B6"/>
       <c r="C6" t="n">
-        <v>83119.3212</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="n">
-        <v>-0.0572</v>
-      </c>
+      <c r="B7"/>
       <c r="C7" t="n">
-        <v>80488.0076</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>0.7756</v>
-      </c>
+      <c r="B8"/>
       <c r="C8" t="n">
-        <v>92489.6876</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>3.8112</v>
+        <v>0.2639</v>
       </c>
       <c r="C9" t="n">
-        <v>62420.4525</v>
+        <v>3.2132</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.9345</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="n">
-        <v>3.742</v>
-      </c>
+      <c r="B10"/>
       <c r="C10" t="n">
-        <v>62420.4525</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="n">
-        <v>-0.3179</v>
-      </c>
+      <c r="B11"/>
       <c r="C11" t="n">
-        <v>83906.3178</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.9737</v>
+        <v>-0.8483</v>
       </c>
       <c r="C12" t="n">
-        <v>1.1433</v>
+        <v>1.6522</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3944</v>
+        <v>0.6077</v>
       </c>
     </row>
     <row r="13">
@@ -604,13 +584,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.6913</v>
+        <v>-1.5957</v>
       </c>
       <c r="C13" t="n">
-        <v>1.5699</v>
+        <v>2.153</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2813</v>
+        <v>0.4586</v>
       </c>
     </row>
     <row r="14">
@@ -618,13 +598,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.5844</v>
+        <v>-1.9388</v>
       </c>
       <c r="C14" t="n">
-        <v>1.5522</v>
+        <v>2.4238</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3074</v>
+        <v>0.4238</v>
       </c>
     </row>
     <row r="15">
@@ -632,13 +612,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.0357</v>
+        <v>-1.926</v>
       </c>
       <c r="C15" t="n">
-        <v>1.3895</v>
+        <v>2.3084</v>
       </c>
       <c r="D15" t="n">
-        <v>0.456</v>
+        <v>0.4041</v>
       </c>
     </row>
     <row r="16">
@@ -646,13 +626,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.5521</v>
+        <v>-1.6234</v>
       </c>
       <c r="C16" t="n">
-        <v>1.3228</v>
+        <v>1.908</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6764</v>
+        <v>0.3949</v>
       </c>
     </row>
     <row r="17">
@@ -660,13 +640,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.1785</v>
+        <v>-1.0878</v>
       </c>
       <c r="C17" t="n">
-        <v>1.2683</v>
+        <v>1.6023</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8881</v>
+        <v>0.4972</v>
       </c>
     </row>
     <row r="18">
@@ -674,13 +654,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.1081</v>
+        <v>-0.9956</v>
       </c>
       <c r="C18" t="n">
-        <v>1.2343</v>
+        <v>1.5973</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9302</v>
+        <v>0.5331</v>
       </c>
     </row>
     <row r="19">
@@ -688,13 +668,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.4785</v>
+        <v>-1.4435</v>
       </c>
       <c r="C19" t="n">
-        <v>1.2374</v>
+        <v>1.5876</v>
       </c>
       <c r="D19" t="n">
-        <v>0.699</v>
+        <v>0.3632</v>
       </c>
     </row>
     <row r="20">
@@ -702,13 +682,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.707</v>
+        <v>-1.4987</v>
       </c>
       <c r="C20" t="n">
-        <v>1.3362</v>
+        <v>1.9321</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5967</v>
+        <v>0.4379</v>
       </c>
     </row>
     <row r="21">
@@ -716,13 +696,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.788</v>
+        <v>-1.5555</v>
       </c>
       <c r="C21" t="n">
-        <v>1.3956</v>
+        <v>3.3057</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5724</v>
+        <v>0.638</v>
       </c>
     </row>
     <row r="22">
@@ -730,13 +710,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.8375</v>
+        <v>-1.6126</v>
       </c>
       <c r="C22" t="n">
-        <v>1.7644</v>
+        <v>5.4767</v>
       </c>
       <c r="D22" t="n">
-        <v>0.635</v>
+        <v>0.7684</v>
       </c>
     </row>
     <row r="23">
@@ -744,13 +724,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.8871</v>
+        <v>-1.6697</v>
       </c>
       <c r="C23" t="n">
-        <v>2.7287</v>
+        <v>8.2019</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7451</v>
+        <v>0.8387</v>
       </c>
     </row>
     <row r="24">
@@ -758,13 +738,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.6448</v>
+        <v>-1.8861</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2082</v>
+        <v>0.4379</v>
       </c>
       <c r="D24" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -800,13 +780,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.8734</v>
+        <v>2.6353</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7008</v>
+        <v>0.3605</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0075</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -814,13 +794,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1831</v>
+        <v>0.1302</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1834</v>
+        <v>0.0924</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3182</v>
+        <v>0.1586</v>
       </c>
     </row>
     <row r="4">
@@ -828,13 +808,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.093</v>
+        <v>0.0416</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1708</v>
+        <v>0.0871</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5861</v>
+        <v>0.6332</v>
       </c>
     </row>
     <row r="5">
@@ -842,13 +822,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1322</v>
+        <v>0.2237</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3238</v>
+        <v>0.1549</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6831</v>
+        <v>0.1486</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +836,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.1211</v>
+        <v>-0.5301</v>
       </c>
       <c r="C6" t="n">
-        <v>0.356</v>
+        <v>0.2023</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0016</v>
+        <v>0.0088</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +850,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3776</v>
+        <v>0.241</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304</v>
+        <v>0.147</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2142</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="8">
@@ -884,13 +864,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8218</v>
+        <v>0.3141</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3197</v>
+        <v>0.1548</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0102</v>
+        <v>0.0424</v>
       </c>
     </row>
     <row r="9">
@@ -898,13 +878,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.3585</v>
+        <v>-0.3997</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4202</v>
+        <v>0.2154</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0012</v>
+        <v>0.0634</v>
       </c>
     </row>
     <row r="10">
@@ -912,13 +892,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.8611</v>
+        <v>-0.2778</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3245</v>
+        <v>0.1692</v>
       </c>
       <c r="D10" t="n">
-        <v>0.008</v>
+        <v>0.1006</v>
       </c>
     </row>
     <row r="11">
@@ -926,13 +906,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0387</v>
+        <v>-0.1211</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3255</v>
+        <v>0.1674</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9053</v>
+        <v>0.4696</v>
       </c>
     </row>
     <row r="12">
@@ -940,13 +920,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.565</v>
+        <v>-0.2446</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4857</v>
+        <v>0.2505</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2447</v>
+        <v>0.3288</v>
       </c>
     </row>
     <row r="13">
@@ -954,13 +934,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.0573</v>
+        <v>-0.4456</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6975</v>
+        <v>0.3584</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1296</v>
+        <v>0.2137</v>
       </c>
     </row>
     <row r="14">
@@ -968,13 +948,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.2854</v>
+        <v>-0.5311</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7403</v>
+        <v>0.3789</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0825</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="15">
@@ -982,13 +962,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.4158</v>
+        <v>-0.5908</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7287</v>
+        <v>0.3746</v>
       </c>
       <c r="D15" t="n">
-        <v>0.052</v>
+        <v>0.1148</v>
       </c>
     </row>
     <row r="16">
@@ -996,13 +976,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.3031</v>
+        <v>-0.5513</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6987</v>
+        <v>0.3624</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0622</v>
+        <v>0.1282</v>
       </c>
     </row>
     <row r="17">
@@ -1010,13 +990,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.0928</v>
+        <v>-0.4823</v>
       </c>
       <c r="C17" t="n">
-        <v>0.672</v>
+        <v>0.3485</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1039</v>
+        <v>0.1664</v>
       </c>
     </row>
     <row r="18">
@@ -1024,13 +1004,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-1.0382</v>
+        <v>-0.4713</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6577</v>
+        <v>0.3404</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1144</v>
+        <v>0.1661</v>
       </c>
     </row>
     <row r="19">
@@ -1038,13 +1018,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.1304</v>
+        <v>-0.5076</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6575</v>
+        <v>0.3404</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0856</v>
+        <v>0.1359</v>
       </c>
     </row>
     <row r="20">
@@ -1052,13 +1032,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.0517</v>
+        <v>-0.4477</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6756</v>
+        <v>0.3486</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1195</v>
+        <v>0.1991</v>
       </c>
     </row>
     <row r="21">
@@ -1066,13 +1046,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.9346</v>
+        <v>-0.3903</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6833</v>
+        <v>0.3512</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1714</v>
+        <v>0.2663</v>
       </c>
     </row>
     <row r="22">
@@ -1080,13 +1060,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.1336</v>
+        <v>-0.555</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6952</v>
+        <v>0.3548</v>
       </c>
       <c r="D22" t="n">
-        <v>0.103</v>
+        <v>0.1178</v>
       </c>
     </row>
     <row r="23">
@@ -1094,13 +1074,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.4026</v>
+        <v>-0.7725</v>
       </c>
       <c r="C23" t="n">
-        <v>0.874</v>
+        <v>0.4429</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1085</v>
+        <v>0.0811</v>
       </c>
     </row>
     <row r="24">
@@ -1108,10 +1088,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2329</v>
+        <v>-0.6532</v>
       </c>
       <c r="C24" t="n">
-        <v>0.055</v>
+        <v>0.0589</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1150,13 +1130,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.6399</v>
+        <v>0.6536</v>
       </c>
       <c r="C2" t="n">
-        <v>1.712</v>
+        <v>1.1937</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3381</v>
+        <v>0.584</v>
       </c>
     </row>
     <row r="3">
@@ -1164,13 +1144,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.1193</v>
+        <v>-0.2104</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3367</v>
+        <v>0.28</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7232</v>
+        <v>0.4523</v>
       </c>
     </row>
     <row r="4">
@@ -1178,13 +1158,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1781</v>
+        <v>-0.1423</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3641</v>
+        <v>0.2809</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6247</v>
+        <v>0.6125</v>
       </c>
     </row>
     <row r="5">
@@ -1192,13 +1172,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.2254</v>
+        <v>-4.1308</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6984</v>
+        <v>31132.3064</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0793</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1186,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1026</v>
+        <v>-0.1033</v>
       </c>
       <c r="C6" t="n">
-        <v>1.1009</v>
+        <v>0.5976</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9257</v>
+        <v>0.8627</v>
       </c>
     </row>
     <row r="7">
@@ -1220,47 +1200,55 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4227</v>
+        <v>0.3199</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7138</v>
+        <v>0.4924</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5537</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>-4.2098</v>
+      </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8"/>
+        <v>33127.983</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9"/>
+      <c r="B9" t="n">
+        <v>-3.3352</v>
+      </c>
       <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9"/>
+        <v>34711.4847</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9999</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5563</v>
+        <v>0.7964</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7364</v>
+        <v>0.4608</v>
       </c>
       <c r="D10" t="n">
-        <v>0.45</v>
+        <v>0.0839</v>
       </c>
     </row>
     <row r="11">
@@ -1268,13 +1256,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.2476</v>
+        <v>-0.3848</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0477</v>
+        <v>0.6546</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8132</v>
+        <v>0.5567</v>
       </c>
     </row>
     <row r="12">
@@ -1282,13 +1270,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0679</v>
+        <v>-0.1796</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0519</v>
+        <v>0.8383</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9485</v>
+        <v>0.8304</v>
       </c>
     </row>
     <row r="13">
@@ -1296,13 +1284,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1438</v>
+        <v>-0.3215</v>
       </c>
       <c r="C13" t="n">
-        <v>1.5938</v>
+        <v>1.2172</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9281</v>
+        <v>0.7917</v>
       </c>
     </row>
     <row r="14">
@@ -1310,13 +1298,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2498</v>
+        <v>-0.2983</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7452</v>
+        <v>1.2949</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8862</v>
+        <v>0.8178</v>
       </c>
     </row>
     <row r="15">
@@ -1324,13 +1312,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.3696</v>
+        <v>-0.0764</v>
       </c>
       <c r="C15" t="n">
-        <v>1.7215</v>
+        <v>1.2655</v>
       </c>
       <c r="D15" t="n">
-        <v>0.83</v>
+        <v>0.9519</v>
       </c>
     </row>
     <row r="16">
@@ -1338,13 +1326,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4681</v>
+        <v>0.2627</v>
       </c>
       <c r="C16" t="n">
-        <v>1.6671</v>
+        <v>1.183</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7789</v>
+        <v>0.8242</v>
       </c>
     </row>
     <row r="17">
@@ -1352,13 +1340,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5075</v>
+        <v>0.6006</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6144</v>
+        <v>1.1302</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7533</v>
+        <v>0.5952</v>
       </c>
     </row>
     <row r="18">
@@ -1366,13 +1354,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.4841</v>
+        <v>0.797</v>
       </c>
       <c r="C18" t="n">
-        <v>1.5968</v>
+        <v>1.1185</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7618</v>
+        <v>0.4761</v>
       </c>
     </row>
     <row r="19">
@@ -1380,13 +1368,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3774</v>
+        <v>0.3992</v>
       </c>
       <c r="C19" t="n">
-        <v>1.5991</v>
+        <v>1.119</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8134</v>
+        <v>0.7213</v>
       </c>
     </row>
     <row r="20">
@@ -1394,13 +1382,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2211</v>
+        <v>0.0343</v>
       </c>
       <c r="C20" t="n">
-        <v>1.6316</v>
+        <v>1.1592</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8922</v>
+        <v>0.9764</v>
       </c>
     </row>
     <row r="21">
@@ -1408,13 +1396,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0864</v>
+        <v>0.0067</v>
       </c>
       <c r="C21" t="n">
-        <v>1.6385</v>
+        <v>1.1774</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9579</v>
+        <v>0.9955</v>
       </c>
     </row>
     <row r="22">
@@ -1422,13 +1410,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0051</v>
+        <v>0.2032</v>
       </c>
       <c r="C22" t="n">
-        <v>1.6412</v>
+        <v>1.1655</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9975</v>
+        <v>0.8616</v>
       </c>
     </row>
     <row r="23">
@@ -1436,13 +1424,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0628</v>
+        <v>0.4415</v>
       </c>
       <c r="C23" t="n">
-        <v>1.9481</v>
+        <v>1.4466</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9743</v>
+        <v>0.7602</v>
       </c>
     </row>
     <row r="24">
@@ -1450,13 +1438,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5412</v>
+        <v>-0.2729</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.1272</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1480,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.8092</v>
+        <v>2.8062</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1797</v>
+        <v>0.1794</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1506,13 +1494,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0312</v>
+        <v>0.0303</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0491</v>
+        <v>0.049</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5251</v>
+        <v>0.5363</v>
       </c>
     </row>
     <row r="4">
@@ -1520,13 +1508,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0392</v>
+        <v>0.0409</v>
       </c>
       <c r="C4" t="n">
-        <v>0.046</v>
+        <v>0.0459</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3937</v>
+        <v>0.3729</v>
       </c>
     </row>
     <row r="5">
@@ -1534,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.053</v>
+        <v>-0.0508</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0903</v>
+        <v>0.09</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5567</v>
+        <v>0.5723</v>
       </c>
     </row>
     <row r="6">
@@ -1548,13 +1536,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0403</v>
+        <v>0.0425</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0824</v>
+        <v>0.0822</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6247</v>
+        <v>0.6055</v>
       </c>
     </row>
     <row r="7">
@@ -1562,13 +1550,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1376</v>
+        <v>-0.1305</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0858</v>
+        <v>0.0857</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1086</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="8">
@@ -1576,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.072</v>
+        <v>-0.0705</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0931</v>
+        <v>0.0929</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4398</v>
+        <v>0.448</v>
       </c>
     </row>
     <row r="9">
@@ -1590,13 +1578,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.1782</v>
+        <v>-0.1751</v>
       </c>
       <c r="C9" t="n">
-        <v>0.105</v>
+        <v>0.1048</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0897</v>
+        <v>0.0948</v>
       </c>
     </row>
     <row r="10">
@@ -1604,13 +1592,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0038</v>
+        <v>0.0062</v>
       </c>
       <c r="C10" t="n">
-        <v>0.081</v>
+        <v>0.0808</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9623</v>
+        <v>0.9385</v>
       </c>
     </row>
     <row r="11">
@@ -1618,13 +1606,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1164</v>
+        <v>-0.1154</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0934</v>
+        <v>0.0932</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2127</v>
+        <v>0.2155</v>
       </c>
     </row>
     <row r="12">
@@ -1632,13 +1620,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0718</v>
+        <v>-0.0717</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1283</v>
+        <v>0.1281</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5759</v>
+        <v>0.5758</v>
       </c>
     </row>
     <row r="13">
@@ -1646,13 +1634,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.1337</v>
+        <v>-0.1335</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1796</v>
+        <v>0.1793</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4568</v>
+        <v>0.4565</v>
       </c>
     </row>
     <row r="14">
@@ -1660,10 +1648,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.1503</v>
+        <v>-0.15</v>
       </c>
       <c r="C14" t="n">
-        <v>0.187</v>
+        <v>0.1866</v>
       </c>
       <c r="D14" t="n">
         <v>0.4216</v>
@@ -1674,13 +1662,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.1746</v>
+        <v>-0.1739</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1834</v>
+        <v>0.183</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3412</v>
+        <v>0.3419</v>
       </c>
     </row>
     <row r="16">
@@ -1688,13 +1676,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2207</v>
+        <v>-0.2197</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1759</v>
+        <v>0.1755</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2095</v>
+        <v>0.2106</v>
       </c>
     </row>
     <row r="17">
@@ -1702,13 +1690,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2472</v>
+        <v>-0.2461</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1708</v>
+        <v>0.1704</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1478</v>
+        <v>0.1487</v>
       </c>
     </row>
     <row r="18">
@@ -1716,13 +1704,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.2335</v>
+        <v>-0.2325</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1671</v>
+        <v>0.1667</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1622</v>
+        <v>0.1632</v>
       </c>
     </row>
     <row r="19">
@@ -1730,13 +1718,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1994</v>
+        <v>-0.1979</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1666</v>
+        <v>0.1663</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2314</v>
+        <v>0.234</v>
       </c>
     </row>
     <row r="20">
@@ -1744,13 +1732,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.1956</v>
+        <v>-0.1916</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1733</v>
+        <v>0.1729</v>
       </c>
       <c r="D20" t="n">
-        <v>0.259</v>
+        <v>0.2678</v>
       </c>
     </row>
     <row r="21">
@@ -1758,13 +1746,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.206</v>
+        <v>-0.2</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1773</v>
+        <v>0.177</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2454</v>
+        <v>0.2585</v>
       </c>
     </row>
     <row r="22">
@@ -1772,13 +1760,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.1742</v>
+        <v>-0.1708</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1819</v>
+        <v>0.1814</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3381</v>
+        <v>0.3462</v>
       </c>
     </row>
     <row r="23">
@@ -1786,13 +1774,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.1302</v>
+        <v>-0.1306</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2343</v>
+        <v>0.2335</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5785</v>
+        <v>0.5759</v>
       </c>
     </row>
     <row r="24">
@@ -1800,10 +1788,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.5092</v>
+        <v>-1.5118</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0796</v>
+        <v>0.0797</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1842,10 +1830,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0942</v>
+        <v>3.6956</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3743</v>
+        <v>0.5517</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1856,13 +1844,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0018</v>
+        <v>0.0617</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0958</v>
+        <v>0.0931</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9848</v>
+        <v>0.5074</v>
       </c>
     </row>
     <row r="4">
@@ -1870,13 +1858,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0009</v>
+        <v>-0.0038</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09</v>
+        <v>0.0992</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9922</v>
+        <v>0.9695</v>
       </c>
     </row>
     <row r="5">
@@ -1884,13 +1872,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0017</v>
+        <v>0.2732</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1872</v>
+        <v>0.4071</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9928</v>
+        <v>0.5022</v>
       </c>
     </row>
     <row r="6">
@@ -1898,13 +1886,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1799</v>
+        <v>0.3417</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1867</v>
+        <v>0.4097</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3351</v>
+        <v>0.4043</v>
       </c>
     </row>
     <row r="7">
@@ -1912,13 +1900,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3136</v>
+        <v>0.0394</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1835</v>
+        <v>0.4375</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874</v>
+        <v>0.9282</v>
       </c>
     </row>
     <row r="8">
@@ -1926,13 +1914,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.1715</v>
+        <v>-0.0368</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2042</v>
+        <v>0.508</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4009</v>
+        <v>0.9422</v>
       </c>
     </row>
     <row r="9">
@@ -1940,13 +1928,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0584</v>
+        <v>0.0543</v>
       </c>
       <c r="C9" t="n">
-        <v>0.218</v>
+        <v>0.467</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7887</v>
+        <v>0.9074</v>
       </c>
     </row>
     <row r="10">
@@ -1954,13 +1942,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.395</v>
+        <v>0.5066</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1704</v>
+        <v>0.4029</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0204</v>
+        <v>0.2086</v>
       </c>
     </row>
     <row r="11">
@@ -1968,13 +1956,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0789</v>
+        <v>0.2517</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1958</v>
+        <v>0.407</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6868</v>
+        <v>0.5363</v>
       </c>
     </row>
     <row r="12">
@@ -1982,13 +1970,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.3232</v>
+        <v>-0.3645</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2668</v>
+        <v>0.3331</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2257</v>
+        <v>0.2739</v>
       </c>
     </row>
     <row r="13">
@@ -1996,13 +1984,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.6132</v>
+        <v>-0.6841</v>
       </c>
       <c r="C13" t="n">
-        <v>0.374</v>
+        <v>0.4614</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1011</v>
+        <v>0.1382</v>
       </c>
     </row>
     <row r="14">
@@ -2010,13 +1998,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.6885</v>
+        <v>-0.7966</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3926</v>
+        <v>0.4828</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0795</v>
+        <v>0.0989</v>
       </c>
     </row>
     <row r="15">
@@ -2024,13 +2012,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5842</v>
+        <v>-0.7271</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3837</v>
+        <v>0.461</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1278</v>
+        <v>0.1147</v>
       </c>
     </row>
     <row r="16">
@@ -2038,13 +2026,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.4721</v>
+        <v>-0.5878</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3623</v>
+        <v>0.4163</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1925</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="17">
@@ -2052,13 +2040,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.3772</v>
+        <v>-0.4762</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3486</v>
+        <v>0.3919</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2793</v>
+        <v>0.2243</v>
       </c>
     </row>
     <row r="18">
@@ -2066,13 +2054,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.3411</v>
+        <v>-0.4278</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3428</v>
+        <v>0.3856</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3196</v>
+        <v>0.2673</v>
       </c>
     </row>
     <row r="19">
@@ -2080,13 +2068,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.3714</v>
+        <v>-0.4209</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3425</v>
+        <v>0.3858</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2782</v>
+        <v>0.2753</v>
       </c>
     </row>
     <row r="20">
@@ -2094,13 +2082,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4237</v>
+        <v>-0.4618</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3589</v>
+        <v>0.4089</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2378</v>
+        <v>0.2587</v>
       </c>
     </row>
     <row r="21">
@@ -2108,13 +2096,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.4652</v>
+        <v>-0.5497</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3717</v>
+        <v>0.4485</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2108</v>
+        <v>0.2203</v>
       </c>
     </row>
     <row r="22">
@@ -2122,13 +2110,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.5103</v>
+        <v>-0.6302</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3885</v>
+        <v>0.5566</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1891</v>
+        <v>0.2575</v>
       </c>
     </row>
     <row r="23">
@@ -2136,13 +2124,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.5647</v>
+        <v>-0.7091</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5063</v>
+        <v>0.8097</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2647</v>
+        <v>0.3812</v>
       </c>
     </row>
     <row r="24">
@@ -2150,10 +2138,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.8452</v>
+        <v>-1.2996</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0784</v>
+        <v>0.1361</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2192,10 +2180,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>1.2969</v>
+        <v>2.5842</v>
       </c>
       <c r="C2" t="n">
-        <v>0.302</v>
+        <v>0.4867</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2206,13 +2194,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3583</v>
+        <v>-0.2709</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0817</v>
+        <v>0.1375</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0489</v>
       </c>
     </row>
     <row r="4">
@@ -2220,13 +2208,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.4469</v>
+        <v>-0.3324</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0836</v>
+        <v>0.1702</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.0509</v>
       </c>
     </row>
     <row r="5">
@@ -2234,13 +2222,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2804</v>
+        <v>-0.3055</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1803</v>
+        <v>0.6103</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1198</v>
+        <v>0.6167</v>
       </c>
     </row>
     <row r="6">
@@ -2248,13 +2236,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8327</v>
+        <v>0.1735</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1584</v>
+        <v>0.3265</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="7">
@@ -2262,13 +2250,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2558</v>
+        <v>0.0735</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1496</v>
+        <v>0.3305</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0874</v>
+        <v>0.8241</v>
       </c>
     </row>
     <row r="8">
@@ -2276,13 +2264,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.0309</v>
+        <v>-0.4025</v>
       </c>
       <c r="C8" t="n">
-        <v>0.201</v>
+        <v>0.9186</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.6612</v>
       </c>
     </row>
     <row r="9">
@@ -2290,13 +2278,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7044</v>
+        <v>0.3616</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1795</v>
+        <v>0.3416</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0001</v>
+        <v>0.2899</v>
       </c>
     </row>
     <row r="10">
@@ -2304,13 +2292,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6026</v>
+        <v>0.2979</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1559</v>
+        <v>0.3143</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0001</v>
+        <v>0.3432</v>
       </c>
     </row>
     <row r="11">
@@ -2318,13 +2306,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0585</v>
+        <v>-0.5077</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2096</v>
+        <v>2.6812</v>
       </c>
       <c r="D11" t="n">
-        <v>0.78</v>
+        <v>0.8498</v>
       </c>
     </row>
     <row r="12">
@@ -2332,13 +2320,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0269</v>
+        <v>-0.0752</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2073</v>
+        <v>0.3127</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8967</v>
+        <v>0.8099</v>
       </c>
     </row>
     <row r="13">
@@ -2346,13 +2334,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0523</v>
+        <v>-0.1424</v>
       </c>
       <c r="C13" t="n">
-        <v>0.289</v>
+        <v>0.422</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8564</v>
+        <v>0.7358</v>
       </c>
     </row>
     <row r="14">
@@ -2360,13 +2348,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0779</v>
+        <v>-0.1519</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3011</v>
+        <v>0.4318</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7959</v>
+        <v>0.7251</v>
       </c>
     </row>
     <row r="15">
@@ -2374,13 +2362,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0992</v>
+        <v>-0.0794</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2952</v>
+        <v>0.4257</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7368</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="16">
@@ -2388,13 +2376,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0602</v>
+        <v>0.0283</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2828</v>
+        <v>0.4025</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8313</v>
+        <v>0.944</v>
       </c>
     </row>
     <row r="17">
@@ -2402,13 +2390,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0191</v>
+        <v>0.1148</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2766</v>
+        <v>0.3913</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9448</v>
+        <v>0.7693</v>
       </c>
     </row>
     <row r="18">
@@ -2416,13 +2404,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0501</v>
+        <v>0.0939</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2737</v>
+        <v>0.3884</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8548</v>
+        <v>0.809</v>
       </c>
     </row>
     <row r="19">
@@ -2430,13 +2418,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1159</v>
+        <v>-0.0478</v>
       </c>
       <c r="C19" t="n">
-        <v>0.273</v>
+        <v>0.3883</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6713</v>
+        <v>0.902</v>
       </c>
     </row>
     <row r="20">
@@ -2444,13 +2432,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.0912</v>
+        <v>-0.103</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2843</v>
+        <v>0.4176</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7483</v>
+        <v>0.8051</v>
       </c>
     </row>
     <row r="21">
@@ -2458,13 +2446,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0396</v>
+        <v>-0.0682</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2897</v>
+        <v>0.4417</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8912</v>
+        <v>0.8773</v>
       </c>
     </row>
     <row r="22">
@@ -2472,13 +2460,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1864</v>
+        <v>0.015</v>
       </c>
       <c r="C22" t="n">
-        <v>0.294</v>
+        <v>0.4708</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5261</v>
+        <v>0.9746</v>
       </c>
     </row>
     <row r="23">
@@ -2486,13 +2474,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3353</v>
+        <v>0.1064</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3785</v>
+        <v>0.6381</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3757</v>
+        <v>0.8676</v>
       </c>
     </row>
     <row r="24">
@@ -2500,10 +2488,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.7384</v>
+        <v>-1.3911</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0538</v>
+        <v>0.1179</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2542,13 +2530,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.254</v>
+        <v>3.5343</v>
       </c>
       <c r="C2" t="n">
-        <v>2.1388</v>
+        <v>800.2282</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1282</v>
+        <v>0.9965</v>
       </c>
     </row>
     <row r="3">
@@ -2556,13 +2544,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>1.5391</v>
+        <v>0.583</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5747</v>
+        <v>0.6629</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0074</v>
+        <v>0.3791</v>
       </c>
     </row>
     <row r="4">
@@ -2570,13 +2558,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7101</v>
+        <v>0.4571</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5475</v>
+        <v>0.6524</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1947</v>
+        <v>0.4835</v>
       </c>
     </row>
     <row r="5">
@@ -2584,13 +2572,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.924</v>
+        <v>0.9492</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7033</v>
+        <v>800.2225</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1889</v>
+        <v>0.9991</v>
       </c>
     </row>
     <row r="6">
@@ -2598,13 +2586,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.0113</v>
+        <v>-0.3583</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9323</v>
+        <v>800.2244</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2781</v>
+        <v>0.9996</v>
       </c>
     </row>
     <row r="7">
@@ -2612,13 +2600,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-5.2372</v>
+        <v>-1.1288</v>
       </c>
       <c r="C7" t="n">
-        <v>12.4554</v>
+        <v>32520.1465</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6741</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -2626,13 +2614,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>1.4573</v>
+        <v>0.8908</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6353</v>
+        <v>800.2225</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0218</v>
+        <v>0.9991</v>
       </c>
     </row>
     <row r="9">
@@ -2640,13 +2628,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.7227</v>
+        <v>-0.4345</v>
       </c>
       <c r="C9" t="n">
-        <v>1.3352</v>
+        <v>800.2271</v>
       </c>
       <c r="D9" t="n">
-        <v>0.197</v>
+        <v>0.9996</v>
       </c>
     </row>
     <row r="10">
@@ -2654,13 +2642,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.3845</v>
+        <v>0.235</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0254</v>
+        <v>800.2257</v>
       </c>
       <c r="D10" t="n">
-        <v>0.7077</v>
+        <v>0.9998</v>
       </c>
     </row>
     <row r="11">
@@ -2668,13 +2656,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.2041</v>
+        <v>-0.2914</v>
       </c>
       <c r="C11" t="n">
-        <v>40.5621</v>
+        <v>46626.5467</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8979</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -2682,13 +2670,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-3.1836</v>
+        <v>-1.0657</v>
       </c>
       <c r="C12" t="n">
-        <v>1.548</v>
+        <v>1.4366</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0397</v>
+        <v>0.4582</v>
       </c>
     </row>
     <row r="13">
@@ -2696,13 +2684,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-5.9304</v>
+        <v>-2.0273</v>
       </c>
       <c r="C13" t="n">
-        <v>2.2456</v>
+        <v>2.2512</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0083</v>
+        <v>0.3678</v>
       </c>
     </row>
     <row r="14">
@@ -2710,13 +2698,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-7.0938</v>
+        <v>-2.6432</v>
       </c>
       <c r="C14" t="n">
-        <v>2.4975</v>
+        <v>2.7724</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0045</v>
+        <v>0.3404</v>
       </c>
     </row>
     <row r="15">
@@ -2724,13 +2712,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-6.9859</v>
+        <v>-2.9255</v>
       </c>
       <c r="C15" t="n">
-        <v>2.5048</v>
+        <v>3.0265</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0053</v>
+        <v>0.3337</v>
       </c>
     </row>
     <row r="16">
@@ -2738,13 +2726,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-6.3219</v>
+        <v>-2.9003</v>
       </c>
       <c r="C16" t="n">
-        <v>2.3375</v>
+        <v>3.0756</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0068</v>
+        <v>0.3457</v>
       </c>
     </row>
     <row r="17">
@@ -2752,13 +2740,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-5.8809</v>
+        <v>-2.5941</v>
       </c>
       <c r="C17" t="n">
-        <v>2.1503</v>
+        <v>3.0473</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0062</v>
+        <v>0.3946</v>
       </c>
     </row>
     <row r="18">
@@ -2766,13 +2754,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-5.7224</v>
+        <v>-2.0346</v>
       </c>
       <c r="C18" t="n">
-        <v>2.0489</v>
+        <v>3.0463</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0052</v>
+        <v>0.5042</v>
       </c>
     </row>
     <row r="19">
@@ -2780,13 +2768,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-5.3077</v>
+        <v>-2.1229</v>
       </c>
       <c r="C19" t="n">
-        <v>2.0464</v>
+        <v>3.0302</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0095</v>
+        <v>0.4836</v>
       </c>
     </row>
     <row r="20">
@@ -2794,13 +2782,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-5.0438</v>
+        <v>-2.2595</v>
       </c>
       <c r="C20" t="n">
-        <v>2.1154</v>
+        <v>3.0375</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0171</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="21">
@@ -2808,13 +2796,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-4.8043</v>
+        <v>-2.0468</v>
       </c>
       <c r="C21" t="n">
-        <v>2.1673</v>
+        <v>3.0412</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0266</v>
+        <v>0.5009</v>
       </c>
     </row>
     <row r="22">
@@ -2822,13 +2810,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.4977</v>
+        <v>-2.227</v>
       </c>
       <c r="C22" t="n">
-        <v>2.1937</v>
+        <v>3.0786</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0403</v>
+        <v>0.4695</v>
       </c>
     </row>
     <row r="23">
@@ -2836,13 +2824,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.2202</v>
+        <v>-2.4611</v>
       </c>
       <c r="C23" t="n">
-        <v>2.6692</v>
+        <v>3.3358</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1139</v>
+        <v>0.4606</v>
       </c>
     </row>
     <row r="24">
@@ -2850,13 +2838,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>0.3007</v>
+        <v>-1.5916</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1664</v>
+        <v>0.3486</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0707</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2892,10 +2880,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.2294</v>
+        <v>3.27</v>
       </c>
       <c r="C2" t="n">
-        <v>0.523</v>
+        <v>0.5094</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2906,13 +2894,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0639</v>
+        <v>-0.0697</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1526</v>
+        <v>0.1491</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6754</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="4">
@@ -2920,13 +2908,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2213</v>
+        <v>0.2093</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1327</v>
+        <v>0.1289</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0954</v>
+        <v>0.1044</v>
       </c>
     </row>
     <row r="5">
@@ -2934,13 +2922,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1373</v>
+        <v>-0.1329</v>
       </c>
       <c r="C5" t="n">
-        <v>0.244</v>
+        <v>0.2392</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5736</v>
+        <v>0.5783</v>
       </c>
     </row>
     <row r="6">
@@ -2948,13 +2936,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0174</v>
+        <v>0.0402</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2479</v>
+        <v>0.2417</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9439</v>
+        <v>0.8679</v>
       </c>
     </row>
     <row r="7">
@@ -2962,13 +2950,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.8588</v>
+        <v>-0.7947</v>
       </c>
       <c r="C7" t="n">
-        <v>0.269</v>
+        <v>0.2635</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0014</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="8">
@@ -2976,13 +2964,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.2574</v>
+        <v>-0.2888</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2609</v>
+        <v>0.2533</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3238</v>
+        <v>0.2543</v>
       </c>
     </row>
     <row r="9">
@@ -2990,13 +2978,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.3713</v>
+        <v>-0.3181</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3048</v>
+        <v>0.2973</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2232</v>
+        <v>0.2846</v>
       </c>
     </row>
     <row r="10">
@@ -3004,13 +2992,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0463</v>
+        <v>-0.0263</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2434</v>
+        <v>0.2367</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8493</v>
+        <v>0.9114</v>
       </c>
     </row>
     <row r="11">
@@ -3018,13 +3006,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.171</v>
+        <v>0.1406</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2456</v>
+        <v>0.2384</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4862</v>
+        <v>0.5555</v>
       </c>
     </row>
     <row r="12">
@@ -3032,13 +3020,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1987</v>
+        <v>-0.1911</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3685</v>
+        <v>0.3592</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5898</v>
+        <v>0.5947</v>
       </c>
     </row>
     <row r="13">
@@ -3046,13 +3034,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.3509</v>
+        <v>-0.3377</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5214</v>
+        <v>0.5081</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5009</v>
+        <v>0.5063</v>
       </c>
     </row>
     <row r="14">
@@ -3060,13 +3048,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.3041</v>
+        <v>-0.292</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5463</v>
+        <v>0.5321</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5778</v>
+        <v>0.5832</v>
       </c>
     </row>
     <row r="15">
@@ -3074,13 +3062,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.2729</v>
+        <v>-0.2599</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5364</v>
+        <v>0.5222</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6109</v>
+        <v>0.6188</v>
       </c>
     </row>
     <row r="16">
@@ -3088,13 +3076,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.3755</v>
+        <v>-0.3529</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5156</v>
+        <v>0.502</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4665</v>
+        <v>0.4822</v>
       </c>
     </row>
     <row r="17">
@@ -3102,13 +3090,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4957</v>
+        <v>-0.4626</v>
       </c>
       <c r="C17" t="n">
-        <v>0.5013</v>
+        <v>0.4881</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3227</v>
+        <v>0.3433</v>
       </c>
     </row>
     <row r="18">
@@ -3116,13 +3104,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.5653</v>
+        <v>-0.5216</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4932</v>
+        <v>0.4803</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2518</v>
+        <v>0.2774</v>
       </c>
     </row>
     <row r="19">
@@ -3130,13 +3118,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.5776</v>
+        <v>-0.5281</v>
       </c>
       <c r="C19" t="n">
-        <v>0.494</v>
+        <v>0.481</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2423</v>
+        <v>0.2722</v>
       </c>
     </row>
     <row r="20">
@@ -3144,13 +3132,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.6027</v>
+        <v>-0.556</v>
       </c>
       <c r="C20" t="n">
-        <v>0.5128</v>
+        <v>0.4993</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2398</v>
+        <v>0.2655</v>
       </c>
     </row>
     <row r="21">
@@ -3158,13 +3146,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.4794</v>
+        <v>-0.4393</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5239</v>
+        <v>0.5104</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3602</v>
+        <v>0.3893</v>
       </c>
     </row>
     <row r="22">
@@ -3172,13 +3160,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.2475</v>
+        <v>-0.2169</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5431</v>
+        <v>0.5292</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6486</v>
+        <v>0.6818</v>
       </c>
     </row>
     <row r="23">
@@ -3186,13 +3174,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.0138</v>
+        <v>0.0068</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6958</v>
+        <v>0.6781</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9842</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="24">
@@ -3200,13 +3188,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.2357</v>
+        <v>-0.2728</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0734</v>
+        <v>0.073</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0013</v>
+        <v>0.0002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #41: Remove chemical categories, where not much was found (#42)
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0747</v>
+        <v>0.4061</v>
       </c>
       <c r="C2" t="n">
-        <v>1.5514</v>
+        <v>31686.6893</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1811</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.406</v>
+        <v>-0.2594</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5495</v>
+        <v>0.2233</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7933</v>
+        <v>0.2453</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3068</v>
+        <v>-0.1332</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5054</v>
+        <v>0.1692</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5438</v>
+        <v>0.4313</v>
       </c>
     </row>
     <row r="5">
@@ -492,91 +492,111 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9294</v>
+        <v>1.6647</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2186</v>
+        <v>31686.6893</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="n">
+        <v>-0.2284</v>
+      </c>
       <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6"/>
+        <v>40824.4892</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="n">
+        <v>-0.2215</v>
+      </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7"/>
+        <v>38695.3832</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>-0.1344</v>
+      </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8"/>
+        <v>42715.2131</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.2639</v>
+        <v>1.19</v>
       </c>
       <c r="C9" t="n">
-        <v>3.2132</v>
+        <v>31686.6893</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9345</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="n">
+        <v>1.5852</v>
+      </c>
       <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10"/>
+        <v>31686.6893</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="n">
+        <v>-0.0641</v>
+      </c>
       <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11"/>
+        <v>42580.1311</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.8483</v>
+        <v>-0.5778</v>
       </c>
       <c r="C12" t="n">
-        <v>1.6522</v>
+        <v>0.6369</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6077</v>
+        <v>0.3643</v>
       </c>
     </row>
     <row r="13">
@@ -584,13 +604,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.5957</v>
+        <v>-1.0665</v>
       </c>
       <c r="C13" t="n">
-        <v>2.153</v>
+        <v>0.8657</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4586</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="14">
@@ -598,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.9388</v>
+        <v>-1.2398</v>
       </c>
       <c r="C14" t="n">
-        <v>2.4238</v>
+        <v>0.8763</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4238</v>
+        <v>0.1571</v>
       </c>
     </row>
     <row r="15">
@@ -612,13 +632,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.926</v>
+        <v>-1.1869</v>
       </c>
       <c r="C15" t="n">
-        <v>2.3084</v>
+        <v>0.8084</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4041</v>
+        <v>0.1421</v>
       </c>
     </row>
     <row r="16">
@@ -626,13 +646,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.6234</v>
+        <v>-1.0491</v>
       </c>
       <c r="C16" t="n">
-        <v>1.908</v>
+        <v>0.7556</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3949</v>
+        <v>0.165</v>
       </c>
     </row>
     <row r="17">
@@ -640,13 +660,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.0878</v>
+        <v>-0.8321</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6023</v>
+        <v>0.7133</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4972</v>
+        <v>0.2434</v>
       </c>
     </row>
     <row r="18">
@@ -654,13 +674,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.9956</v>
+        <v>-0.7644</v>
       </c>
       <c r="C18" t="n">
-        <v>1.5973</v>
+        <v>0.6983</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5331</v>
+        <v>0.2736</v>
       </c>
     </row>
     <row r="19">
@@ -668,13 +688,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-1.4435</v>
+        <v>-0.9932</v>
       </c>
       <c r="C19" t="n">
-        <v>1.5876</v>
+        <v>0.6979</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3632</v>
+        <v>0.1547</v>
       </c>
     </row>
     <row r="20">
@@ -682,13 +702,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.4987</v>
+        <v>-1.1157</v>
       </c>
       <c r="C20" t="n">
-        <v>1.9321</v>
+        <v>0.7571</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4379</v>
+        <v>0.1406</v>
       </c>
     </row>
     <row r="21">
@@ -696,13 +716,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.5555</v>
+        <v>-1.1348</v>
       </c>
       <c r="C21" t="n">
-        <v>3.3057</v>
+        <v>0.8509</v>
       </c>
       <c r="D21" t="n">
-        <v>0.638</v>
+        <v>0.1823</v>
       </c>
     </row>
     <row r="22">
@@ -710,13 +730,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.6126</v>
+        <v>-1.1315</v>
       </c>
       <c r="C22" t="n">
-        <v>5.4767</v>
+        <v>1.151</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7684</v>
+        <v>0.3256</v>
       </c>
     </row>
     <row r="23">
@@ -724,13 +744,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.6697</v>
+        <v>-1.1283</v>
       </c>
       <c r="C23" t="n">
-        <v>8.2019</v>
+        <v>1.7581</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8387</v>
+        <v>0.521</v>
       </c>
     </row>
     <row r="24">
@@ -738,10 +758,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.8861</v>
+        <v>-1.225</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4379</v>
+        <v>0.2217</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2180,10 +2200,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.5842</v>
+        <v>2.315</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4867</v>
+        <v>0.2838</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2194,13 +2214,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2709</v>
+        <v>-0.2653</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1375</v>
+        <v>0.0817</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0489</v>
+        <v>0.0012</v>
       </c>
     </row>
     <row r="4">
@@ -2208,13 +2228,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3324</v>
+        <v>-0.3223</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1702</v>
+        <v>0.0884</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0509</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="5">
@@ -2222,13 +2242,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3055</v>
+        <v>-0.3065</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6103</v>
+        <v>0.2529</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6167</v>
+        <v>0.2254</v>
       </c>
     </row>
     <row r="6">
@@ -2236,13 +2256,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1735</v>
+        <v>0.2063</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3265</v>
+        <v>0.1625</v>
       </c>
       <c r="D6" t="n">
-        <v>0.595</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="7">
@@ -2250,13 +2270,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0735</v>
+        <v>0.061</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3305</v>
+        <v>0.1622</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8241</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="8">
@@ -2264,13 +2284,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.4025</v>
+        <v>-0.4051</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9186</v>
+        <v>0.342</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6612</v>
+        <v>0.2362</v>
       </c>
     </row>
     <row r="9">
@@ -2278,13 +2298,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3616</v>
+        <v>0.3051</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3416</v>
+        <v>0.1764</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2899</v>
+        <v>0.0836</v>
       </c>
     </row>
     <row r="10">
@@ -2292,13 +2312,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2979</v>
+        <v>0.2152</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3143</v>
+        <v>0.1585</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3432</v>
+        <v>0.1745</v>
       </c>
     </row>
     <row r="11">
@@ -2306,13 +2326,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.5077</v>
+        <v>-0.4734</v>
       </c>
       <c r="C11" t="n">
-        <v>2.6812</v>
+        <v>0.5145</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8498</v>
+        <v>0.3575</v>
       </c>
     </row>
     <row r="12">
@@ -2320,13 +2340,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0752</v>
+        <v>-0.0528</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3127</v>
+        <v>0.1969</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8099</v>
+        <v>0.7886</v>
       </c>
     </row>
     <row r="13">
@@ -2334,13 +2354,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.1424</v>
+        <v>-0.0986</v>
       </c>
       <c r="C13" t="n">
-        <v>0.422</v>
+        <v>0.2659</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7358</v>
+        <v>0.7109</v>
       </c>
     </row>
     <row r="14">
@@ -2348,13 +2368,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.1519</v>
+        <v>-0.1032</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4318</v>
+        <v>0.2718</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7251</v>
+        <v>0.7043</v>
       </c>
     </row>
     <row r="15">
@@ -2362,13 +2382,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0794</v>
+        <v>-0.0517</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4257</v>
+        <v>0.2678</v>
       </c>
       <c r="D15" t="n">
-        <v>0.852</v>
+        <v>0.847</v>
       </c>
     </row>
     <row r="16">
@@ -2376,13 +2396,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0283</v>
+        <v>0.0129</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4025</v>
+        <v>0.2559</v>
       </c>
       <c r="D16" t="n">
-        <v>0.944</v>
+        <v>0.9599</v>
       </c>
     </row>
     <row r="17">
@@ -2390,13 +2410,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1148</v>
+        <v>0.0513</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3913</v>
+        <v>0.2506</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7693</v>
+        <v>0.8379</v>
       </c>
     </row>
     <row r="18">
@@ -2404,13 +2424,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0939</v>
+        <v>0.0151</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3884</v>
+        <v>0.2487</v>
       </c>
       <c r="D18" t="n">
-        <v>0.809</v>
+        <v>0.9516</v>
       </c>
     </row>
     <row r="19">
@@ -2418,13 +2438,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.0478</v>
+        <v>-0.0803</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3883</v>
+        <v>0.2484</v>
       </c>
       <c r="D19" t="n">
-        <v>0.902</v>
+        <v>0.7466</v>
       </c>
     </row>
     <row r="20">
@@ -2432,13 +2452,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.103</v>
+        <v>-0.1165</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4176</v>
+        <v>0.2637</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8051</v>
+        <v>0.6586</v>
       </c>
     </row>
     <row r="21">
@@ -2446,13 +2466,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.0682</v>
+        <v>-0.0855</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4417</v>
+        <v>0.2735</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8773</v>
+        <v>0.7547</v>
       </c>
     </row>
     <row r="22">
@@ -2460,13 +2480,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.015</v>
+        <v>-0.0216</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4708</v>
+        <v>0.2851</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9746</v>
+        <v>0.9396</v>
       </c>
     </row>
     <row r="23">
@@ -2474,13 +2494,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1064</v>
+        <v>0.048</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6381</v>
+        <v>0.3831</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8676</v>
+        <v>0.9003</v>
       </c>
     </row>
     <row r="24">
@@ -2488,10 +2508,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.3911</v>
+        <v>-1.3513</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1179</v>
+        <v>0.0814</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2530,13 +2550,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.5343</v>
+        <v>3.3025</v>
       </c>
       <c r="C2" t="n">
-        <v>800.2282</v>
+        <v>1.2803</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9965</v>
+        <v>0.0099</v>
       </c>
     </row>
     <row r="3">
@@ -2544,13 +2564,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.583</v>
+        <v>0.5262</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6629</v>
+        <v>0.243</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3791</v>
+        <v>0.0303</v>
       </c>
     </row>
     <row r="4">
@@ -2558,13 +2578,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4571</v>
+        <v>0.3542</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6524</v>
+        <v>0.233</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4835</v>
+        <v>0.1285</v>
       </c>
     </row>
     <row r="5">
@@ -2572,13 +2592,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9492</v>
+        <v>0.607</v>
       </c>
       <c r="C5" t="n">
-        <v>800.2225</v>
+        <v>0.5845</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9991</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="6">
@@ -2586,13 +2606,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3583</v>
+        <v>-0.2895</v>
       </c>
       <c r="C6" t="n">
-        <v>800.2244</v>
+        <v>0.7234</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9996</v>
+        <v>0.6891</v>
       </c>
     </row>
     <row r="7">
@@ -2600,13 +2620,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.1288</v>
+        <v>-2.0377</v>
       </c>
       <c r="C7" t="n">
-        <v>32520.1465</v>
+        <v>2189.6613</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0.9993</v>
       </c>
     </row>
     <row r="8">
@@ -2614,13 +2634,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8908</v>
+        <v>0.6646</v>
       </c>
       <c r="C8" t="n">
-        <v>800.2225</v>
+        <v>0.5659</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9991</v>
+        <v>0.2402</v>
       </c>
     </row>
     <row r="9">
@@ -2628,13 +2648,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.4345</v>
+        <v>-0.4127</v>
       </c>
       <c r="C9" t="n">
-        <v>800.2271</v>
+        <v>0.7752</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9996</v>
+        <v>0.5945</v>
       </c>
     </row>
     <row r="10">
@@ -2642,13 +2662,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.235</v>
+        <v>0.1365</v>
       </c>
       <c r="C10" t="n">
-        <v>800.2257</v>
+        <v>0.6849</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9998</v>
+        <v>0.842</v>
       </c>
     </row>
     <row r="11">
@@ -2656,13 +2676,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.2914</v>
+        <v>-1.4508</v>
       </c>
       <c r="C11" t="n">
-        <v>46626.5467</v>
+        <v>2981.6323</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0.9996</v>
       </c>
     </row>
     <row r="12">
@@ -2670,13 +2690,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.0657</v>
+        <v>-1.2623</v>
       </c>
       <c r="C12" t="n">
-        <v>1.4366</v>
+        <v>0.9743</v>
       </c>
       <c r="D12" t="n">
-        <v>0.4582</v>
+        <v>0.1951</v>
       </c>
     </row>
     <row r="13">
@@ -2684,13 +2704,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.0273</v>
+        <v>-2.3668</v>
       </c>
       <c r="C13" t="n">
-        <v>2.2512</v>
+        <v>1.4649</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3678</v>
+        <v>0.1062</v>
       </c>
     </row>
     <row r="14">
@@ -2698,13 +2718,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.6432</v>
+        <v>-2.9957</v>
       </c>
       <c r="C14" t="n">
-        <v>2.7724</v>
+        <v>1.7185</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3404</v>
+        <v>0.0813</v>
       </c>
     </row>
     <row r="15">
@@ -2712,13 +2732,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-2.9255</v>
+        <v>-3.2126</v>
       </c>
       <c r="C15" t="n">
-        <v>3.0265</v>
+        <v>1.744</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3337</v>
+        <v>0.0655</v>
       </c>
     </row>
     <row r="16">
@@ -2726,13 +2746,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-2.9003</v>
+        <v>-3.1079</v>
       </c>
       <c r="C16" t="n">
-        <v>3.0756</v>
+        <v>1.5638</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3457</v>
+        <v>0.0469</v>
       </c>
     </row>
     <row r="17">
@@ -2740,13 +2760,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.5941</v>
+        <v>-2.7713</v>
       </c>
       <c r="C17" t="n">
-        <v>3.0473</v>
+        <v>1.3013</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3946</v>
+        <v>0.0332</v>
       </c>
     </row>
     <row r="18">
@@ -2754,13 +2774,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.0346</v>
+        <v>-2.2698</v>
       </c>
       <c r="C18" t="n">
-        <v>3.0463</v>
+        <v>1.1417</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5042</v>
+        <v>0.0468</v>
       </c>
     </row>
     <row r="19">
@@ -2768,13 +2788,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-2.1229</v>
+        <v>-2.1592</v>
       </c>
       <c r="C19" t="n">
-        <v>3.0302</v>
+        <v>1.1317</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4836</v>
+        <v>0.0564</v>
       </c>
     </row>
     <row r="20">
@@ -2782,13 +2802,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-2.2595</v>
+        <v>-2.2244</v>
       </c>
       <c r="C20" t="n">
-        <v>3.0375</v>
+        <v>1.1697</v>
       </c>
       <c r="D20" t="n">
-        <v>0.457</v>
+        <v>0.0572</v>
       </c>
     </row>
     <row r="21">
@@ -2796,13 +2816,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-2.0468</v>
+        <v>-2.0845</v>
       </c>
       <c r="C21" t="n">
-        <v>3.0412</v>
+        <v>1.187</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5009</v>
+        <v>0.0791</v>
       </c>
     </row>
     <row r="22">
@@ -2810,13 +2830,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-2.227</v>
+        <v>-2.3118</v>
       </c>
       <c r="C22" t="n">
-        <v>3.0786</v>
+        <v>1.2185</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4695</v>
+        <v>0.0578</v>
       </c>
     </row>
     <row r="23">
@@ -2824,13 +2844,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-2.4611</v>
+        <v>-2.6108</v>
       </c>
       <c r="C23" t="n">
-        <v>3.3358</v>
+        <v>1.5281</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4606</v>
+        <v>0.0875</v>
       </c>
     </row>
     <row r="24">
@@ -2838,10 +2858,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.5916</v>
+        <v>-0.9765</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3486</v>
+        <v>0.2063</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Issue #40: Incorporate the feedback on graphics (#47)
* Change the label 'Calf' to 'Fawn'

* Fix the spelling of 'Eifel'

* Translate the month labels to English

* Rearrange the parks alphabetically

* Change colors of the parks

* Adjust the color gradient for the categorical coefficients

* Make the y-axis in the seasonality plot start from 0
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -42,13 +42,13 @@
     <t xml:space="preserve">AgeAdult</t>
   </si>
   <si>
+    <t xml:space="preserve">ParkEifel</t>
+  </si>
+  <si>
     <t xml:space="preserve">ParkHainich</t>
   </si>
   <si>
     <t xml:space="preserve">ParkHunsrueck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkJasmund</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">ParkKellerwald</t>
   </si>
   <si>
-    <t xml:space="preserve">ParkEiffel</t>
+    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkVorpomm</t>
@@ -450,10 +450,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4061</v>
+        <v>0.2467</v>
       </c>
       <c r="C2" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -492,10 +492,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.6647</v>
+        <v>1.7447</v>
       </c>
       <c r="C5" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -506,10 +506,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2284</v>
+        <v>1.8242</v>
       </c>
       <c r="C6" t="n">
-        <v>40824.4892</v>
+        <v>85816.1197</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -519,39 +519,31 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="n">
-        <v>-0.2215</v>
-      </c>
+      <c r="B7"/>
       <c r="C7" t="n">
-        <v>38695.3832</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n">
-        <v>-0.1344</v>
-      </c>
+      <c r="B8"/>
       <c r="C8" t="n">
-        <v>42715.2131</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>1.19</v>
+        <v>1.3494</v>
       </c>
       <c r="C9" t="n">
-        <v>31686.6893</v>
+        <v>85816.1197</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -561,29 +553,21 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="n">
-        <v>1.5852</v>
-      </c>
+      <c r="B10"/>
       <c r="C10" t="n">
-        <v>31686.6893</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="n">
-        <v>-0.0641</v>
-      </c>
+      <c r="B11"/>
       <c r="C11" t="n">
-        <v>42580.1311</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -842,13 +826,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2237</v>
+        <v>-0.2778</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1549</v>
+        <v>0.1692</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1486</v>
+        <v>0.1006</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +840,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.5301</v>
+        <v>0.2237</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2023</v>
+        <v>0.1549</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0088</v>
+        <v>0.1486</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +854,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.241</v>
+        <v>-0.5301</v>
       </c>
       <c r="C7" t="n">
-        <v>0.147</v>
+        <v>0.2023</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1011</v>
+        <v>0.0088</v>
       </c>
     </row>
     <row r="8">
@@ -912,13 +896,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2778</v>
+        <v>0.241</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1692</v>
+        <v>0.147</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1006</v>
+        <v>0.1011</v>
       </c>
     </row>
     <row r="11">
@@ -1192,13 +1176,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.1308</v>
+        <v>0.7964</v>
       </c>
       <c r="C5" t="n">
-        <v>31132.3064</v>
+        <v>0.4608</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9999</v>
+        <v>0.0839</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1190,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.1033</v>
+        <v>-4.1308</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5976</v>
+        <v>31132.3064</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8627</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="7">
@@ -1220,13 +1204,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3199</v>
+        <v>-0.1033</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4924</v>
+        <v>0.5976</v>
       </c>
       <c r="D7" t="n">
-        <v>0.516</v>
+        <v>0.8627</v>
       </c>
     </row>
     <row r="8">
@@ -1262,13 +1246,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7964</v>
+        <v>0.3199</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4608</v>
+        <v>0.4924</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0839</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="11">
@@ -1542,13 +1526,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0508</v>
+        <v>0.0062</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09</v>
+        <v>0.0808</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5723</v>
+        <v>0.9385</v>
       </c>
     </row>
     <row r="6">
@@ -1556,13 +1540,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0425</v>
+        <v>-0.0508</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0822</v>
+        <v>0.09</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6055</v>
+        <v>0.5723</v>
       </c>
     </row>
     <row r="7">
@@ -1570,13 +1554,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1305</v>
+        <v>0.0425</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0857</v>
+        <v>0.0822</v>
       </c>
       <c r="D7" t="n">
-        <v>0.128</v>
+        <v>0.6055</v>
       </c>
     </row>
     <row r="8">
@@ -1612,13 +1596,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0062</v>
+        <v>-0.1305</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0808</v>
+        <v>0.0857</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9385</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="11">
@@ -1892,13 +1876,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2732</v>
+        <v>0.5066</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4071</v>
+        <v>0.4029</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5022</v>
+        <v>0.2086</v>
       </c>
     </row>
     <row r="6">
@@ -1906,13 +1890,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3417</v>
+        <v>0.2732</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4097</v>
+        <v>0.4071</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4043</v>
+        <v>0.5022</v>
       </c>
     </row>
     <row r="7">
@@ -1920,13 +1904,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0394</v>
+        <v>0.3417</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4375</v>
+        <v>0.4097</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9282</v>
+        <v>0.4043</v>
       </c>
     </row>
     <row r="8">
@@ -1962,13 +1946,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5066</v>
+        <v>0.0394</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4029</v>
+        <v>0.4375</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2086</v>
+        <v>0.9282</v>
       </c>
     </row>
     <row r="11">
@@ -2242,13 +2226,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.3065</v>
+        <v>0.2152</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2529</v>
+        <v>0.1585</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2254</v>
+        <v>0.1745</v>
       </c>
     </row>
     <row r="6">
@@ -2256,13 +2240,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2063</v>
+        <v>-0.3065</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1625</v>
+        <v>0.2529</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2041</v>
+        <v>0.2254</v>
       </c>
     </row>
     <row r="7">
@@ -2270,13 +2254,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.061</v>
+        <v>0.2063</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1622</v>
+        <v>0.1625</v>
       </c>
       <c r="D7" t="n">
-        <v>0.707</v>
+        <v>0.2041</v>
       </c>
     </row>
     <row r="8">
@@ -2312,13 +2296,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2152</v>
+        <v>0.061</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1585</v>
+        <v>0.1622</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1745</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="11">
@@ -2592,13 +2576,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.607</v>
+        <v>0.1365</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5845</v>
+        <v>0.6849</v>
       </c>
       <c r="D5" t="n">
-        <v>0.299</v>
+        <v>0.842</v>
       </c>
     </row>
     <row r="6">
@@ -2606,13 +2590,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.2895</v>
+        <v>0.607</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7234</v>
+        <v>0.5845</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6891</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="7">
@@ -2620,13 +2604,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-2.0377</v>
+        <v>-0.2895</v>
       </c>
       <c r="C7" t="n">
-        <v>2189.6613</v>
+        <v>0.7234</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9993</v>
+        <v>0.6891</v>
       </c>
     </row>
     <row r="8">
@@ -2662,13 +2646,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1365</v>
+        <v>-2.0377</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6849</v>
+        <v>2189.6613</v>
       </c>
       <c r="D10" t="n">
-        <v>0.842</v>
+        <v>0.9993</v>
       </c>
     </row>
     <row r="11">
@@ -2942,13 +2926,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1329</v>
+        <v>-0.0263</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2392</v>
+        <v>0.2367</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5783</v>
+        <v>0.9114</v>
       </c>
     </row>
     <row r="6">
@@ -2956,13 +2940,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0402</v>
+        <v>-0.1329</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2417</v>
+        <v>0.2392</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8679</v>
+        <v>0.5783</v>
       </c>
     </row>
     <row r="7">
@@ -2970,13 +2954,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.7947</v>
+        <v>0.0402</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2635</v>
+        <v>0.2417</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0026</v>
+        <v>0.8679</v>
       </c>
     </row>
     <row r="8">
@@ -3012,13 +2996,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0263</v>
+        <v>-0.7947</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2367</v>
+        <v>0.2635</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9114</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Apply the graphical updates
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -42,13 +42,13 @@
     <t xml:space="preserve">AgeAdult</t>
   </si>
   <si>
+    <t xml:space="preserve">ParkEifel</t>
+  </si>
+  <si>
     <t xml:space="preserve">ParkHainich</t>
   </si>
   <si>
     <t xml:space="preserve">ParkHunsrueck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkJasmund</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">ParkKellerwald</t>
   </si>
   <si>
-    <t xml:space="preserve">ParkEiffel</t>
+    <t xml:space="preserve">ParkSaechs_Schw</t>
   </si>
   <si>
     <t xml:space="preserve">ParkVorpomm</t>
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2012</v>
+        <v>0.1788</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3619</v>
+        <v>0.368</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5782</v>
+        <v>0.6271</v>
       </c>
     </row>
     <row r="6">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-4.5034</v>
+        <v>0.2012</v>
       </c>
       <c r="C6" t="n">
-        <v>76547.695</v>
+        <v>0.3619</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.5782</v>
       </c>
     </row>
     <row r="7">
@@ -520,13 +520,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-4.4454</v>
+        <v>-4.5034</v>
       </c>
       <c r="C7" t="n">
-        <v>67350.3807</v>
+        <v>76547.695</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -562,13 +562,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1788</v>
+        <v>-4.4454</v>
       </c>
       <c r="C10" t="n">
-        <v>0.368</v>
+        <v>67350.3807</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6271</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="11">
@@ -842,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2428</v>
+        <v>-0.304</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1882</v>
+        <v>0.1885</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1971</v>
+        <v>0.1069</v>
       </c>
     </row>
     <row r="6">
@@ -856,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.4781</v>
+        <v>0.2428</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2056</v>
+        <v>0.1882</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0201</v>
+        <v>0.1971</v>
       </c>
     </row>
     <row r="7">
@@ -870,13 +870,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4481</v>
+        <v>-0.4781</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1745</v>
+        <v>0.2056</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0102</v>
+        <v>0.0201</v>
       </c>
     </row>
     <row r="8">
@@ -912,13 +912,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.304</v>
+        <v>0.4481</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1885</v>
+        <v>0.1745</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1069</v>
+        <v>0.0102</v>
       </c>
     </row>
     <row r="11">
@@ -1192,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2097</v>
+        <v>0.5337</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1206</v>
+        <v>0.1185</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0822</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1206,13 +1206,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3294</v>
+        <v>-0.2097</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1316</v>
+        <v>0.1206</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0123</v>
+        <v>0.0822</v>
       </c>
     </row>
     <row r="7">
@@ -1220,13 +1220,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1474</v>
+        <v>0.3294</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1129</v>
+        <v>0.1316</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1916</v>
+        <v>0.0123</v>
       </c>
     </row>
     <row r="8">
@@ -1262,13 +1262,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.5337</v>
+        <v>0.1474</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1185</v>
+        <v>0.1129</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.1916</v>
       </c>
     </row>
     <row r="11">
@@ -1542,13 +1542,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1128</v>
+        <v>-0.0065</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0824</v>
+        <v>0.0706</v>
       </c>
       <c r="D5" t="n">
-        <v>0.171</v>
+        <v>0.9264</v>
       </c>
     </row>
     <row r="6">
@@ -1556,13 +1556,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0491</v>
+        <v>-0.1128</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0715</v>
+        <v>0.0824</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4922</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="7">
@@ -1570,13 +1570,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1129</v>
+        <v>0.0491</v>
       </c>
       <c r="C7" t="n">
-        <v>0.071</v>
+        <v>0.0715</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1119</v>
+        <v>0.4922</v>
       </c>
     </row>
     <row r="8">
@@ -1612,13 +1612,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0065</v>
+        <v>-0.1129</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0706</v>
+        <v>0.071</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9264</v>
+        <v>0.1119</v>
       </c>
     </row>
     <row r="11">
@@ -1892,13 +1892,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0157</v>
+        <v>0.2896</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1312</v>
+        <v>0.1193</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9046</v>
+        <v>0.0153</v>
       </c>
     </row>
     <row r="6">
@@ -1906,13 +1906,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1359</v>
+        <v>0.0157</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1298</v>
+        <v>0.1312</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2948</v>
+        <v>0.9046</v>
       </c>
     </row>
     <row r="7">
@@ -1920,13 +1920,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1722</v>
+        <v>0.1359</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1279</v>
+        <v>0.1298</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1783</v>
+        <v>0.2948</v>
       </c>
     </row>
     <row r="8">
@@ -1962,13 +1962,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2896</v>
+        <v>-0.1722</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1193</v>
+        <v>0.1279</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0153</v>
+        <v>0.1783</v>
       </c>
     </row>
     <row r="11">
@@ -2242,13 +2242,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.1849</v>
+        <v>0.3727</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1226</v>
+        <v>0.1055</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1315</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="6">
@@ -2256,13 +2256,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4938</v>
+        <v>-0.1849</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1076</v>
+        <v>0.1226</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.1315</v>
       </c>
     </row>
     <row r="7">
@@ -2270,13 +2270,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1287</v>
+        <v>0.4938</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1034</v>
+        <v>0.1076</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2312,13 +2312,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3727</v>
+        <v>0.1287</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1055</v>
+        <v>0.1034</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0004</v>
+        <v>0.2132</v>
       </c>
     </row>
     <row r="11">
@@ -2592,13 +2592,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1766</v>
+        <v>-0.1254</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2343</v>
+        <v>0.259</v>
       </c>
       <c r="D5" t="n">
-        <v>0.451</v>
+        <v>0.6284</v>
       </c>
     </row>
     <row r="6">
@@ -2606,13 +2606,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3861</v>
+        <v>0.1766</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2777</v>
+        <v>0.2343</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1644</v>
+        <v>0.451</v>
       </c>
     </row>
     <row r="7">
@@ -2620,13 +2620,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.6188</v>
+        <v>-0.3861</v>
       </c>
       <c r="C7" t="n">
-        <v>0.266</v>
+        <v>0.2777</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02</v>
+        <v>0.1644</v>
       </c>
     </row>
     <row r="8">
@@ -2662,13 +2662,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.1254</v>
+        <v>-0.6188</v>
       </c>
       <c r="C10" t="n">
-        <v>0.259</v>
+        <v>0.266</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6284</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
@@ -2942,13 +2942,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0679</v>
+        <v>0.0157</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1331</v>
+        <v>0.1299</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6098</v>
+        <v>0.9036</v>
       </c>
     </row>
     <row r="6">
@@ -2956,13 +2956,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0203</v>
+        <v>-0.0679</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1366</v>
+        <v>0.1331</v>
       </c>
       <c r="D6" t="n">
-        <v>0.882</v>
+        <v>0.6098</v>
       </c>
     </row>
     <row r="7">
@@ -2970,13 +2970,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3214</v>
+        <v>0.0203</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1248</v>
+        <v>0.1366</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01</v>
+        <v>0.882</v>
       </c>
     </row>
     <row r="8">
@@ -3012,13 +3012,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0157</v>
+        <v>-0.3214</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1299</v>
+        <v>0.1248</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9036</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Fit the Weibull distribution
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -8,12 +8,11 @@
   <sheets>
     <sheet name="API" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Anthropogenic pollution" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Industrial chemical" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="PAH" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PCP" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="POP" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Pesticide" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Plasticizer" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="PAH" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PCP" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="POP" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Pesticide" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Plasticizer" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -450,13 +449,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2467</v>
+        <v>1.0719</v>
       </c>
       <c r="C2" t="n">
-        <v>85816.1197</v>
+        <v>6147.9054</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="3">
@@ -464,13 +463,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2594</v>
+        <v>-0.3268</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2233</v>
+        <v>0.2382</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2453</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1332</v>
+        <v>-0.1697</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1692</v>
+        <v>0.1871</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4313</v>
+        <v>0.3644</v>
       </c>
     </row>
     <row r="5">
@@ -492,13 +491,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>1.7447</v>
+        <v>1.0187</v>
       </c>
       <c r="C5" t="n">
-        <v>85816.1197</v>
+        <v>6147.9054</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="6">
@@ -506,81 +505,97 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>1.8242</v>
+        <v>1.1801</v>
       </c>
       <c r="C6" t="n">
-        <v>85816.1197</v>
+        <v>6147.9054</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0.9998</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="n">
+        <v>-0.1754</v>
+      </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7"/>
+        <v>6160.976</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="n">
+        <v>-0.1637</v>
+      </c>
       <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8"/>
+        <v>23587.6925</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>1.3494</v>
+        <v>0.5556</v>
       </c>
       <c r="C9" t="n">
-        <v>85816.1197</v>
+        <v>6147.9054</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0.9999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="n">
+        <v>-0.22</v>
+      </c>
       <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10"/>
+        <v>6177.3998</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="n">
+        <v>-0.0765</v>
+      </c>
       <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11"/>
+        <v>16756.1251</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.5778</v>
+        <v>-0.6316</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6369</v>
+        <v>0.654</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3643</v>
+        <v>0.3341</v>
       </c>
     </row>
     <row r="13">
@@ -588,13 +603,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.0665</v>
+        <v>-1.1726</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8657</v>
+        <v>0.8919</v>
       </c>
       <c r="D13" t="n">
-        <v>0.218</v>
+        <v>0.1886</v>
       </c>
     </row>
     <row r="14">
@@ -602,13 +617,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.2398</v>
+        <v>-1.3815</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8763</v>
+        <v>0.9042</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1571</v>
+        <v>0.1265</v>
       </c>
     </row>
     <row r="15">
@@ -616,13 +631,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.1869</v>
+        <v>-1.3359</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8084</v>
+        <v>0.8403</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1421</v>
+        <v>0.1119</v>
       </c>
     </row>
     <row r="16">
@@ -630,13 +645,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.0491</v>
+        <v>-1.1726</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7556</v>
+        <v>0.7894</v>
       </c>
       <c r="D16" t="n">
-        <v>0.165</v>
+        <v>0.1374</v>
       </c>
     </row>
     <row r="17">
@@ -644,13 +659,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.8321</v>
+        <v>-0.91</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7133</v>
+        <v>0.7453</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2434</v>
+        <v>0.2221</v>
       </c>
     </row>
     <row r="18">
@@ -658,13 +673,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.7644</v>
+        <v>-0.8464</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6983</v>
+        <v>0.7287</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2736</v>
+        <v>0.2454</v>
       </c>
     </row>
     <row r="19">
@@ -672,13 +687,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.9932</v>
+        <v>-1.1697</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6979</v>
+        <v>0.7287</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1547</v>
+        <v>0.1085</v>
       </c>
     </row>
     <row r="20">
@@ -686,13 +701,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-1.1157</v>
+        <v>-1.3015</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7571</v>
+        <v>0.7867</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1406</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="21">
@@ -700,13 +715,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-1.1348</v>
+        <v>-1.2545</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8509</v>
+        <v>0.8756</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1823</v>
+        <v>0.1519</v>
       </c>
     </row>
     <row r="22">
@@ -714,13 +729,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-1.1315</v>
+        <v>-1.1691</v>
       </c>
       <c r="C22" t="n">
-        <v>1.151</v>
+        <v>1.171</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3256</v>
+        <v>0.3181</v>
       </c>
     </row>
     <row r="23">
@@ -728,13 +743,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-1.1283</v>
+        <v>-1.0838</v>
       </c>
       <c r="C23" t="n">
-        <v>1.7581</v>
+        <v>1.7815</v>
       </c>
       <c r="D23" t="n">
-        <v>0.521</v>
+        <v>0.543</v>
       </c>
     </row>
     <row r="24">
@@ -742,13 +757,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.225</v>
+        <v>-0.7614</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2217</v>
+        <v>0.2437</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +799,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.6353</v>
+        <v>3.0173</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3605</v>
+        <v>0.3728</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -798,13 +813,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1302</v>
+        <v>0.19</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0924</v>
+        <v>0.1014</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1586</v>
+        <v>0.061</v>
       </c>
     </row>
     <row r="4">
@@ -812,13 +827,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0416</v>
+        <v>0.0258</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0871</v>
+        <v>0.0949</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6332</v>
+        <v>0.786</v>
       </c>
     </row>
     <row r="5">
@@ -826,13 +841,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2778</v>
+        <v>-0.3186</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1692</v>
+        <v>0.1797</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1006</v>
+        <v>0.0762</v>
       </c>
     </row>
     <row r="6">
@@ -840,13 +855,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2237</v>
+        <v>0.4603</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1549</v>
+        <v>0.164</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1486</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="7">
@@ -854,13 +869,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.5301</v>
+        <v>-0.6218</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2023</v>
+        <v>0.2105</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0088</v>
+        <v>0.0031</v>
       </c>
     </row>
     <row r="8">
@@ -868,13 +883,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3141</v>
+        <v>0.3614</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1548</v>
+        <v>0.1707</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0424</v>
+        <v>0.0343</v>
       </c>
     </row>
     <row r="9">
@@ -882,13 +897,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.3997</v>
+        <v>-0.4868</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2154</v>
+        <v>0.2259</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0634</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="10">
@@ -896,13 +911,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.241</v>
+        <v>0.3827</v>
       </c>
       <c r="C10" t="n">
-        <v>0.147</v>
+        <v>0.1594</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1011</v>
+        <v>0.0164</v>
       </c>
     </row>
     <row r="11">
@@ -910,13 +925,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1211</v>
+        <v>-0.1948</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1674</v>
+        <v>0.1808</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4696</v>
+        <v>0.2812</v>
       </c>
     </row>
     <row r="12">
@@ -924,13 +939,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.2446</v>
+        <v>-0.3746</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2505</v>
+        <v>0.2636</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3288</v>
+        <v>0.1553</v>
       </c>
     </row>
     <row r="13">
@@ -938,13 +953,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.4456</v>
+        <v>-0.6891</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3584</v>
+        <v>0.3711</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2137</v>
+        <v>0.0633</v>
       </c>
     </row>
     <row r="14">
@@ -952,13 +967,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.5311</v>
+        <v>-0.837</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3789</v>
+        <v>0.3889</v>
       </c>
       <c r="D14" t="n">
-        <v>0.161</v>
+        <v>0.0314</v>
       </c>
     </row>
     <row r="15">
@@ -966,13 +981,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5908</v>
+        <v>-0.9047</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3746</v>
+        <v>0.388</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1148</v>
+        <v>0.0197</v>
       </c>
     </row>
     <row r="16">
@@ -980,13 +995,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.5513</v>
+        <v>-0.8325</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3624</v>
+        <v>0.3752</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1282</v>
+        <v>0.0265</v>
       </c>
     </row>
     <row r="17">
@@ -994,13 +1009,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4823</v>
+        <v>-0.7239</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3485</v>
+        <v>0.3594</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1664</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="18">
@@ -1008,13 +1023,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.4713</v>
+        <v>-0.6939</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3404</v>
+        <v>0.3492</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1661</v>
+        <v>0.0469</v>
       </c>
     </row>
     <row r="19">
@@ -1022,13 +1037,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.5076</v>
+        <v>-0.7323</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3404</v>
+        <v>0.3497</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1359</v>
+        <v>0.0363</v>
       </c>
     </row>
     <row r="20">
@@ -1036,13 +1051,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4477</v>
+        <v>-0.6578</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3486</v>
+        <v>0.3608</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1991</v>
+        <v>0.0682</v>
       </c>
     </row>
     <row r="21">
@@ -1050,13 +1065,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3903</v>
+        <v>-0.6246</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3512</v>
+        <v>0.3637</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2663</v>
+        <v>0.0859</v>
       </c>
     </row>
     <row r="22">
@@ -1064,13 +1079,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.555</v>
+        <v>-0.8915</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3548</v>
+        <v>0.3769</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1178</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="23">
@@ -1078,13 +1093,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.7725</v>
+        <v>-1.2286</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4429</v>
+        <v>0.4868</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0811</v>
+        <v>0.0116</v>
       </c>
     </row>
     <row r="24">
@@ -1092,10 +1107,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.6532</v>
+        <v>-0.3838</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0589</v>
+        <v>0.0526</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1134,13 +1149,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6536</v>
+        <v>3.0154</v>
       </c>
       <c r="C2" t="n">
-        <v>1.1937</v>
+        <v>0.2362</v>
       </c>
       <c r="D2" t="n">
-        <v>0.584</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1148,13 +1163,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2104</v>
+        <v>0.0007</v>
       </c>
       <c r="C3" t="n">
-        <v>0.28</v>
+        <v>0.0633</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4523</v>
+        <v>0.9909</v>
       </c>
     </row>
     <row r="4">
@@ -1162,13 +1177,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.1423</v>
+        <v>0.049</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2809</v>
+        <v>0.0582</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6125</v>
+        <v>0.4003</v>
       </c>
     </row>
     <row r="5">
@@ -1176,13 +1191,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7964</v>
+        <v>0.0258</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4608</v>
+        <v>0.1063</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0839</v>
+        <v>0.8078</v>
       </c>
     </row>
     <row r="6">
@@ -1190,13 +1205,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-4.1308</v>
+        <v>0.0984</v>
       </c>
       <c r="C6" t="n">
-        <v>31132.3064</v>
+        <v>0.1105</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9999</v>
+        <v>0.3729</v>
       </c>
     </row>
     <row r="7">
@@ -1204,13 +1219,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.1033</v>
+        <v>0.0582</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5976</v>
+        <v>0.1088</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8627</v>
+        <v>0.5927</v>
       </c>
     </row>
     <row r="8">
@@ -1218,13 +1233,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-4.2098</v>
+        <v>-0.0619</v>
       </c>
       <c r="C8" t="n">
-        <v>33127.983</v>
+        <v>0.1145</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9999</v>
+        <v>0.5889</v>
       </c>
     </row>
     <row r="9">
@@ -1232,13 +1247,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-3.3352</v>
+        <v>-0.2267</v>
       </c>
       <c r="C9" t="n">
-        <v>34711.4847</v>
+        <v>0.1372</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9999</v>
+        <v>0.0985</v>
       </c>
     </row>
     <row r="10">
@@ -1246,13 +1261,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3199</v>
+        <v>-0.1448</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4924</v>
+        <v>0.111</v>
       </c>
       <c r="D10" t="n">
-        <v>0.516</v>
+        <v>0.1922</v>
       </c>
     </row>
     <row r="11">
@@ -1260,13 +1275,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.3848</v>
+        <v>-0.1693</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6546</v>
+        <v>0.119</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5567</v>
+        <v>0.1547</v>
       </c>
     </row>
     <row r="12">
@@ -1274,13 +1289,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1796</v>
+        <v>-0.173</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8383</v>
+        <v>0.1649</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8304</v>
+        <v>0.294</v>
       </c>
     </row>
     <row r="13">
@@ -1288,13 +1303,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.3215</v>
+        <v>-0.3233</v>
       </c>
       <c r="C13" t="n">
-        <v>1.2172</v>
+        <v>0.2305</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7917</v>
+        <v>0.1607</v>
       </c>
     </row>
     <row r="14">
@@ -1302,13 +1317,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.2983</v>
+        <v>-0.3871</v>
       </c>
       <c r="C14" t="n">
-        <v>1.2949</v>
+        <v>0.238</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8178</v>
+        <v>0.1039</v>
       </c>
     </row>
     <row r="15">
@@ -1316,13 +1331,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0764</v>
+        <v>-0.4319</v>
       </c>
       <c r="C15" t="n">
-        <v>1.2655</v>
+        <v>0.2329</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9519</v>
+        <v>0.0637</v>
       </c>
     </row>
     <row r="16">
@@ -1330,13 +1345,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2627</v>
+        <v>-0.4815</v>
       </c>
       <c r="C16" t="n">
-        <v>1.183</v>
+        <v>0.2254</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8242</v>
+        <v>0.0327</v>
       </c>
     </row>
     <row r="17">
@@ -1344,13 +1359,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.6006</v>
+        <v>-0.5076</v>
       </c>
       <c r="C17" t="n">
-        <v>1.1302</v>
+        <v>0.2194</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5952</v>
+        <v>0.0207</v>
       </c>
     </row>
     <row r="18">
@@ -1358,13 +1373,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.797</v>
+        <v>-0.475</v>
       </c>
       <c r="C18" t="n">
-        <v>1.1185</v>
+        <v>0.2142</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4761</v>
+        <v>0.0266</v>
       </c>
     </row>
     <row r="19">
@@ -1372,13 +1387,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>0.3992</v>
+        <v>-0.4041</v>
       </c>
       <c r="C19" t="n">
-        <v>1.119</v>
+        <v>0.2133</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7213</v>
+        <v>0.0582</v>
       </c>
     </row>
     <row r="20">
@@ -1386,13 +1401,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0343</v>
+        <v>-0.3984</v>
       </c>
       <c r="C20" t="n">
-        <v>1.1592</v>
+        <v>0.2221</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9764</v>
+        <v>0.0728</v>
       </c>
     </row>
     <row r="21">
@@ -1400,13 +1415,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>0.0067</v>
+        <v>-0.4137</v>
       </c>
       <c r="C21" t="n">
-        <v>1.1774</v>
+        <v>0.2277</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9955</v>
+        <v>0.0693</v>
       </c>
     </row>
     <row r="22">
@@ -1414,13 +1429,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>0.2032</v>
+        <v>-0.3643</v>
       </c>
       <c r="C22" t="n">
-        <v>1.1655</v>
+        <v>0.2334</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8616</v>
+        <v>0.1185</v>
       </c>
     </row>
     <row r="23">
@@ -1428,13 +1443,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4415</v>
+        <v>-0.2967</v>
       </c>
       <c r="C23" t="n">
-        <v>1.4466</v>
+        <v>0.3006</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7602</v>
+        <v>0.3236</v>
       </c>
     </row>
     <row r="24">
@@ -1442,13 +1457,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.2729</v>
+        <v>-0.9546</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1272</v>
+        <v>0.0661</v>
       </c>
       <c r="D24" t="n">
-        <v>0.032</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1499,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.8062</v>
+        <v>3.7515</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1794</v>
+        <v>0.4089</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1498,13 +1513,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0303</v>
+        <v>0.0611</v>
       </c>
       <c r="C3" t="n">
-        <v>0.049</v>
+        <v>0.0838</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5363</v>
+        <v>0.4659</v>
       </c>
     </row>
     <row r="4">
@@ -1512,13 +1527,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0409</v>
+        <v>0.0081</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0459</v>
+        <v>0.0822</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3729</v>
+        <v>0.9215</v>
       </c>
     </row>
     <row r="5">
@@ -1526,13 +1541,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0062</v>
+        <v>0.4339</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0808</v>
+        <v>0.2323</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9385</v>
+        <v>0.0618</v>
       </c>
     </row>
     <row r="6">
@@ -1540,13 +1555,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.0508</v>
+        <v>0.1996</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09</v>
+        <v>0.2332</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5723</v>
+        <v>0.392</v>
       </c>
     </row>
     <row r="7">
@@ -1554,13 +1569,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0425</v>
+        <v>0.2214</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0822</v>
+        <v>0.2435</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6055</v>
+        <v>0.3633</v>
       </c>
     </row>
     <row r="8">
@@ -1568,13 +1583,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0705</v>
+        <v>-0.0493</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0929</v>
+        <v>0.3057</v>
       </c>
       <c r="D8" t="n">
-        <v>0.448</v>
+        <v>0.8719</v>
       </c>
     </row>
     <row r="9">
@@ -1582,13 +1597,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.1751</v>
+        <v>0.0826</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1048</v>
+        <v>0.296</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0948</v>
+        <v>0.7803</v>
       </c>
     </row>
     <row r="10">
@@ -1596,13 +1611,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.1305</v>
+        <v>-0.0255</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0857</v>
+        <v>0.2845</v>
       </c>
       <c r="D10" t="n">
-        <v>0.128</v>
+        <v>0.9286</v>
       </c>
     </row>
     <row r="11">
@@ -1610,13 +1625,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1154</v>
+        <v>0.1265</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0932</v>
+        <v>0.2355</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2155</v>
+        <v>0.5912</v>
       </c>
     </row>
     <row r="12">
@@ -1624,13 +1639,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0717</v>
+        <v>-0.2965</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1281</v>
+        <v>0.2866</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5758</v>
+        <v>0.3009</v>
       </c>
     </row>
     <row r="13">
@@ -1638,13 +1653,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.1335</v>
+        <v>-0.5605</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1793</v>
+        <v>0.4005</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4565</v>
+        <v>0.1617</v>
       </c>
     </row>
     <row r="14">
@@ -1652,13 +1667,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.15</v>
+        <v>-0.6597</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1866</v>
+        <v>0.4219</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4216</v>
+        <v>0.1179</v>
       </c>
     </row>
     <row r="15">
@@ -1666,13 +1681,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.1739</v>
+        <v>-0.6071</v>
       </c>
       <c r="C15" t="n">
-        <v>0.183</v>
+        <v>0.4086</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3419</v>
+        <v>0.1373</v>
       </c>
     </row>
     <row r="16">
@@ -1680,13 +1695,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.2197</v>
+        <v>-0.4944</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1755</v>
+        <v>0.3736</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2106</v>
+        <v>0.1857</v>
       </c>
     </row>
     <row r="17">
@@ -1694,13 +1709,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.2461</v>
+        <v>-0.3852</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1704</v>
+        <v>0.3505</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1487</v>
+        <v>0.2718</v>
       </c>
     </row>
     <row r="18">
@@ -1708,13 +1723,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.2325</v>
+        <v>-0.2984</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1667</v>
+        <v>0.3429</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1632</v>
+        <v>0.3842</v>
       </c>
     </row>
     <row r="19">
@@ -1722,13 +1737,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.1979</v>
+        <v>-0.2582</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1663</v>
+        <v>0.3434</v>
       </c>
       <c r="D19" t="n">
-        <v>0.234</v>
+        <v>0.4521</v>
       </c>
     </row>
     <row r="20">
@@ -1736,13 +1751,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.1916</v>
+        <v>-0.2897</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1729</v>
+        <v>0.3607</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2678</v>
+        <v>0.4218</v>
       </c>
     </row>
     <row r="21">
@@ -1750,13 +1765,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.2</v>
+        <v>-0.3663</v>
       </c>
       <c r="C21" t="n">
-        <v>0.177</v>
+        <v>0.3838</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2585</v>
+        <v>0.3399</v>
       </c>
     </row>
     <row r="22">
@@ -1764,13 +1779,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.1708</v>
+        <v>-0.4244</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1814</v>
+        <v>0.4507</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3462</v>
+        <v>0.3464</v>
       </c>
     </row>
     <row r="23">
@@ -1778,13 +1793,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.1306</v>
+        <v>-0.4789</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2335</v>
+        <v>0.6402</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5759</v>
+        <v>0.4544</v>
       </c>
     </row>
     <row r="24">
@@ -1792,10 +1807,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.5118</v>
+        <v>-1.0572</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0797</v>
+        <v>0.1036</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -1834,10 +1849,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.6956</v>
+        <v>2.2819</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5517</v>
+        <v>0.3198</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1848,13 +1863,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0617</v>
+        <v>-0.3976</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0931</v>
+        <v>0.0877</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1862,13 +1877,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.0038</v>
+        <v>-0.4152</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0992</v>
+        <v>0.091</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9695</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1876,13 +1891,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5066</v>
+        <v>0.4098</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4029</v>
+        <v>0.1705</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2086</v>
+        <v>0.0162</v>
       </c>
     </row>
     <row r="6">
@@ -1890,13 +1905,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2732</v>
+        <v>-0.3434</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4071</v>
+        <v>0.2282</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5022</v>
+        <v>0.1324</v>
       </c>
     </row>
     <row r="7">
@@ -1904,13 +1919,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3417</v>
+        <v>0.2732</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4097</v>
+        <v>0.1781</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4043</v>
+        <v>0.1251</v>
       </c>
     </row>
     <row r="8">
@@ -1918,13 +1933,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0368</v>
+        <v>-0.4675</v>
       </c>
       <c r="C8" t="n">
-        <v>0.508</v>
+        <v>0.2682</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9422</v>
+        <v>0.0813</v>
       </c>
     </row>
     <row r="9">
@@ -1932,13 +1947,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0543</v>
+        <v>0.4277</v>
       </c>
       <c r="C9" t="n">
-        <v>0.467</v>
+        <v>0.1958</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9074</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="10">
@@ -1946,13 +1961,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0394</v>
+        <v>0.1174</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4375</v>
+        <v>0.1772</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9282</v>
+        <v>0.5076</v>
       </c>
     </row>
     <row r="11">
@@ -1960,13 +1975,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2517</v>
+        <v>-0.4106</v>
       </c>
       <c r="C11" t="n">
-        <v>0.407</v>
+        <v>0.2805</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5363</v>
+        <v>0.1432</v>
       </c>
     </row>
     <row r="12">
@@ -1974,13 +1989,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.3645</v>
+        <v>-0.0623</v>
       </c>
       <c r="C12" t="n">
-        <v>0.3331</v>
+        <v>0.2198</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2739</v>
+        <v>0.7768</v>
       </c>
     </row>
     <row r="13">
@@ -1988,13 +2003,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.6841</v>
+        <v>-0.1169</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4614</v>
+        <v>0.3014</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1382</v>
+        <v>0.6981</v>
       </c>
     </row>
     <row r="14">
@@ -2002,13 +2017,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.7966</v>
+        <v>-0.1194</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4828</v>
+        <v>0.3122</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0989</v>
+        <v>0.7022</v>
       </c>
     </row>
     <row r="15">
@@ -2016,13 +2031,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.7271</v>
+        <v>-0.0318</v>
       </c>
       <c r="C15" t="n">
-        <v>0.461</v>
+        <v>0.3081</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1147</v>
+        <v>0.9177</v>
       </c>
     </row>
     <row r="16">
@@ -2030,13 +2045,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.5878</v>
+        <v>0.0892</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4163</v>
+        <v>0.2944</v>
       </c>
       <c r="D16" t="n">
-        <v>0.158</v>
+        <v>0.7619</v>
       </c>
     </row>
     <row r="17">
@@ -2044,13 +2059,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4762</v>
+        <v>0.2285</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3919</v>
+        <v>0.2871</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2243</v>
+        <v>0.4261</v>
       </c>
     </row>
     <row r="18">
@@ -2058,13 +2073,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.4278</v>
+        <v>0.2597</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3856</v>
+        <v>0.2835</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2673</v>
+        <v>0.3596</v>
       </c>
     </row>
     <row r="19">
@@ -2072,13 +2087,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.4209</v>
+        <v>0.048</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3858</v>
+        <v>0.2842</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2753</v>
+        <v>0.8658</v>
       </c>
     </row>
     <row r="20">
@@ -2086,13 +2101,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4618</v>
+        <v>-0.0453</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4089</v>
+        <v>0.2999</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2587</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="21">
@@ -2100,13 +2115,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.5497</v>
+        <v>0.0083</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4485</v>
+        <v>0.3088</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2203</v>
+        <v>0.9786</v>
       </c>
     </row>
     <row r="22">
@@ -2114,13 +2129,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.6302</v>
+        <v>0.1138</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5566</v>
+        <v>0.3171</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2575</v>
+        <v>0.7196</v>
       </c>
     </row>
     <row r="23">
@@ -2128,13 +2143,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.7091</v>
+        <v>0.2256</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8097</v>
+        <v>0.4173</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3812</v>
+        <v>0.5887</v>
       </c>
     </row>
     <row r="24">
@@ -2142,10 +2157,10 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.2996</v>
+        <v>-0.9581</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1361</v>
+        <v>0.0612</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -2184,13 +2199,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>2.315</v>
+        <v>3.4383</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2838</v>
+        <v>1.18</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
     </row>
     <row r="3">
@@ -2198,13 +2213,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2653</v>
+        <v>0.6208</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0817</v>
+        <v>0.2413</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0012</v>
+        <v>0.0101</v>
       </c>
     </row>
     <row r="4">
@@ -2212,13 +2227,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.3223</v>
+        <v>0.3603</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0884</v>
+        <v>0.2329</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0003</v>
+        <v>0.1218</v>
       </c>
     </row>
     <row r="5">
@@ -2226,13 +2241,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2152</v>
+        <v>-0.0803</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1585</v>
+        <v>0.5219</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1745</v>
+        <v>0.8778</v>
       </c>
     </row>
     <row r="6">
@@ -2240,13 +2255,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3065</v>
+        <v>0.5088</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2529</v>
+        <v>0.3949</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2254</v>
+        <v>0.1975</v>
       </c>
     </row>
     <row r="7">
@@ -2254,13 +2269,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2063</v>
+        <v>-0.4649</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1625</v>
+        <v>0.6191</v>
       </c>
       <c r="D7" t="n">
-        <v>0.2041</v>
+        <v>0.4527</v>
       </c>
     </row>
     <row r="8">
@@ -2268,13 +2283,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.4051</v>
+        <v>0.4744</v>
       </c>
       <c r="C8" t="n">
-        <v>0.342</v>
+        <v>0.3789</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2362</v>
+        <v>0.2106</v>
       </c>
     </row>
     <row r="9">
@@ -2282,13 +2297,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3051</v>
+        <v>-0.6808</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1764</v>
+        <v>0.6625</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0836</v>
+        <v>0.3041</v>
       </c>
     </row>
     <row r="10">
@@ -2296,13 +2311,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.061</v>
+        <v>-1.6174</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1622</v>
+        <v>942.2577</v>
       </c>
       <c r="D10" t="n">
-        <v>0.707</v>
+        <v>0.9986</v>
       </c>
     </row>
     <row r="11">
@@ -2310,13 +2325,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.4734</v>
+        <v>-1.0266</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5145</v>
+        <v>1300.57</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3575</v>
+        <v>0.9994</v>
       </c>
     </row>
     <row r="12">
@@ -2324,13 +2339,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0528</v>
+        <v>-1.1952</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1969</v>
+        <v>0.9579</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7886</v>
+        <v>0.2121</v>
       </c>
     </row>
     <row r="13">
@@ -2338,13 +2353,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.0986</v>
+        <v>-2.2438</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2659</v>
+        <v>1.4255</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7109</v>
+        <v>0.1155</v>
       </c>
     </row>
     <row r="14">
@@ -2352,13 +2367,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.1032</v>
+        <v>-2.8393</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2718</v>
+        <v>1.6632</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7043</v>
+        <v>0.0878</v>
       </c>
     </row>
     <row r="15">
@@ -2366,13 +2381,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.0517</v>
+        <v>-3.0455</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2678</v>
+        <v>1.6886</v>
       </c>
       <c r="D15" t="n">
-        <v>0.847</v>
+        <v>0.0713</v>
       </c>
     </row>
     <row r="16">
@@ -2380,13 +2395,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0129</v>
+        <v>-2.9566</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2559</v>
+        <v>1.5161</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9599</v>
+        <v>0.0512</v>
       </c>
     </row>
     <row r="17">
@@ -2394,13 +2409,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0513</v>
+        <v>-2.6644</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2506</v>
+        <v>1.2651</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8379</v>
+        <v>0.0352</v>
       </c>
     </row>
     <row r="18">
@@ -2408,13 +2423,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0151</v>
+        <v>-2.1991</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2487</v>
+        <v>1.1244</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9516</v>
+        <v>0.0505</v>
       </c>
     </row>
     <row r="19">
@@ -2422,13 +2437,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.0803</v>
+        <v>-2.1341</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2484</v>
+        <v>1.1177</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7466</v>
+        <v>0.0562</v>
       </c>
     </row>
     <row r="20">
@@ -2436,13 +2451,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.1165</v>
+        <v>-2.2101</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2637</v>
+        <v>1.1493</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6586</v>
+        <v>0.0545</v>
       </c>
     </row>
     <row r="21">
@@ -2450,13 +2465,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.0855</v>
+        <v>-2.0527</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2735</v>
+        <v>1.1667</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7547</v>
+        <v>0.0785</v>
       </c>
     </row>
     <row r="22">
@@ -2464,13 +2479,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.0216</v>
+        <v>-2.2439</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2851</v>
+        <v>1.2008</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9396</v>
+        <v>0.0617</v>
       </c>
     </row>
     <row r="23">
@@ -2478,13 +2493,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>0.048</v>
+        <v>-2.505</v>
       </c>
       <c r="C23" t="n">
-        <v>0.3831</v>
+        <v>1.5055</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9003</v>
+        <v>0.0961</v>
       </c>
     </row>
     <row r="24">
@@ -2492,13 +2507,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-1.3513</v>
+        <v>-0.6015</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0814</v>
+        <v>0.1774</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
     </row>
   </sheetData>
@@ -2534,13 +2549,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>3.3025</v>
+        <v>3.3102</v>
       </c>
       <c r="C2" t="n">
-        <v>1.2803</v>
+        <v>0.6893</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2548,13 +2563,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5262</v>
+        <v>-0.0768</v>
       </c>
       <c r="C3" t="n">
-        <v>0.243</v>
+        <v>0.2004</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0303</v>
+        <v>0.7013</v>
       </c>
     </row>
     <row r="4">
@@ -2562,13 +2577,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3542</v>
+        <v>0.3973</v>
       </c>
       <c r="C4" t="n">
-        <v>0.233</v>
+        <v>0.1766</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1285</v>
+        <v>0.0245</v>
       </c>
     </row>
     <row r="5">
@@ -2576,13 +2591,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1365</v>
+        <v>0.0691</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6849</v>
+        <v>0.3382</v>
       </c>
       <c r="D5" t="n">
-        <v>0.842</v>
+        <v>0.8382</v>
       </c>
     </row>
     <row r="6">
@@ -2590,13 +2605,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.607</v>
+        <v>-0.0892</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5845</v>
+        <v>0.3434</v>
       </c>
       <c r="D6" t="n">
-        <v>0.299</v>
+        <v>0.7949</v>
       </c>
     </row>
     <row r="7">
@@ -2604,13 +2619,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.2895</v>
+        <v>0.1367</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7234</v>
+        <v>0.3414</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6891</v>
+        <v>0.6888</v>
       </c>
     </row>
     <row r="8">
@@ -2618,13 +2633,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6646</v>
+        <v>0.1667</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5659</v>
+        <v>0.3501</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2402</v>
+        <v>0.6339</v>
       </c>
     </row>
     <row r="9">
@@ -2632,13 +2647,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.4127</v>
+        <v>-0.282</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7752</v>
+        <v>0.4135</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5945</v>
+        <v>0.4952</v>
       </c>
     </row>
     <row r="10">
@@ -2646,13 +2661,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.0377</v>
+        <v>-0.8794</v>
       </c>
       <c r="C10" t="n">
-        <v>2189.6613</v>
+        <v>0.3386</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9993</v>
+        <v>0.0094</v>
       </c>
     </row>
     <row r="11">
@@ -2660,13 +2675,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-1.4508</v>
+        <v>0.432</v>
       </c>
       <c r="C11" t="n">
-        <v>2981.6323</v>
+        <v>0.3456</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9996</v>
+        <v>0.2113</v>
       </c>
     </row>
     <row r="12">
@@ -2674,13 +2689,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-1.2623</v>
+        <v>-0.3069</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9743</v>
+        <v>0.4892</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1951</v>
+        <v>0.5305</v>
       </c>
     </row>
     <row r="13">
@@ -2688,13 +2703,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.3668</v>
+        <v>-0.541</v>
       </c>
       <c r="C13" t="n">
-        <v>1.4649</v>
+        <v>0.6848</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1062</v>
+        <v>0.4295</v>
       </c>
     </row>
     <row r="14">
@@ -2702,13 +2717,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="n">
-        <v>-2.9957</v>
+        <v>-0.4909</v>
       </c>
       <c r="C14" t="n">
-        <v>1.7185</v>
+        <v>0.7054</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0813</v>
+        <v>0.4865</v>
       </c>
     </row>
     <row r="15">
@@ -2716,13 +2731,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="n">
-        <v>-3.2126</v>
+        <v>-0.4449</v>
       </c>
       <c r="C15" t="n">
-        <v>1.744</v>
+        <v>0.6915</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0655</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="16">
@@ -2730,13 +2745,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="n">
-        <v>-3.1079</v>
+        <v>-0.5284</v>
       </c>
       <c r="C16" t="n">
-        <v>1.5638</v>
+        <v>0.6708</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0469</v>
+        <v>0.4309</v>
       </c>
     </row>
     <row r="17">
@@ -2744,13 +2759,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.7713</v>
+        <v>-0.6134</v>
       </c>
       <c r="C17" t="n">
-        <v>1.3013</v>
+        <v>0.6539</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0332</v>
+        <v>0.3483</v>
       </c>
     </row>
     <row r="18">
@@ -2758,13 +2773,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.2698</v>
+        <v>-0.6791</v>
       </c>
       <c r="C18" t="n">
-        <v>1.1417</v>
+        <v>0.6436</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0468</v>
+        <v>0.2913</v>
       </c>
     </row>
     <row r="19">
@@ -2772,13 +2787,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>-2.1592</v>
+        <v>-0.7422</v>
       </c>
       <c r="C19" t="n">
-        <v>1.1317</v>
+        <v>0.6429</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0564</v>
+        <v>0.2483</v>
       </c>
     </row>
     <row r="20">
@@ -2786,13 +2801,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>-2.2244</v>
+        <v>-0.8439</v>
       </c>
       <c r="C20" t="n">
-        <v>1.1697</v>
+        <v>0.6685</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0572</v>
+        <v>0.2068</v>
       </c>
     </row>
     <row r="21">
@@ -2800,13 +2815,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="n">
-        <v>-2.0845</v>
+        <v>-0.7499</v>
       </c>
       <c r="C21" t="n">
-        <v>1.187</v>
+        <v>0.6845</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0791</v>
+        <v>0.2733</v>
       </c>
     </row>
     <row r="22">
@@ -2814,13 +2829,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="n">
-        <v>-2.3118</v>
+        <v>-0.5143</v>
       </c>
       <c r="C22" t="n">
-        <v>1.2185</v>
+        <v>0.7125</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0578</v>
+        <v>0.4704</v>
       </c>
     </row>
     <row r="23">
@@ -2828,13 +2843,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="n">
-        <v>-2.6108</v>
+        <v>-0.2765</v>
       </c>
       <c r="C23" t="n">
-        <v>1.5281</v>
+        <v>0.9239</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0875</v>
+        <v>0.7647</v>
       </c>
     </row>
     <row r="24">
@@ -2842,363 +2857,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.9765</v>
+        <v>0.2522</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2063</v>
+        <v>0.0658</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.5094</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="n">
-        <v>-0.0697</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.1491</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.2093</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.1289</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.1044</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-0.0263</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2367</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.9114</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-0.1329</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.2392</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5783</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.0402</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.2417</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.8679</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-0.2888</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.2533</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.2543</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.3181</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.2973</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.2846</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.7947</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.2635</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0026</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.1406</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.2384</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.5555</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="n">
-        <v>-0.1911</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.3592</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.5947</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="n">
-        <v>-0.3377</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.5081</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.5063</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="n">
-        <v>-0.292</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.5321</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.5832</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="n">
-        <v>-0.2599</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.5222</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.6188</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="n">
-        <v>-0.3529</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.502</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.4822</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="n">
-        <v>-0.4626</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.4881</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.3433</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="n">
-        <v>-0.5216</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.4803</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.2774</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="n">
-        <v>-0.5281</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.481</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.2722</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="n">
-        <v>-0.556</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.4993</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.2655</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="n">
-        <v>-0.4393</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.5104</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.3893</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.2169</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.5292</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.6818</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.0068</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.6781</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="n">
-        <v>-0.2728</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #70: Add the calculation of the confidence intervals to the files with results (#76)
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate_on_the_response_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lwr_on_the_response_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uppr_on_the_response_scale</t>
   </si>
   <si>
     <t xml:space="preserve">(Intercept)</t>
@@ -444,10 +453,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>0.2467</v>
@@ -458,10 +476,19 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
+      <c r="E2" t="n">
+        <v>1.2798</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2594</v>
@@ -472,10 +499,19 @@
       <c r="D3" t="n">
         <v>0.2453</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.7715</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.1951</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.1332</v>
@@ -486,10 +522,19 @@
       <c r="D4" t="n">
         <v>0.4313</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.8753</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6283</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2195</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>1.7447</v>
@@ -500,10 +545,19 @@
       <c r="D5" t="n">
         <v>1</v>
       </c>
+      <c r="E5" t="n">
+        <v>5.7239</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>1.8242</v>
@@ -514,30 +568,45 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="n">
+        <v>6.1975</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>1.3494</v>
@@ -548,30 +617,45 @@
       <c r="D9" t="n">
         <v>1</v>
       </c>
+      <c r="E9" t="n">
+        <v>3.8551</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.5778</v>
@@ -582,10 +666,19 @@
       <c r="D12" t="n">
         <v>0.3643</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.5611</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.9553</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-1.0665</v>
@@ -596,10 +689,19 @@
       <c r="D13" t="n">
         <v>0.218</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.3442</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0631</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.878</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-1.2398</v>
@@ -610,10 +712,19 @@
       <c r="D14" t="n">
         <v>0.1571</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.2895</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.6125</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-1.1869</v>
@@ -624,10 +735,19 @@
       <c r="D15" t="n">
         <v>0.1421</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.3052</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0626</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.4883</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-1.0491</v>
@@ -638,10 +758,19 @@
       <c r="D16" t="n">
         <v>0.165</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.3503</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0797</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.5401</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.8321</v>
@@ -652,10 +781,19 @@
       <c r="D17" t="n">
         <v>0.2434</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.4351</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1075</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.761</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.7644</v>
@@ -666,10 +804,19 @@
       <c r="D18" t="n">
         <v>0.2736</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.4656</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1185</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.8297</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.9932</v>
@@ -680,10 +827,19 @@
       <c r="D19" t="n">
         <v>0.1547</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.3704</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0943</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.4546</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-1.1157</v>
@@ -694,10 +850,19 @@
       <c r="D20" t="n">
         <v>0.1406</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.3277</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0743</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4452</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-1.1348</v>
@@ -708,10 +873,19 @@
       <c r="D21" t="n">
         <v>0.1823</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.3215</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0607</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.7041</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-1.1315</v>
@@ -722,10 +896,19 @@
       <c r="D22" t="n">
         <v>0.3256</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.3225</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0338</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3.0786</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-1.1283</v>
@@ -736,10 +919,19 @@
       <c r="D23" t="n">
         <v>0.521</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.3236</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0103</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10.1497</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.225</v>
@@ -749,6 +941,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2938</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1902</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.4536</v>
       </c>
     </row>
   </sheetData>
@@ -778,10 +979,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.6353</v>
@@ -792,10 +1002,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>13.9481</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6.8806</v>
+      </c>
+      <c r="G2" t="n">
+        <v>28.2752</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.1302</v>
@@ -806,10 +1025,19 @@
       <c r="D3" t="n">
         <v>0.1586</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.1391</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9504</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.3651</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.0416</v>
@@ -820,10 +1048,19 @@
       <c r="D4" t="n">
         <v>0.6332</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.0424</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8788</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2365</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>-0.2778</v>
@@ -834,10 +1071,19 @@
       <c r="D5" t="n">
         <v>0.1006</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.7575</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5437</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.0553</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.2237</v>
@@ -848,10 +1094,19 @@
       <c r="D6" t="n">
         <v>0.1486</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.2508</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9233</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.6944</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.5301</v>
@@ -862,10 +1117,19 @@
       <c r="D7" t="n">
         <v>0.0088</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.5885</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3959</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>0.3141</v>
@@ -876,10 +1140,19 @@
       <c r="D8" t="n">
         <v>0.0424</v>
       </c>
+      <c r="E8" t="n">
+        <v>1.369</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.0108</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.8541</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.3997</v>
@@ -890,10 +1163,19 @@
       <c r="D9" t="n">
         <v>0.0634</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.6705</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4396</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.0226</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.241</v>
@@ -904,10 +1186,19 @@
       <c r="D10" t="n">
         <v>0.1011</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.2726</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.954</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.6975</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.1211</v>
@@ -918,10 +1209,19 @@
       <c r="D11" t="n">
         <v>0.4696</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6381</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.2301</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.2446</v>
@@ -932,10 +1232,19 @@
       <c r="D12" t="n">
         <v>0.3288</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4792</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.2793</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.4456</v>
@@ -946,10 +1255,19 @@
       <c r="D13" t="n">
         <v>0.2137</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.6404</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.3173</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2927</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.5311</v>
@@ -960,10 +1278,19 @@
       <c r="D14" t="n">
         <v>0.161</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.588</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.2798</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.2356</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.5908</v>
@@ -974,10 +1301,19 @@
       <c r="D15" t="n">
         <v>0.1148</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.5539</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.2658</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.1542</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.5513</v>
@@ -988,10 +1324,19 @@
       <c r="D16" t="n">
         <v>0.1282</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.5762</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2832</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.1724</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4823</v>
@@ -1002,10 +1347,19 @@
       <c r="D17" t="n">
         <v>0.1664</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6174</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3118</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.2224</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.4713</v>
@@ -1016,10 +1370,19 @@
       <c r="D18" t="n">
         <v>0.1661</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.6242</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3203</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.2163</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.5076</v>
@@ -1030,10 +1393,19 @@
       <c r="D19" t="n">
         <v>0.1359</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3089</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.173</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.4477</v>
@@ -1044,10 +1416,19 @@
       <c r="D20" t="n">
         <v>0.1991</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.6391</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.3227</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.2656</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.3903</v>
@@ -1058,10 +1439,19 @@
       <c r="D21" t="n">
         <v>0.2663</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.6768</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.3401</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.3471</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.555</v>
@@ -1072,10 +1462,19 @@
       <c r="D22" t="n">
         <v>0.1178</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.5741</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.2864</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.1508</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.7725</v>
@@ -1086,10 +1485,19 @@
       <c r="D23" t="n">
         <v>0.0811</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.4618</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1939</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.1003</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.6532</v>
@@ -1099,6 +1507,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5204</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.4637</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.584</v>
       </c>
     </row>
   </sheetData>
@@ -1128,10 +1545,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>0.6536</v>
@@ -1142,10 +1568,19 @@
       <c r="D2" t="n">
         <v>0.584</v>
       </c>
+      <c r="E2" t="n">
+        <v>1.9225</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1853</v>
+      </c>
+      <c r="G2" t="n">
+        <v>19.9503</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2104</v>
@@ -1156,10 +1591,19 @@
       <c r="D3" t="n">
         <v>0.4523</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.8103</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.4681</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.4025</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.1423</v>
@@ -1170,10 +1614,19 @@
       <c r="D4" t="n">
         <v>0.6125</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.8674</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5001</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.5043</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.7964</v>
@@ -1184,10 +1637,19 @@
       <c r="D5" t="n">
         <v>0.0839</v>
       </c>
+      <c r="E5" t="n">
+        <v>2.2176</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8987</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5.4718</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-4.1308</v>
@@ -1198,10 +1660,19 @@
       <c r="D6" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.0161</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.1033</v>
@@ -1212,10 +1683,19 @@
       <c r="D7" t="n">
         <v>0.8627</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.9018</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2795</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.9096</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-4.2098</v>
@@ -1226,10 +1706,19 @@
       <c r="D8" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.0148</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-3.3352</v>
@@ -1240,10 +1729,19 @@
       <c r="D9" t="n">
         <v>0.9999</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.0356</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.3199</v>
@@ -1254,10 +1752,19 @@
       <c r="D10" t="n">
         <v>0.516</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.3769</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5245</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.6145</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.3848</v>
@@ -1268,10 +1775,19 @@
       <c r="D11" t="n">
         <v>0.5567</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.6806</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1887</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.4553</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.1796</v>
@@ -1282,10 +1798,19 @@
       <c r="D12" t="n">
         <v>0.8304</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.8356</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1616</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.3206</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.3215</v>
@@ -1296,10 +1821,19 @@
       <c r="D13" t="n">
         <v>0.7917</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0667</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.8782</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.2983</v>
@@ -1310,10 +1844,19 @@
       <c r="D14" t="n">
         <v>0.8178</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.7421</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0586</v>
+      </c>
+      <c r="G14" t="n">
+        <v>9.3895</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.0764</v>
@@ -1324,10 +1867,19 @@
       <c r="D15" t="n">
         <v>0.9519</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.9264</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0776</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11.0659</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>0.2627</v>
@@ -1338,10 +1890,19 @@
       <c r="D16" t="n">
         <v>0.8242</v>
       </c>
+      <c r="E16" t="n">
+        <v>1.3005</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="G16" t="n">
+        <v>13.2141</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>0.6006</v>
@@ -1352,10 +1913,19 @@
       <c r="D17" t="n">
         <v>0.5952</v>
       </c>
+      <c r="E17" t="n">
+        <v>1.8232</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16.7071</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>0.797</v>
@@ -1366,10 +1936,19 @@
       <c r="D18" t="n">
         <v>0.4761</v>
       </c>
+      <c r="E18" t="n">
+        <v>2.219</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.2478</v>
+      </c>
+      <c r="G18" t="n">
+        <v>19.8728</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>0.3992</v>
@@ -1380,10 +1959,19 @@
       <c r="D19" t="n">
         <v>0.7213</v>
       </c>
+      <c r="E19" t="n">
+        <v>1.4906</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1663</v>
+      </c>
+      <c r="G19" t="n">
+        <v>13.3622</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>0.0343</v>
@@ -1394,10 +1982,19 @@
       <c r="D20" t="n">
         <v>0.9764</v>
       </c>
+      <c r="E20" t="n">
+        <v>1.0348</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1067</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10.0359</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>0.0067</v>
@@ -1408,10 +2005,19 @@
       <c r="D21" t="n">
         <v>0.9955</v>
       </c>
+      <c r="E21" t="n">
+        <v>1.0067</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1002</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10.1188</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>0.2032</v>
@@ -1422,10 +2028,19 @@
       <c r="D22" t="n">
         <v>0.8616</v>
       </c>
+      <c r="E22" t="n">
+        <v>1.2253</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1248</v>
+      </c>
+      <c r="G22" t="n">
+        <v>12.0323</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.4415</v>
@@ -1436,10 +2051,19 @@
       <c r="D23" t="n">
         <v>0.7602</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.555</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0913</v>
+      </c>
+      <c r="G23" t="n">
+        <v>26.4917</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.2729</v>
@@ -1449,6 +2073,15 @@
       </c>
       <c r="D24" t="n">
         <v>0.032</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.7612</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.5932</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9768</v>
       </c>
     </row>
   </sheetData>
@@ -1478,10 +2111,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.8062</v>
@@ -1492,10 +2134,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>16.5472</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11.6429</v>
+      </c>
+      <c r="G2" t="n">
+        <v>23.5174</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.0303</v>
@@ -1506,10 +2157,19 @@
       <c r="D3" t="n">
         <v>0.5363</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.0307</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9364</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.1346</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.0409</v>
@@ -1520,10 +2180,19 @@
       <c r="D4" t="n">
         <v>0.3729</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.0417</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9521</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.1398</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.0062</v>
@@ -1534,10 +2203,19 @@
       <c r="D5" t="n">
         <v>0.9385</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.0063</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8588</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.179</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.0508</v>
@@ -1548,10 +2226,19 @@
       <c r="D6" t="n">
         <v>0.5723</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.9504</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7967</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.1339</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.0425</v>
@@ -1562,10 +2249,19 @@
       <c r="D7" t="n">
         <v>0.6055</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.0434</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8881</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.2259</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0705</v>
@@ -1576,10 +2272,19 @@
       <c r="D8" t="n">
         <v>0.448</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.9319</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7768</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.1181</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.1751</v>
@@ -1590,10 +2295,19 @@
       <c r="D9" t="n">
         <v>0.0948</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.8394</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.6835</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.0308</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-0.1305</v>
@@ -1604,10 +2318,19 @@
       <c r="D10" t="n">
         <v>0.128</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.8777</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7419</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.0383</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.1154</v>
@@ -1618,10 +2341,19 @@
       <c r="D11" t="n">
         <v>0.2155</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.891</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7423</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.0695</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.0717</v>
@@ -1632,10 +2364,19 @@
       <c r="D12" t="n">
         <v>0.5758</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.9308</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.7241</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.1965</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.1335</v>
@@ -1646,10 +2387,19 @@
       <c r="D13" t="n">
         <v>0.4565</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6158</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2434</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.15</v>
@@ -1660,10 +2410,19 @@
       <c r="D14" t="n">
         <v>0.4216</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.8607</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.597</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.2408</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.1739</v>
@@ -1674,10 +2433,19 @@
       <c r="D15" t="n">
         <v>0.3419</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.8404</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5871</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.2029</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.2197</v>
@@ -1688,10 +2456,19 @@
       <c r="D16" t="n">
         <v>0.2106</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.8027</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5691</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.1323</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.2461</v>
@@ -1702,10 +2479,19 @@
       <c r="D17" t="n">
         <v>0.1487</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.7818</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5598</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.0919</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.2325</v>
@@ -1716,10 +2502,19 @@
       <c r="D18" t="n">
         <v>0.1632</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.7925</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.5716</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.0989</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.1979</v>
@@ -1730,10 +2525,19 @@
       <c r="D19" t="n">
         <v>0.234</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.8205</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5923</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.1365</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.1916</v>
@@ -1744,10 +2548,19 @@
       <c r="D20" t="n">
         <v>0.2678</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.8256</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5883</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.1587</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.2</v>
@@ -1758,10 +2571,19 @@
       <c r="D21" t="n">
         <v>0.2585</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.8187</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5787</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.1583</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.1708</v>
@@ -1772,10 +2594,19 @@
       <c r="D22" t="n">
         <v>0.3462</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5908</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.2028</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.1306</v>
@@ -1786,10 +2617,19 @@
       <c r="D23" t="n">
         <v>0.5759</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.8775</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.5552</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.3869</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.5118</v>
@@ -1799,6 +2639,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2205</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1886</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.2578</v>
       </c>
     </row>
   </sheetData>
@@ -1828,10 +2677,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.6956</v>
@@ -1842,10 +2700,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>40.2687</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13.6576</v>
+      </c>
+      <c r="G2" t="n">
+        <v>118.7305</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.0617</v>
@@ -1856,10 +2723,19 @@
       <c r="D3" t="n">
         <v>0.5074</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.0637</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8862</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.2766</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.0038</v>
@@ -1870,10 +2746,19 @@
       <c r="D4" t="n">
         <v>0.9695</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.9962</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8201</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.2101</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.5066</v>
@@ -1884,10 +2769,19 @@
       <c r="D5" t="n">
         <v>0.2086</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.6597</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7535</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.6557</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.2732</v>
@@ -1898,10 +2792,19 @@
       <c r="D6" t="n">
         <v>0.5022</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.3141</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5917</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.9184</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.3417</v>
@@ -1912,10 +2815,19 @@
       <c r="D7" t="n">
         <v>0.4043</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.4074</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6305</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.1416</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.0368</v>
@@ -1926,10 +2838,19 @@
       <c r="D8" t="n">
         <v>0.9422</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.9639</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3561</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2.6086</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>0.0543</v>
@@ -1940,10 +2861,19 @@
       <c r="D9" t="n">
         <v>0.9074</v>
       </c>
+      <c r="E9" t="n">
+        <v>1.0558</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4228</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.6367</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.0394</v>
@@ -1954,10 +2884,19 @@
       <c r="D10" t="n">
         <v>0.9282</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.0402</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4413</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.4519</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>0.2517</v>
@@ -1968,10 +2907,19 @@
       <c r="D11" t="n">
         <v>0.5363</v>
       </c>
+      <c r="E11" t="n">
+        <v>1.2862</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.5792</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.8563</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.3645</v>
@@ -1982,10 +2930,19 @@
       <c r="D12" t="n">
         <v>0.2739</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.6946</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3615</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.3344</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.6841</v>
@@ -1996,10 +2953,19 @@
       <c r="D13" t="n">
         <v>0.1382</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.5046</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.2043</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.2464</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.7966</v>
@@ -2010,10 +2976,19 @@
       <c r="D14" t="n">
         <v>0.0989</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.4509</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.1614</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.7271</v>
@@ -2024,10 +2999,19 @@
       <c r="D15" t="n">
         <v>0.1147</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.4833</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1958</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.1929</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.5878</v>
@@ -2038,10 +3022,19 @@
       <c r="D16" t="n">
         <v>0.158</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.5555</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2457</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.2563</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4762</v>
@@ -2052,10 +3045,19 @@
       <c r="D17" t="n">
         <v>0.2243</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6211</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2881</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.339</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.4278</v>
@@ -2066,10 +3068,19 @@
       <c r="D18" t="n">
         <v>0.2673</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3062</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.3883</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.4209</v>
@@ -2080,10 +3091,19 @@
       <c r="D19" t="n">
         <v>0.2753</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.6564</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3082</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.3983</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.4618</v>
@@ -2094,10 +3114,19 @@
       <c r="D20" t="n">
         <v>0.2587</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.6301</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.2827</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4044</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.5497</v>
@@ -2108,10 +3137,19 @@
       <c r="D21" t="n">
         <v>0.2203</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.5771</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.2396</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.39</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.6302</v>
@@ -2122,10 +3160,19 @@
       <c r="D22" t="n">
         <v>0.2575</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.5325</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1789</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.5852</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-0.7091</v>
@@ -2136,10 +3183,19 @@
       <c r="D23" t="n">
         <v>0.3812</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.4921</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.406</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.2996</v>
@@ -2149,6 +3205,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2726</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2088</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.356</v>
       </c>
     </row>
   </sheetData>
@@ -2178,10 +3243,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>2.315</v>
@@ -2192,10 +3266,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>10.1249</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5.8048</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17.66</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.2653</v>
@@ -2206,10 +3289,19 @@
       <c r="D3" t="n">
         <v>0.0012</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.767</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6535</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.9002</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>-0.3223</v>
@@ -2220,10 +3312,19 @@
       <c r="D4" t="n">
         <v>0.0003</v>
       </c>
+      <c r="E4" t="n">
+        <v>0.7245</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6092</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8615</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.2152</v>
@@ -2234,10 +3335,19 @@
       <c r="D5" t="n">
         <v>0.1745</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.2401</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.6919</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.3065</v>
@@ -2248,10 +3358,19 @@
       <c r="D6" t="n">
         <v>0.2254</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.4484</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.2081</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.2063</v>
@@ -2262,10 +3381,19 @@
       <c r="D7" t="n">
         <v>0.2041</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.2292</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8939</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.6901</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.4051</v>
@@ -2276,10 +3404,19 @@
       <c r="D8" t="n">
         <v>0.2362</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.6669</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3412</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.3037</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>0.3051</v>
@@ -2290,10 +3427,19 @@
       <c r="D9" t="n">
         <v>0.0836</v>
       </c>
+      <c r="E9" t="n">
+        <v>1.3568</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.9602</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.917</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>0.061</v>
@@ -2304,10 +3450,19 @@
       <c r="D10" t="n">
         <v>0.707</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.0629</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7734</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.4607</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-0.4734</v>
@@ -2318,10 +3473,19 @@
       <c r="D11" t="n">
         <v>0.3575</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.6229</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2272</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.7073</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.0528</v>
@@ -2332,10 +3496,19 @@
       <c r="D12" t="n">
         <v>0.7886</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.9486</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.6449</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.3952</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.0986</v>
@@ -2346,10 +3519,19 @@
       <c r="D13" t="n">
         <v>0.7109</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.9061</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5381</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.5258</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.1032</v>
@@ -2360,10 +3542,19 @@
       <c r="D14" t="n">
         <v>0.7043</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.902</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.5295</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.5365</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.0517</v>
@@ -2374,10 +3565,19 @@
       <c r="D15" t="n">
         <v>0.847</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.9497</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5618</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.6051</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>0.0129</v>
@@ -2388,10 +3588,19 @@
       <c r="D16" t="n">
         <v>0.9599</v>
       </c>
+      <c r="E16" t="n">
+        <v>1.0129</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.6134</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.6726</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>0.0513</v>
@@ -2402,10 +3611,19 @@
       <c r="D17" t="n">
         <v>0.8379</v>
       </c>
+      <c r="E17" t="n">
+        <v>1.0526</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.6441</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.7203</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>0.0151</v>
@@ -2416,10 +3634,19 @@
       <c r="D18" t="n">
         <v>0.9516</v>
       </c>
+      <c r="E18" t="n">
+        <v>1.0152</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6236</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.6528</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.0803</v>
@@ -2430,10 +3657,19 @@
       <c r="D19" t="n">
         <v>0.7466</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.9229</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5671</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5018</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.1165</v>
@@ -2444,10 +3680,19 @@
       <c r="D20" t="n">
         <v>0.6586</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5308</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.4923</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.0855</v>
@@ -2458,10 +3703,19 @@
       <c r="D21" t="n">
         <v>0.7547</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.9181</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.5371</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.5693</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.0216</v>
@@ -2472,10 +3726,19 @@
       <c r="D22" t="n">
         <v>0.9396</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.9786</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.5596</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.7113</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.048</v>
@@ -2486,10 +3749,19 @@
       <c r="D23" t="n">
         <v>0.9003</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.0492</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.4951</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.2232</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-1.3513</v>
@@ -2499,6 +3771,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2589</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2207</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.3037</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +3809,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.3025</v>
@@ -2542,10 +3832,19 @@
       <c r="D2" t="n">
         <v>0.0099</v>
       </c>
+      <c r="E2" t="n">
+        <v>27.1793</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.2101</v>
+      </c>
+      <c r="G2" t="n">
+        <v>334.2463</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>0.5262</v>
@@ -2556,10 +3855,19 @@
       <c r="D3" t="n">
         <v>0.0303</v>
       </c>
+      <c r="E3" t="n">
+        <v>1.6924</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.0513</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.7247</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.3542</v>
@@ -2570,10 +3878,19 @@
       <c r="D4" t="n">
         <v>0.1285</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.425</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9025</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.2501</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>0.1365</v>
@@ -2584,10 +3901,19 @@
       <c r="D5" t="n">
         <v>0.842</v>
       </c>
+      <c r="E5" t="n">
+        <v>1.1463</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2994</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4.3885</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>0.607</v>
@@ -2598,10 +3924,19 @@
       <c r="D6" t="n">
         <v>0.299</v>
       </c>
+      <c r="E6" t="n">
+        <v>1.8349</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5836</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.7691</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>-0.2895</v>
@@ -2612,10 +3947,19 @@
       <c r="D7" t="n">
         <v>0.6891</v>
       </c>
+      <c r="E7" t="n">
+        <v>0.7487</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1813</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.0907</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>0.6646</v>
@@ -2626,10 +3970,19 @@
       <c r="D8" t="n">
         <v>0.2402</v>
       </c>
+      <c r="E8" t="n">
+        <v>1.9438</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6411</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5.8934</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.4127</v>
@@ -2640,10 +3993,19 @@
       <c r="D9" t="n">
         <v>0.5945</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.6618</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.1448</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.0243</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-2.0377</v>
@@ -2654,10 +4016,19 @@
       <c r="D10" t="n">
         <v>0.9993</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.1303</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>-1.4508</v>
@@ -2668,10 +4039,19 @@
       <c r="D11" t="n">
         <v>0.9996</v>
       </c>
+      <c r="E11" t="n">
+        <v>0.2344</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="e">
+        <v>#NUM!</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-1.2623</v>
@@ -2682,10 +4062,19 @@
       <c r="D12" t="n">
         <v>0.1951</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.283</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0419</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.9104</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-2.3668</v>
@@ -2696,10 +4085,19 @@
       <c r="D13" t="n">
         <v>0.1062</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.0938</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0053</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.656</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-2.9957</v>
@@ -2710,10 +4108,19 @@
       <c r="D14" t="n">
         <v>0.0813</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.4513</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-3.2126</v>
@@ -2724,10 +4131,19 @@
       <c r="D15" t="n">
         <v>0.0655</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.0403</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.2282</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-3.1079</v>
@@ -2738,10 +4154,19 @@
       <c r="D16" t="n">
         <v>0.0469</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.0447</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0021</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.9579</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-2.7713</v>
@@ -2752,10 +4177,19 @@
       <c r="D17" t="n">
         <v>0.0332</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.0626</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0049</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8019</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-2.2698</v>
@@ -2766,10 +4200,19 @@
       <c r="D18" t="n">
         <v>0.0468</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.1033</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9684</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-2.1592</v>
@@ -2780,10 +4223,19 @@
       <c r="D19" t="n">
         <v>0.0564</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.1154</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0126</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.0606</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-2.2244</v>
@@ -2794,10 +4246,19 @@
       <c r="D20" t="n">
         <v>0.0572</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.1081</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0109</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.0705</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-2.0845</v>
@@ -2808,10 +4269,19 @@
       <c r="D21" t="n">
         <v>0.0791</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.1244</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0121</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.2738</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-2.3118</v>
@@ -2822,10 +4292,19 @@
       <c r="D22" t="n">
         <v>0.0578</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.0991</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.0795</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>-2.6108</v>
@@ -2836,10 +4315,19 @@
       <c r="D23" t="n">
         <v>0.0875</v>
       </c>
+      <c r="E23" t="n">
+        <v>0.0735</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0037</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.4684</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.9765</v>
@@ -2849,6 +4337,15 @@
       </c>
       <c r="D24" t="n">
         <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.3766</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.2514</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.5643</v>
       </c>
     </row>
   </sheetData>
@@ -2878,10 +4375,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
         <v>3.27</v>
@@ -2892,10 +4398,19 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>26.3105</v>
+      </c>
+      <c r="F2" t="n">
+        <v>9.6939</v>
+      </c>
+      <c r="G2" t="n">
+        <v>71.41</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="n">
         <v>-0.0697</v>
@@ -2906,10 +4421,19 @@
       <c r="D3" t="n">
         <v>0.64</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.9326</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6963</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.2493</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="n">
         <v>0.2093</v>
@@ -2920,10 +4444,19 @@
       <c r="D4" t="n">
         <v>0.1044</v>
       </c>
+      <c r="E4" t="n">
+        <v>1.2329</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9576</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.5873</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
         <v>-0.0263</v>
@@ -2934,10 +4467,19 @@
       <c r="D5" t="n">
         <v>0.9114</v>
       </c>
+      <c r="E5" t="n">
+        <v>0.974</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1.5489</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="n">
         <v>-0.1329</v>
@@ -2948,10 +4490,19 @@
       <c r="D6" t="n">
         <v>0.5783</v>
       </c>
+      <c r="E6" t="n">
+        <v>0.8755</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5479</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.3991</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
         <v>0.0402</v>
@@ -2962,10 +4513,19 @@
       <c r="D7" t="n">
         <v>0.8679</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.041</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.6482</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.6718</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
         <v>-0.2888</v>
@@ -2976,10 +4536,19 @@
       <c r="D8" t="n">
         <v>0.2543</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.7492</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.456</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.2309</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="n">
         <v>-0.3181</v>
@@ -2990,10 +4559,19 @@
       <c r="D9" t="n">
         <v>0.2846</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.7275</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4062</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.3029</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>-0.7947</v>
@@ -3004,10 +4582,19 @@
       <c r="D10" t="n">
         <v>0.0026</v>
       </c>
+      <c r="E10" t="n">
+        <v>0.4517</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2695</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.7571</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="n">
         <v>0.1406</v>
@@ -3018,10 +4605,19 @@
       <c r="D11" t="n">
         <v>0.5555</v>
       </c>
+      <c r="E11" t="n">
+        <v>1.1509</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7212</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.8366</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B12" t="n">
         <v>-0.1911</v>
@@ -3032,10 +4628,19 @@
       <c r="D12" t="n">
         <v>0.5947</v>
       </c>
+      <c r="E12" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.4085</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.6701</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" t="n">
         <v>-0.3377</v>
@@ -3046,10 +4651,19 @@
       <c r="D13" t="n">
         <v>0.5063</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.7134</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.2636</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.9312</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14" t="n">
         <v>-0.292</v>
@@ -3060,10 +4674,19 @@
       <c r="D14" t="n">
         <v>0.5832</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.7468</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.2632</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2.1189</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
         <v>-0.2599</v>
@@ -3074,10 +4697,19 @@
       <c r="D15" t="n">
         <v>0.6188</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.7712</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.2771</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.1462</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
         <v>-0.3529</v>
@@ -3088,10 +4720,19 @@
       <c r="D16" t="n">
         <v>0.4822</v>
       </c>
+      <c r="E16" t="n">
+        <v>0.7027</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2627</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.8797</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4626</v>
@@ -3102,10 +4743,19 @@
       <c r="D17" t="n">
         <v>0.3433</v>
       </c>
+      <c r="E17" t="n">
+        <v>0.6297</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2419</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.6391</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="n">
         <v>-0.5216</v>
@@ -3116,10 +4766,19 @@
       <c r="D18" t="n">
         <v>0.2774</v>
       </c>
+      <c r="E18" t="n">
+        <v>0.5935</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.2316</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.5214</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B19" t="n">
         <v>-0.5281</v>
@@ -3130,10 +4789,19 @@
       <c r="D19" t="n">
         <v>0.2722</v>
       </c>
+      <c r="E19" t="n">
+        <v>0.5897</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.2297</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.5139</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B20" t="n">
         <v>-0.556</v>
@@ -3144,10 +4812,19 @@
       <c r="D20" t="n">
         <v>0.2655</v>
       </c>
+      <c r="E20" t="n">
+        <v>0.5735</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.2156</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.526</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B21" t="n">
         <v>-0.4393</v>
@@ -3158,10 +4835,19 @@
       <c r="D21" t="n">
         <v>0.3893</v>
       </c>
+      <c r="E21" t="n">
+        <v>0.6445</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.7524</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B22" t="n">
         <v>-0.2169</v>
@@ -3172,10 +4858,19 @@
       <c r="D22" t="n">
         <v>0.6818</v>
       </c>
+      <c r="E22" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.2853</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2.271</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B23" t="n">
         <v>0.0068</v>
@@ -3186,10 +4881,19 @@
       <c r="D23" t="n">
         <v>0.992</v>
       </c>
+      <c r="E23" t="n">
+        <v>1.0068</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.2665</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.8036</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B24" t="n">
         <v>-0.2728</v>
@@ -3199,6 +4903,15 @@
       </c>
       <c r="D24" t="n">
         <v>0.0002</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.7612</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.6598</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.8783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #77: Remove the 1e-6 regularization for zero values (#78)
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -471,7 +471,7 @@
         <v>0.2467</v>
       </c>
       <c r="C2" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -537,16 +537,16 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>1.7447</v>
+        <v>1.7446</v>
       </c>
       <c r="C5" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>5.7239</v>
+        <v>5.7236</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -560,16 +560,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>1.8242</v>
+        <v>1.8241</v>
       </c>
       <c r="C6" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>6.1975</v>
+        <v>6.1972</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -609,16 +609,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>1.3494</v>
+        <v>1.3493</v>
       </c>
       <c r="C9" t="n">
-        <v>85816.1197</v>
+        <v>85835.7724</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>3.8551</v>
+        <v>3.8549</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Issue #99: Fix the G19 observation and other data inconsistencies (#100)
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -994,22 +994,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>2.6353</v>
+        <v>2.6061</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3605</v>
+        <v>0.3602</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>13.9481</v>
+        <v>13.5462</v>
       </c>
       <c r="F2" t="n">
-        <v>6.8806</v>
+        <v>6.6873</v>
       </c>
       <c r="G2" t="n">
-        <v>28.2752</v>
+        <v>27.4403</v>
       </c>
     </row>
     <row r="3">
@@ -1017,22 +1017,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1302</v>
+        <v>0.1333</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0924</v>
+        <v>0.0922</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1586</v>
+        <v>0.1481</v>
       </c>
       <c r="E3" t="n">
-        <v>1.1391</v>
+        <v>1.1426</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9504</v>
+        <v>0.9538</v>
       </c>
       <c r="G3" t="n">
-        <v>1.3651</v>
+        <v>1.3687</v>
       </c>
     </row>
     <row r="4">
@@ -1040,22 +1040,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0416</v>
+        <v>0.051</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0871</v>
+        <v>0.0868</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6332</v>
+        <v>0.5572</v>
       </c>
       <c r="E4" t="n">
-        <v>1.0424</v>
+        <v>1.0523</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8788</v>
+        <v>0.8876</v>
       </c>
       <c r="G4" t="n">
-        <v>1.2365</v>
+        <v>1.2475</v>
       </c>
     </row>
     <row r="5">
@@ -1063,22 +1063,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.2778</v>
+        <v>-0.2528</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1692</v>
+        <v>0.1693</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1006</v>
+        <v>0.1354</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7575</v>
+        <v>0.7766</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5437</v>
+        <v>0.5573</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0553</v>
+        <v>1.0823</v>
       </c>
     </row>
     <row r="6">
@@ -1086,22 +1086,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2237</v>
+        <v>0.2477</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1549</v>
+        <v>0.1551</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1486</v>
+        <v>0.1103</v>
       </c>
       <c r="E6" t="n">
-        <v>1.2508</v>
+        <v>1.2811</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9233</v>
+        <v>0.9453</v>
       </c>
       <c r="G6" t="n">
-        <v>1.6944</v>
+        <v>1.7362</v>
       </c>
     </row>
     <row r="7">
@@ -1109,22 +1109,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.5301</v>
+        <v>-0.5064</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2023</v>
+        <v>0.2024</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0088</v>
+        <v>0.0124</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5885</v>
+        <v>0.6027</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3959</v>
+        <v>0.4053</v>
       </c>
       <c r="G7" t="n">
-        <v>0.875</v>
+        <v>0.8962</v>
       </c>
     </row>
     <row r="8">
@@ -1132,22 +1132,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3141</v>
+        <v>0.345</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1548</v>
+        <v>0.1549</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0424</v>
+        <v>0.0259</v>
       </c>
       <c r="E8" t="n">
-        <v>1.369</v>
+        <v>1.4119</v>
       </c>
       <c r="F8" t="n">
-        <v>1.0108</v>
+        <v>1.0422</v>
       </c>
       <c r="G8" t="n">
-        <v>1.8541</v>
+        <v>1.9128</v>
       </c>
     </row>
     <row r="9">
@@ -1155,22 +1155,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.3997</v>
+        <v>-0.3807</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2154</v>
+        <v>0.2159</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0634</v>
+        <v>0.0778</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6705</v>
+        <v>0.6834</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4396</v>
+        <v>0.4476</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0226</v>
+        <v>1.0433</v>
       </c>
     </row>
     <row r="10">
@@ -1178,22 +1178,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>0.241</v>
+        <v>0.2623</v>
       </c>
       <c r="C10" t="n">
-        <v>0.147</v>
+        <v>0.1473</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1011</v>
+        <v>0.075</v>
       </c>
       <c r="E10" t="n">
-        <v>1.2726</v>
+        <v>1.2999</v>
       </c>
       <c r="F10" t="n">
-        <v>0.954</v>
+        <v>0.9739</v>
       </c>
       <c r="G10" t="n">
-        <v>1.6975</v>
+        <v>1.7351</v>
       </c>
     </row>
     <row r="11">
@@ -1201,22 +1201,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1211</v>
+        <v>-0.098</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1674</v>
+        <v>0.1677</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4696</v>
+        <v>0.559</v>
       </c>
       <c r="E11" t="n">
-        <v>0.886</v>
+        <v>0.9066</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6381</v>
+        <v>0.6527</v>
       </c>
       <c r="G11" t="n">
-        <v>1.2301</v>
+        <v>1.2595</v>
       </c>
     </row>
     <row r="12">
@@ -1224,22 +1224,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.2446</v>
+        <v>-0.2421</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2505</v>
+        <v>0.2499</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3288</v>
+        <v>0.3326</v>
       </c>
       <c r="E12" t="n">
-        <v>0.783</v>
+        <v>0.785</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4792</v>
+        <v>0.481</v>
       </c>
       <c r="G12" t="n">
-        <v>1.2793</v>
+        <v>1.281</v>
       </c>
     </row>
     <row r="13">
@@ -1247,22 +1247,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.4456</v>
+        <v>-0.4407</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3584</v>
+        <v>0.3576</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2137</v>
+        <v>0.2177</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6404</v>
+        <v>0.6436</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3173</v>
+        <v>0.3193</v>
       </c>
       <c r="G13" t="n">
-        <v>1.2927</v>
+        <v>1.297</v>
       </c>
     </row>
     <row r="14">
@@ -1270,22 +1270,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.5311</v>
+        <v>-0.5253</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3789</v>
+        <v>0.378</v>
       </c>
       <c r="D14" t="n">
-        <v>0.161</v>
+        <v>0.1647</v>
       </c>
       <c r="E14" t="n">
-        <v>0.588</v>
+        <v>0.5914</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2798</v>
+        <v>0.2819</v>
       </c>
       <c r="G14" t="n">
-        <v>1.2356</v>
+        <v>1.2407</v>
       </c>
     </row>
     <row r="15">
@@ -1293,22 +1293,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.5908</v>
+        <v>-0.5852</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3746</v>
+        <v>0.3738</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1148</v>
+        <v>0.1174</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5539</v>
+        <v>0.557</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2658</v>
+        <v>0.2677</v>
       </c>
       <c r="G15" t="n">
-        <v>1.1542</v>
+        <v>1.1588</v>
       </c>
     </row>
     <row r="16">
@@ -1316,22 +1316,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.5513</v>
+        <v>-0.5458</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3624</v>
+        <v>0.3616</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1282</v>
+        <v>0.1312</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5762</v>
+        <v>0.5794</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2832</v>
+        <v>0.2852</v>
       </c>
       <c r="G16" t="n">
-        <v>1.1724</v>
+        <v>1.1769</v>
       </c>
     </row>
     <row r="17">
@@ -1339,22 +1339,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4823</v>
+        <v>-0.4765</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3485</v>
+        <v>0.3477</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1664</v>
+        <v>0.1705</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6174</v>
+        <v>0.6209</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3118</v>
+        <v>0.3141</v>
       </c>
       <c r="G17" t="n">
-        <v>1.2224</v>
+        <v>1.2274</v>
       </c>
     </row>
     <row r="18">
@@ -1362,22 +1362,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.4713</v>
+        <v>-0.4667</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3404</v>
+        <v>0.3396</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1661</v>
+        <v>0.1693</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6242</v>
+        <v>0.6271</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3203</v>
+        <v>0.3223</v>
       </c>
       <c r="G18" t="n">
-        <v>1.2163</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="19">
@@ -1385,22 +1385,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.5076</v>
+        <v>-0.5035</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3404</v>
+        <v>0.3396</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1359</v>
+        <v>0.1382</v>
       </c>
       <c r="E19" t="n">
-        <v>0.602</v>
+        <v>0.6044</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3089</v>
+        <v>0.3106</v>
       </c>
       <c r="G19" t="n">
-        <v>1.173</v>
+        <v>1.176</v>
       </c>
     </row>
     <row r="20">
@@ -1408,22 +1408,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4477</v>
+        <v>-0.4435</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3486</v>
+        <v>0.3478</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1991</v>
+        <v>0.2022</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6391</v>
+        <v>0.6418</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3227</v>
+        <v>0.3246</v>
       </c>
       <c r="G20" t="n">
-        <v>1.2656</v>
+        <v>1.2688</v>
       </c>
     </row>
     <row r="21">
@@ -1431,22 +1431,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3903</v>
+        <v>-0.3859</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3512</v>
+        <v>0.3503</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2663</v>
+        <v>0.2705</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6768</v>
+        <v>0.6798</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3401</v>
+        <v>0.3422</v>
       </c>
       <c r="G21" t="n">
-        <v>1.3471</v>
+        <v>1.3506</v>
       </c>
     </row>
     <row r="22">
@@ -1454,22 +1454,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.555</v>
+        <v>-0.5485</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3548</v>
+        <v>0.3539</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1178</v>
+        <v>0.1212</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5741</v>
+        <v>0.5778</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2864</v>
+        <v>0.2888</v>
       </c>
       <c r="G22" t="n">
-        <v>1.1508</v>
+        <v>1.1563</v>
       </c>
     </row>
     <row r="23">
@@ -1477,22 +1477,22 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.7725</v>
+        <v>-0.7638</v>
       </c>
       <c r="C23" t="n">
-        <v>0.4429</v>
+        <v>0.4418</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0811</v>
+        <v>0.0838</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4618</v>
+        <v>0.4659</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1939</v>
+        <v>0.196</v>
       </c>
       <c r="G23" t="n">
-        <v>1.1003</v>
+        <v>1.1075</v>
       </c>
     </row>
     <row r="24">
@@ -1500,7 +1500,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.6532</v>
+        <v>-0.6584</v>
       </c>
       <c r="C24" t="n">
         <v>0.0589</v>
@@ -1509,13 +1509,13 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5204</v>
+        <v>0.5177</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4637</v>
+        <v>0.4613</v>
       </c>
       <c r="G24" t="n">
-        <v>0.584</v>
+        <v>0.581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix the ordering of the sex covariate
</commit_message>
<xml_diff>
--- a/tables/model_summaries.xlsx
+++ b/tables/model_summaries.xlsx
@@ -72,7 +72,7 @@
     <t xml:space="preserve">ParkVorpomm</t>
   </si>
   <si>
-    <t xml:space="preserve">Sexmale</t>
+    <t xml:space="preserve">Sexfemale</t>
   </si>
   <si>
     <t xml:space="preserve">ps(Date_numeric)3</t>
@@ -471,16 +471,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4954</v>
+        <v>0.3383</v>
       </c>
       <c r="C2" t="n">
-        <v>31287.1649</v>
+        <v>31285.9137</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1.6412</v>
+        <v>1.4025</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -543,7 +543,7 @@
         <v>1.4986</v>
       </c>
       <c r="C5" t="n">
-        <v>31287.1649</v>
+        <v>31285.9137</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -566,7 +566,7 @@
         <v>1.5607</v>
       </c>
       <c r="C6" t="n">
-        <v>31287.1649</v>
+        <v>31285.9137</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -586,10 +586,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.2932</v>
+        <v>-0.2933</v>
       </c>
       <c r="C7" t="n">
-        <v>39729.0333</v>
+        <v>39728.0479</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -612,7 +612,7 @@
         <v>-0.2467</v>
       </c>
       <c r="C8" t="n">
-        <v>41853.7631</v>
+        <v>41852.8278</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -635,7 +635,7 @@
         <v>1.1088</v>
       </c>
       <c r="C9" t="n">
-        <v>31287.1649</v>
+        <v>31285.9137</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -658,7 +658,7 @@
         <v>-0.1804</v>
       </c>
       <c r="C10" t="n">
-        <v>38074.9733</v>
+        <v>38073.9451</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -681,7 +681,7 @@
         <v>-0.178</v>
       </c>
       <c r="C11" t="n">
-        <v>41811.4045</v>
+        <v>41810.4683</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1572</v>
+        <v>0.1572</v>
       </c>
       <c r="C12" t="n">
         <v>0.1534</v>
@@ -710,13 +710,13 @@
         <v>0.3056</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8546</v>
+        <v>1.1702</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6326</v>
+        <v>0.8663</v>
       </c>
       <c r="G12" t="n">
-        <v>1.1543</v>
+        <v>1.5807</v>
       </c>
     </row>
     <row r="13">
@@ -1060,22 +1060,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>2.7173</v>
+        <v>2.5812</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3645</v>
+        <v>0.3598</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>15.1397</v>
+        <v>13.2123</v>
       </c>
       <c r="F2" t="n">
-        <v>7.4101</v>
+        <v>6.527</v>
       </c>
       <c r="G2" t="n">
-        <v>30.9322</v>
+        <v>26.745</v>
       </c>
     </row>
     <row r="3">
@@ -1290,7 +1290,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.1362</v>
+        <v>0.1362</v>
       </c>
       <c r="C12" t="n">
         <v>0.0786</v>
@@ -1299,13 +1299,13 @@
         <v>0.0831</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8727</v>
+        <v>1.1459</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7481</v>
+        <v>0.9823</v>
       </c>
       <c r="G12" t="n">
-        <v>1.018</v>
+        <v>1.3367</v>
       </c>
     </row>
     <row r="13">
@@ -1648,53 +1648,93 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" t="n">
+        <v>1.07</v>
+      </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
+        <v>1.9288</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5791</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.9154</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0665</v>
+      </c>
+      <c r="G2" t="n">
+        <v>127.7926</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="n">
+        <v>-0.2994</v>
+      </c>
       <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+        <v>0.2902</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.3021</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.7413</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.4197</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.309</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="n">
+        <v>-0.0995</v>
+      </c>
       <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
+        <v>0.2852</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.7272</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9053</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.5176</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.5833</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="n">
+        <v>0.7754</v>
+      </c>
       <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
+        <v>0.4652</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0955</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.1714</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.8726</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5.4037</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -1713,14 +1753,24 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="n">
+        <v>-0.0794</v>
+      </c>
       <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
+        <v>0.5963</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.894</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.9236</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2.9723</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -1752,62 +1802,92 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="n">
+        <v>0.3387</v>
+      </c>
       <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
+        <v>0.4898</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.4892</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.4031</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.5373</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.6646</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11"/>
+      <c r="B11" t="n">
+        <v>-0.3059</v>
+      </c>
       <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
+        <v>0.6584</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.6422</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.7365</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2026</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.6764</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="n">
+        <v>-0.1631</v>
+      </c>
       <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
+        <v>0.2262</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8495</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5453</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.3235</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>-0.4088</v>
       </c>
       <c r="C13" t="n">
-        <v>3.603</v>
+        <v>1.7762</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0.818</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0.6644</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0009</v>
+        <v>0.0204</v>
       </c>
       <c r="G13" t="n">
-        <v>1166.4223</v>
+        <v>21.596</v>
       </c>
     </row>
     <row r="14">
@@ -1815,22 +1895,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>-0.6868</v>
       </c>
       <c r="C14" t="n">
-        <v>6.4865</v>
+        <v>2.1718</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0.7518</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0.5032</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>0.0071</v>
       </c>
       <c r="G14" t="n">
-        <v>332110.95</v>
+        <v>35.5142</v>
       </c>
     </row>
     <row r="15">
@@ -1838,22 +1918,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>-0.6534</v>
       </c>
       <c r="C15" t="n">
-        <v>8.729</v>
+        <v>2.0353</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0.7482</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.5203</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>0.0096</v>
       </c>
       <c r="G15" t="n">
-        <v>26923312.199</v>
+        <v>28.0977</v>
       </c>
     </row>
     <row r="16">
@@ -1861,22 +1941,22 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>-0.4285</v>
       </c>
       <c r="C16" t="n">
-        <v>10.3308</v>
+        <v>1.9944</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0.8299</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0.6515</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>0.0131</v>
       </c>
       <c r="G16" t="n">
-        <v>621671097.3528</v>
+        <v>32.4743</v>
       </c>
     </row>
     <row r="17">
@@ -1884,22 +1964,22 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>-0.1135</v>
       </c>
       <c r="C17" t="n">
-        <v>11.2918</v>
+        <v>1.9461</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0.9535</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0.8927</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>0.0197</v>
       </c>
       <c r="G17" t="n">
-        <v>4088964951.5398</v>
+        <v>40.4767</v>
       </c>
     </row>
     <row r="18">
@@ -1907,22 +1987,22 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>0.1647</v>
       </c>
       <c r="C18" t="n">
-        <v>11.6122</v>
+        <v>1.9332</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0.9321</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>1.1791</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.0267</v>
       </c>
       <c r="G18" t="n">
-        <v>7661199964.3239</v>
+        <v>52.1313</v>
       </c>
     </row>
     <row r="19">
@@ -1930,22 +2010,22 @@
         <v>24</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>0.7484</v>
       </c>
       <c r="C19" t="n">
-        <v>11.2918</v>
+        <v>1.9218</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>0.6969</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>2.1137</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.0489</v>
       </c>
       <c r="G19" t="n">
-        <v>4088964951.5397</v>
+        <v>91.3776</v>
       </c>
     </row>
     <row r="20">
@@ -1953,22 +2033,22 @@
         <v>25</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>-0.0321</v>
       </c>
       <c r="C20" t="n">
-        <v>10.3308</v>
+        <v>1.9143</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0.9866</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0.9684</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>0.0227</v>
       </c>
       <c r="G20" t="n">
-        <v>621671097.3528</v>
+        <v>41.2564</v>
       </c>
     </row>
     <row r="21">
@@ -1976,22 +2056,22 @@
         <v>26</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>-0.6122</v>
       </c>
       <c r="C21" t="n">
-        <v>8.729</v>
+        <v>1.9791</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0.7571</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0.5422</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>0.0112</v>
       </c>
       <c r="G21" t="n">
-        <v>26923312.199</v>
+        <v>26.2274</v>
       </c>
     </row>
     <row r="22">
@@ -1999,22 +2079,22 @@
         <v>27</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>-0.5695</v>
       </c>
       <c r="C22" t="n">
-        <v>6.4865</v>
+        <v>2.0431</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.7805</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0.5658</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>0.0103</v>
       </c>
       <c r="G22" t="n">
-        <v>332110.95</v>
+        <v>31.0316</v>
       </c>
     </row>
     <row r="23">
@@ -2022,49 +2102,69 @@
         <v>28</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>-0.0195</v>
       </c>
       <c r="C23" t="n">
-        <v>3.603</v>
+        <v>1.9316</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0.9919</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0.9806</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0009</v>
+        <v>0.0222</v>
       </c>
       <c r="G23" t="n">
-        <v>1166.4223</v>
+        <v>43.2244</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24"/>
+      <c r="B24" t="n">
+        <v>0.6483</v>
+      </c>
       <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
+        <v>2.5766</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.8013</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.9123</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0123</v>
+      </c>
+      <c r="G24" t="n">
+        <v>298.3704</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B25"/>
+      <c r="B25" t="n">
+        <v>-0.2978</v>
+      </c>
       <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
+        <v>0.1281</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.7424</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.5776</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.9543</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2108,22 +2208,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>2.8072</v>
+        <v>2.8056</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1806</v>
+        <v>0.1809</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>16.5633</v>
+        <v>16.5377</v>
       </c>
       <c r="F2" t="n">
-        <v>11.6251</v>
+        <v>11.6003</v>
       </c>
       <c r="G2" t="n">
-        <v>23.599</v>
+        <v>23.5766</v>
       </c>
     </row>
     <row r="3">
@@ -2338,7 +2438,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0015</v>
+        <v>0.0015</v>
       </c>
       <c r="C12" t="n">
         <v>0.0403</v>
@@ -2347,13 +2447,13 @@
         <v>0.9695</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9985</v>
+        <v>1.0015</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9226</v>
+        <v>0.9255</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0805</v>
+        <v>1.0839</v>
       </c>
     </row>
     <row r="13">
@@ -2697,22 +2797,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>3.6956</v>
+        <v>3.7037</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5512</v>
+        <v>0.5554</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>40.2688</v>
+        <v>40.5976</v>
       </c>
       <c r="F2" t="n">
-        <v>13.6696</v>
+        <v>13.668</v>
       </c>
       <c r="G2" t="n">
-        <v>118.627</v>
+        <v>120.5855</v>
       </c>
     </row>
     <row r="3">
@@ -2927,7 +3027,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0081</v>
+        <v>-0.0081</v>
       </c>
       <c r="C12" t="n">
         <v>0.0816</v>
@@ -2936,13 +3036,13 @@
         <v>0.9206</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0082</v>
+        <v>0.9919</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8591</v>
+        <v>0.8453</v>
       </c>
       <c r="G12" t="n">
-        <v>1.183</v>
+        <v>1.164</v>
       </c>
     </row>
     <row r="13">
@@ -3286,22 +3386,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>2.3422</v>
+        <v>2.3067</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2862</v>
+        <v>0.2827</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>10.4046</v>
+        <v>10.0414</v>
       </c>
       <c r="F2" t="n">
-        <v>5.9379</v>
+        <v>5.7698</v>
       </c>
       <c r="G2" t="n">
-        <v>18.2311</v>
+        <v>17.4752</v>
       </c>
     </row>
     <row r="3">
@@ -3516,7 +3616,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0355</v>
+        <v>0.0355</v>
       </c>
       <c r="C12" t="n">
         <v>0.0623</v>
@@ -3525,13 +3625,13 @@
         <v>0.5686</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9651</v>
+        <v>1.0362</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8541</v>
+        <v>0.917</v>
       </c>
       <c r="G12" t="n">
-        <v>1.0905</v>
+        <v>1.1708</v>
       </c>
     </row>
     <row r="13">
@@ -3875,22 +3975,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>4.0988</v>
+        <v>4.6817</v>
       </c>
       <c r="C2" t="n">
-        <v>1.4925</v>
+        <v>1.5309</v>
       </c>
       <c r="D2" t="n">
-        <v>0.006</v>
+        <v>0.0022</v>
       </c>
       <c r="E2" t="n">
-        <v>60.2681</v>
+        <v>107.9553</v>
       </c>
       <c r="F2" t="n">
-        <v>3.2338</v>
+        <v>5.3722</v>
       </c>
       <c r="G2" t="n">
-        <v>1123.2223</v>
+        <v>2169.3619</v>
       </c>
     </row>
     <row r="3">
@@ -4085,7 +4185,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5829</v>
+        <v>-0.5829</v>
       </c>
       <c r="C12" t="n">
         <v>0.1984</v>
@@ -4094,13 +4194,13 @@
         <v>0.0033</v>
       </c>
       <c r="E12" t="n">
-        <v>1.7912</v>
+        <v>0.5583</v>
       </c>
       <c r="F12" t="n">
-        <v>1.2141</v>
+        <v>0.3784</v>
       </c>
       <c r="G12" t="n">
-        <v>2.6429</v>
+        <v>0.8237</v>
       </c>
     </row>
     <row r="13">
@@ -4444,22 +4544,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>3.2903</v>
+        <v>3.2524</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5129</v>
+        <v>0.5121</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>26.8496</v>
+        <v>25.8515</v>
       </c>
       <c r="F2" t="n">
-        <v>9.8258</v>
+        <v>9.4743</v>
       </c>
       <c r="G2" t="n">
-        <v>73.3682</v>
+        <v>70.5384</v>
       </c>
     </row>
     <row r="3">
@@ -4674,7 +4774,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.0379</v>
+        <v>0.0379</v>
       </c>
       <c r="C12" t="n">
         <v>0.1166</v>
@@ -4683,13 +4783,13 @@
         <v>0.7454</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9628</v>
+        <v>1.0386</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7661</v>
+        <v>0.8263</v>
       </c>
       <c r="G12" t="n">
-        <v>1.2101</v>
+        <v>1.3054</v>
       </c>
     </row>
     <row r="13">

</xml_diff>